<commit_message>
qa tables and OperationDefinition
</commit_message>
<xml_diff>
--- a/input/images/data-element-mapping.xlsx
+++ b/input/images/data-element-mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/davinci-ecdx/input/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E5A78468-E594-2F49-BB9A-5C40B046F5C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{66F7307A-569A-E54B-B33D-C69C50F4D5DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36100" yWindow="1780" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="40520" yWindow="500" windowWidth="37260" windowHeight="17440"/>
   </bookViews>
   <sheets>
     <sheet name="data-element-mapping" sheetId="1" r:id="rId1"/>
@@ -63,6 +63,9 @@
     <t>Task.identifier</t>
   </si>
   <si>
+    <t>Provider or Payer assigned tracking control number</t>
+  </si>
+  <si>
     <t>Use</t>
   </si>
   <si>
@@ -72,9 +75,6 @@
     <t>Task.reasonCode</t>
   </si>
   <si>
-    <t>Claim or Prior Authorization.</t>
-  </si>
-  <si>
     <t>Payer ID</t>
   </si>
   <si>
@@ -87,9 +87,6 @@
     <t>Task.reasonReference.identifier</t>
   </si>
   <si>
-    <t>Payer ID - should be a business ID -requester.reference</t>
-  </si>
-  <si>
     <t>Payer URL</t>
   </si>
   <si>
@@ -102,15 +99,15 @@
     <t>"payer-url" Task.input</t>
   </si>
   <si>
+    <t>Payer endpoint where the attachments are submitted using the $submit-operation</t>
+  </si>
+  <si>
     <t>Organization ID</t>
   </si>
   <si>
     <t>OrganizationId</t>
   </si>
   <si>
-    <t>Organization of Provider who submitted Claim/Prior-Auth</t>
-  </si>
-  <si>
     <t>Provider ID</t>
   </si>
   <si>
@@ -120,15 +117,9 @@
     <t>Task.owner.identifier</t>
   </si>
   <si>
-    <t>Provider who submitted Claim/Prior-Auth</t>
-  </si>
-  <si>
     <t>Claim/PreAuth ID</t>
   </si>
   <si>
-    <t>Claim/Prior-Auth ID (Provider or Payer Assigned)</t>
-  </si>
-  <si>
     <t>Line Item(s)</t>
   </si>
   <si>
@@ -138,9 +129,6 @@
     <t>“code” Task.input.extension</t>
   </si>
   <si>
-    <t>Claim/Prior-Auth line item # nos</t>
-  </si>
-  <si>
     <t>LOINC Attachment code</t>
   </si>
   <si>
@@ -153,7 +141,7 @@
     <t>“code” Task.input </t>
   </si>
   <si>
-    <t>LOINCs</t>
+    <t>LOINC attachment codes</t>
   </si>
   <si>
     <t>Due Date</t>
@@ -165,7 +153,7 @@
     <t>Task.restriction.period</t>
   </si>
   <si>
-    <t>When attachments are Due</t>
+    <t>Deadline form submitting  attachments  to  Payer</t>
   </si>
   <si>
     <t>Date of Service</t>
@@ -180,9 +168,6 @@
     <t>“service-date” Task.input </t>
   </si>
   <si>
-    <t xml:space="preserve">Claim/Prior-Auth Date of Service (encounter info) </t>
-  </si>
-  <si>
     <t>Member ID</t>
   </si>
   <si>
@@ -195,7 +180,7 @@
     <t>Patient.identifier</t>
   </si>
   <si>
-    <t>Member ID (patient info)</t>
+    <t>Payer assigned patient identifier</t>
   </si>
   <si>
     <t>Patient Name</t>
@@ -207,7 +192,7 @@
     <t>Patient.name</t>
   </si>
   <si>
-    <t>Patient Name (patient info)</t>
+    <t>Patient Demographic information for patient matching</t>
   </si>
   <si>
     <t>Patient Account No.</t>
@@ -216,7 +201,7 @@
     <t>CLM01(837)</t>
   </si>
   <si>
-    <t>Patient Account No. PreAuth Only (patient info)</t>
+    <t>Provider assigned patient identifer only for prior authorizatons</t>
   </si>
   <si>
     <t>Date of Birth</t>
@@ -228,7 +213,22 @@
     <t>Patient.birthDate</t>
   </si>
   <si>
-    <t>Date of Birth (patient info)</t>
+    <t>Organization of Provider who submitted claim/prior authorization</t>
+  </si>
+  <si>
+    <t>Provider who submitted claim/prior authorization</t>
+  </si>
+  <si>
+    <t>claim/prior authorization ID (Provider or Payer Assigned)</t>
+  </si>
+  <si>
+    <t>claim/prior authorization line item numbers</t>
+  </si>
+  <si>
+    <t>Date of Service for claim/prior authorization</t>
+  </si>
+  <si>
+    <t>Choice of "claim" or "preauthorization"</t>
   </si>
 </sst>
 </file>
@@ -1071,9 +1071,21 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="71" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -1118,7 +1130,7 @@
         <v>11</v>
       </c>
       <c r="H2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -1126,16 +1138,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H3" t="s">
-        <v>15</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -1155,7 +1167,7 @@
         <v>19</v>
       </c>
       <c r="H4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -1163,25 +1175,25 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>23</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>24</v>
-      </c>
-      <c r="H5" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -1192,22 +1204,22 @@
         <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F6" t="s">
         <v>26</v>
       </c>
       <c r="G6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H6" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -1215,16 +1227,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" t="s">
         <v>28</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>29</v>
       </c>
-      <c r="G7" t="s">
-        <v>30</v>
-      </c>
       <c r="H7" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -1232,16 +1244,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G8" t="s">
         <v>19</v>
       </c>
       <c r="H8" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -1249,16 +1261,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H9" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -1266,19 +1278,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" t="s">
         <v>38</v>
-      </c>
-      <c r="C10" t="s">
-        <v>39</v>
-      </c>
-      <c r="F10" t="s">
-        <v>40</v>
-      </c>
-      <c r="G10" t="s">
-        <v>41</v>
-      </c>
-      <c r="H10" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -1286,19 +1298,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G11" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="H11" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -1306,19 +1318,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F12" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G12" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H12" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -1326,19 +1338,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F13" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G13" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H13" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -1346,19 +1358,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C14" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G14" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="H14" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -1366,19 +1378,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C15" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G15" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H15" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -1386,19 +1398,19 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C16" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G16" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="H16" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pre-Applied FHIR-38172, FHIR-38174, FHIR-38194 partial pre-applied FHIR-38189
</commit_message>
<xml_diff>
--- a/input/images/data-element-mapping.xlsx
+++ b/input/images/data-element-mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10708"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/davinci-ecdx/input/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{66F7307A-569A-E54B-B33D-C69C50F4D5DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{8460BBD2-1085-D440-9426-C6C6B853D98E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40520" yWindow="500" windowWidth="37260" windowHeight="17440"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="34120" windowHeight="28300"/>
   </bookViews>
   <sheets>
     <sheet name="data-element-mapping" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="83" uniqueCount="68">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="99" uniqueCount="71">
   <si>
     <t>No</t>
   </si>
@@ -42,15 +42,9 @@
     <t>X12n 275</t>
   </si>
   <si>
-    <t>CDex #submit-attachment Parameter</t>
-  </si>
-  <si>
     <t>CDex Request Attachment Task Profile Element</t>
   </si>
   <si>
-    <t>Comments</t>
-  </si>
-  <si>
     <t>Tracking ID (Provider or Payer Assigned)</t>
   </si>
   <si>
@@ -63,9 +57,6 @@
     <t>Task.identifier</t>
   </si>
   <si>
-    <t>Provider or Payer assigned tracking control number</t>
-  </si>
-  <si>
     <t>Use</t>
   </si>
   <si>
@@ -75,6 +66,9 @@
     <t>Task.reasonCode</t>
   </si>
   <si>
+    <t>Choice of "claim" or "preauthorization"</t>
+  </si>
+  <si>
     <t>Payer ID</t>
   </si>
   <si>
@@ -117,6 +111,9 @@
     <t>Task.owner.identifier</t>
   </si>
   <si>
+    <t>Provider who submitted claim/prior authorization</t>
+  </si>
+  <si>
     <t>Claim/PreAuth ID</t>
   </si>
   <si>
@@ -129,7 +126,7 @@
     <t>“code” Task.input.extension</t>
   </si>
   <si>
-    <t>LOINC Attachment code</t>
+    <t>LOINC Attachment Code</t>
   </si>
   <si>
     <t>STC01-02</t>
@@ -153,9 +150,6 @@
     <t>Task.restriction.period</t>
   </si>
   <si>
-    <t>Deadline form submitting  attachments  to  Payer</t>
-  </si>
-  <si>
     <t>Date of Service</t>
   </si>
   <si>
@@ -192,18 +186,12 @@
     <t>Patient.name</t>
   </si>
   <si>
-    <t>Patient Demographic information for patient matching</t>
-  </si>
-  <si>
     <t>Patient Account No.</t>
   </si>
   <si>
     <t>CLM01(837)</t>
   </si>
   <si>
-    <t>Provider assigned patient identifer only for prior authorizatons</t>
-  </si>
-  <si>
     <t>Date of Birth</t>
   </si>
   <si>
@@ -213,29 +201,50 @@
     <t>Patient.birthDate</t>
   </si>
   <si>
-    <t>Organization of Provider who submitted claim/prior authorization</t>
-  </si>
-  <si>
-    <t>Provider who submitted claim/prior authorization</t>
-  </si>
-  <si>
-    <t>claim/prior authorization ID (Provider or Payer Assigned)</t>
-  </si>
-  <si>
-    <t>claim/prior authorization line item numbers</t>
-  </si>
-  <si>
-    <t>Date of Service for claim/prior authorization</t>
-  </si>
-  <si>
-    <t>Choice of "claim" or "preauthorization"</t>
+    <t>Task.requester.identifier</t>
+  </si>
+  <si>
+    <t>Submit Attachments Comments</t>
+  </si>
+  <si>
+    <t>Request Attachments Comments</t>
+  </si>
+  <si>
+    <t>For *unsolicited* attachments, this is the provider-assigned tracking/control number. For *solicited* attachments, this is the payer-assigned tracking/control number.</t>
+  </si>
+  <si>
+    <t>Deadline for submitting attachments to Payer</t>
+  </si>
+  <si>
+    <t>CDex $submit-attachment Parameter</t>
+  </si>
+  <si>
+    <t>Payer-assigned tracking/control number.</t>
+  </si>
+  <si>
+    <t>Provider-assigned claim/prior authorization ID</t>
+  </si>
+  <si>
+    <t>Patient Account Number is a provider-assigned identifier</t>
+  </si>
+  <si>
+    <t>Patient demographic information for patient matching</t>
+  </si>
+  <si>
+    <t>Date of service for claim/prior authorization</t>
+  </si>
+  <si>
+    <t>Organization of provider who submitted claim/prior authorization</t>
+  </si>
+  <si>
+    <t>Claim/prior-authorization line item numbers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -369,6 +378,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF5E6C84"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -712,8 +727,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1069,25 +1088,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="41" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="71" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="70.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1104,313 +1123,361 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
       <c r="H1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+      <c r="I1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="57" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="G2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
         <v>13</v>
       </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" t="s">
-        <v>18</v>
-      </c>
       <c r="G4" t="s">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="H4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="I4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" t="s">
         <v>20</v>
       </c>
-      <c r="C5" t="s">
+      <c r="G5" t="s">
         <v>21</v>
       </c>
-      <c r="D5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>22</v>
       </c>
-      <c r="G5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G6" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="H6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+      <c r="I6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" t="s">
         <v>27</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H7" t="s">
         <v>28</v>
       </c>
-      <c r="G7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G8" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" t="s">
         <v>31</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>32</v>
       </c>
-      <c r="G9" t="s">
-        <v>33</v>
-      </c>
       <c r="H9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+      <c r="I9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
         <v>34</v>
       </c>
-      <c r="C10" t="s">
+      <c r="F10" t="s">
         <v>35</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>36</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>37</v>
       </c>
-      <c r="H10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
         <v>39</v>
       </c>
-      <c r="C11" t="s">
+      <c r="F11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" t="s">
         <v>40</v>
       </c>
-      <c r="F11" t="s">
-        <v>21</v>
-      </c>
-      <c r="G11" t="s">
-        <v>41</v>
-      </c>
       <c r="H11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+      <c r="I11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" t="s">
         <v>43</v>
       </c>
-      <c r="C12" t="s">
+      <c r="G12" t="s">
         <v>44</v>
       </c>
-      <c r="F12" t="s">
-        <v>45</v>
-      </c>
-      <c r="G12" t="s">
-        <v>46</v>
-      </c>
       <c r="H12" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="I12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" t="s">
         <v>47</v>
       </c>
-      <c r="C13" t="s">
+      <c r="G13" t="s">
         <v>48</v>
       </c>
-      <c r="F13" t="s">
+      <c r="H13" t="s">
         <v>49</v>
       </c>
-      <c r="G13" t="s">
-        <v>50</v>
-      </c>
-      <c r="H13" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" t="s">
         <v>52</v>
       </c>
-      <c r="C14" t="s">
-        <v>53</v>
-      </c>
-      <c r="F14" t="s">
-        <v>21</v>
-      </c>
-      <c r="G14" t="s">
-        <v>54</v>
-      </c>
       <c r="H14" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="I14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G15" t="s">
-        <v>50</v>
-      </c>
-      <c r="H15" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C16" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G16" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="H16" t="s">
-        <v>55</v>
+        <v>67</v>
+      </c>
+      <c r="I16" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated X12 element mappings and X12 required citations FHIR-38287
</commit_message>
<xml_diff>
--- a/input/images/data-element-mapping.xlsx
+++ b/input/images/data-element-mapping.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/davinci-ecdx/input/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{8460BBD2-1085-D440-9426-C6C6B853D98E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{479C103E-F463-9840-8AE7-F626EBE76960}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="34120" windowHeight="28300"/>
+    <workbookView xWindow="54900" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data-element-mapping" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="99" uniqueCount="71">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="135" uniqueCount="105">
   <si>
     <t>No</t>
   </si>
@@ -33,30 +44,33 @@
     <t>Data Element</t>
   </si>
   <si>
-    <t>X12n 277</t>
-  </si>
-  <si>
-    <t>X12n 278 Response</t>
-  </si>
-  <si>
-    <t>X12n 275</t>
+    <t>CDex $submit-attachment Parameter</t>
   </si>
   <si>
     <t>CDex Request Attachment Task Profile Element</t>
   </si>
   <si>
+    <t>Submit Attachments Comments</t>
+  </si>
+  <si>
+    <t>Request Attachments Comments</t>
+  </si>
+  <si>
     <t>Tracking ID (Provider or Payer Assigned)</t>
   </si>
   <si>
-    <t>REF02</t>
-  </si>
-  <si>
     <t>TrackingId</t>
   </si>
   <si>
     <t>Task.identifier</t>
   </si>
   <si>
+    <t>&lt;span class="bg-success" markdown="1"&gt;For *unsolicited* attachments, this is the provider-assigned tracking/control number. For *solicited* attachments, this is the payer-assigned tracking/control number.&lt;/span&gt;&lt;!-- new-content --&gt;</t>
+  </si>
+  <si>
+    <t>&lt;span class="bg-success" markdown="1"&gt;Payer-assigned tracking/control number&lt;/span&gt;&lt;!-- new-content --&gt;</t>
+  </si>
+  <si>
     <t>Use</t>
   </si>
   <si>
@@ -72,49 +86,55 @@
     <t>Payer ID</t>
   </si>
   <si>
-    <t>NM108</t>
-  </si>
-  <si>
     <t>PayerId</t>
   </si>
   <si>
+    <t>Task.requester.identifier</t>
+  </si>
+  <si>
+    <t>Payer URL</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>(operation endpoint)</t>
+  </si>
+  <si>
+    <t>"payer-url" Task.input</t>
+  </si>
+  <si>
+    <t>Payer endpoint where the attachments are submitted using the $submit-operation</t>
+  </si>
+  <si>
+    <t>Organization ID</t>
+  </si>
+  <si>
+    <t>OrganizationId</t>
+  </si>
+  <si>
+    <t>Task.owner.identifier</t>
+  </si>
+  <si>
+    <t>Organization of provider who submitted claim/prior authorization</t>
+  </si>
+  <si>
+    <t>Provider ID</t>
+  </si>
+  <si>
+    <t>ProviderId</t>
+  </si>
+  <si>
+    <t>Provider who submitted claim/prior authorization</t>
+  </si>
+  <si>
+    <t>Claim/PreAuth ID</t>
+  </si>
+  <si>
     <t>Task.reasonReference.identifier</t>
   </si>
   <si>
-    <t>Payer URL</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>(operation endpoint)</t>
-  </si>
-  <si>
-    <t>"payer-url" Task.input</t>
-  </si>
-  <si>
-    <t>Payer endpoint where the attachments are submitted using the $submit-operation</t>
-  </si>
-  <si>
-    <t>Organization ID</t>
-  </si>
-  <si>
-    <t>OrganizationId</t>
-  </si>
-  <si>
-    <t>Provider ID</t>
-  </si>
-  <si>
-    <t>ProviderId</t>
-  </si>
-  <si>
-    <t>Task.owner.identifier</t>
-  </si>
-  <si>
-    <t>Provider who submitted claim/prior authorization</t>
-  </si>
-  <si>
-    <t>Claim/PreAuth ID</t>
+    <t>&lt;span class="bg-success" markdown="1"&gt;Provider-assigned claim/prior authorization ID&lt;/span&gt;&lt;!-- new-content --&gt;</t>
   </si>
   <si>
     <t>Line Item(s)</t>
@@ -126,12 +146,12 @@
     <t>“code” Task.input.extension</t>
   </si>
   <si>
+    <t>Claim/prior-authorization line item numbers</t>
+  </si>
+  <si>
     <t>LOINC Attachment Code</t>
   </si>
   <si>
-    <t>STC01-02</t>
-  </si>
-  <si>
     <t>Attachment.Code</t>
   </si>
   <si>
@@ -144,30 +164,27 @@
     <t>Due Date</t>
   </si>
   <si>
-    <t>DPT02</t>
-  </si>
-  <si>
     <t>Task.restriction.period</t>
   </si>
   <si>
+    <t>Deadline for submitting attachments to Payer</t>
+  </si>
+  <si>
     <t>Date of Service</t>
   </si>
   <si>
-    <t>DTP03</t>
-  </si>
-  <si>
     <t>ServiceDate</t>
   </si>
   <si>
     <t>“service-date” Task.input </t>
   </si>
   <si>
+    <t>Date of service for claim/prior authorization</t>
+  </si>
+  <si>
     <t>Member ID</t>
   </si>
   <si>
-    <t>X2100D NM</t>
-  </si>
-  <si>
     <t>MemberId</t>
   </si>
   <si>
@@ -180,70 +197,169 @@
     <t>Patient Name</t>
   </si>
   <si>
-    <t>X2100D NM103-7</t>
-  </si>
-  <si>
     <t>Patient.name</t>
   </si>
   <si>
+    <t>Patient demographic information for patient matching</t>
+  </si>
+  <si>
     <t>Patient Account No.</t>
   </si>
   <si>
-    <t>CLM01(837)</t>
+    <t>&lt;span class="bg-success" markdown="1"&gt;Patient Account Number is a provider-assigned identifier&lt;/span&gt;&lt;!-- new-content --&gt;</t>
   </si>
   <si>
     <t>Date of Birth</t>
   </si>
   <si>
-    <t>X12</t>
-  </si>
-  <si>
     <t>Patient.birthDate</t>
   </si>
   <si>
-    <t>Task.requester.identifier</t>
-  </si>
-  <si>
-    <t>Submit Attachments Comments</t>
-  </si>
-  <si>
-    <t>Request Attachments Comments</t>
-  </si>
-  <si>
-    <t>For *unsolicited* attachments, this is the provider-assigned tracking/control number. For *solicited* attachments, this is the payer-assigned tracking/control number.</t>
-  </si>
-  <si>
-    <t>Deadline for submitting attachments to Payer</t>
-  </si>
-  <si>
-    <t>CDex $submit-attachment Parameter</t>
-  </si>
-  <si>
-    <t>Payer-assigned tracking/control number.</t>
-  </si>
-  <si>
-    <t>Provider-assigned claim/prior authorization ID</t>
-  </si>
-  <si>
-    <t>Patient Account Number is a provider-assigned identifier</t>
-  </si>
-  <si>
-    <t>Patient demographic information for patient matching</t>
-  </si>
-  <si>
-    <t>Date of service for claim/prior authorization</t>
-  </si>
-  <si>
-    <t>Organization of provider who submitted claim/prior authorization</t>
-  </si>
-  <si>
-    <t>Claim/prior-authorization line item numbers</t>
+    <t>X12 277RFAI-v6020</t>
+  </si>
+  <si>
+    <t>X12n 278 Response-v5010</t>
+  </si>
+  <si>
+    <t>X12n 275-v6020</t>
+  </si>
+  <si>
+    <t>X12n 275-v5010</t>
+  </si>
+  <si>
+    <t>2200D  TRN01 =1, TRN02 is payer assigned control number</t>
+  </si>
+  <si>
+    <t>2000E Event level TRN01= 1current or 2 references, TRN02 =Patient event Tracking Number.   2000F Service Level TRN01=1 current and 2 reference, TRN02 = Service level tracking number</t>
+  </si>
+  <si>
+    <t>2000A TRN02</t>
+  </si>
+  <si>
+    <t>Claim</t>
+  </si>
+  <si>
+    <t>Prior Auth</t>
+  </si>
+  <si>
+    <t>2100A NM108 "PI" NM109  payer id</t>
+  </si>
+  <si>
+    <t>loop 2010A NM108 "PI" NM109  payer id</t>
+  </si>
+  <si>
+    <t>Loop 1000A NM1 segment NM109 is payer ID</t>
+  </si>
+  <si>
+    <t>Not available</t>
+  </si>
+  <si>
+    <t>2100B NM108 Qualifier, NM109 is Org ID</t>
+  </si>
+  <si>
+    <t>loop 2010B 'NM101 NM102=2, NM109=ID#</t>
+  </si>
+  <si>
+    <t>Loop 1000B NM109 qualifer 46 Electronic Transmitter ID Number</t>
+  </si>
+  <si>
+    <t>2100C NM108 Qualifier, NM109 is Provider/org ID</t>
+  </si>
+  <si>
+    <t>2010EA NM101, NM102=1,NM109=ID#</t>
+  </si>
+  <si>
+    <t>1000C NM109 qualifer of XX is provider ID which is NPI</t>
+  </si>
+  <si>
+    <t>2200D REF01=X1, REF02= provider assigned identifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2000F Service Level TRN01=1 current and 2 reference, TRN02 =  service trace number</t>
+  </si>
+  <si>
+    <t>Loop 1000D Ref Segment Qualifier Ref01=X1 Provider's Claim number and Ref02 is the number assigned by the provider</t>
+  </si>
+  <si>
+    <t>2220D SVC01 qualifier, SVC02 is the $, SVC04 is REV Code. Does not list what line this came in on in claim.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Line item level 2000F TRN01=1, TRN02 is Payer Tracking </t>
+  </si>
+  <si>
+    <t>2220D  STC01-02, STC10-02, STC11-02</t>
+  </si>
+  <si>
+    <t>2000E HI or 2000F PWK?</t>
+  </si>
+  <si>
+    <t>Loop 2200D DTP01 = 106, DTP02= D8 CCYYMMDD, DTP03 =Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We cannot find a "due date" in the 278 response.
+</t>
+  </si>
+  <si>
+    <t>2220D DTP01=472, DTP02= single date or date range, DTP03 =claim date/s</t>
+  </si>
+  <si>
+    <t>2000E event level, 2000F line level   DTP 01=742, 02=format, 03=date</t>
+  </si>
+  <si>
+    <t>Loop 2100A DTP03</t>
+  </si>
+  <si>
+    <t>2100D NM108 qualifier, NM109 is ID</t>
+  </si>
+  <si>
+    <t>2010C NM1 Segment element 08 is the  Qualifier and NM109 is the actual ID.</t>
+  </si>
+  <si>
+    <t>1000D  NM108==Qualifier MI, NM109 is the number</t>
+  </si>
+  <si>
+    <t>2100D NM102 Qualifer, NM103 last NM104 first, NM105 MI, NM107 suffix</t>
+  </si>
+  <si>
+    <t>2010C NM1 Segment element 03 is the last name, 04 is first, qualifier is NM101.</t>
+  </si>
+  <si>
+    <t>1000D  NM102 = 1 person, NM103=last name, NM104=first name, NM105=Middle Initial</t>
+  </si>
+  <si>
+    <t>2200D REF01= Qualifier, REF02=number assigned by provider</t>
+  </si>
+  <si>
+    <t>loop 2010C REF "EJ" REF02 "#"</t>
+  </si>
+  <si>
+    <t>Not available..must be pulled from the claim or the payer system</t>
+  </si>
+  <si>
+    <t>not in 227 RFAI</t>
+  </si>
+  <si>
+    <t>2010C Loop DMG01 is the qualifier and DMG02 is actual date of birth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000A STC01-01 is the code. Ex.  STC*R4:19002-5::LOI~
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loop 2000A STC10 Used to convey status of the entire claim or a specific service line. Situational.
+</t>
+  </si>
+  <si>
+    <t>2100A PER03=UR, PER04 is the payer url</t>
+  </si>
+  <si>
+    <t>loop 2010A PER07 'UR', PER08 is the payer url</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -380,13 +496,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color rgb="FF5E6C84"/>
-      <name val="Helvetica Neue"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -566,8 +683,20 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <start/>
       <end/>
@@ -682,6 +811,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <start style="thin">
+        <color auto="1"/>
+      </start>
+      <end style="thin">
+        <color auto="1"/>
+      </end>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -727,10 +871,26 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1087,86 +1247,143 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I16"/>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="40.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="70.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" customWidth="1"/>
+    <col min="5" max="5" width="19.1640625" customWidth="1"/>
+    <col min="6" max="6" width="25" customWidth="1"/>
+    <col min="7" max="7" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.5" customWidth="1"/>
+    <col min="10" max="10" width="42.5" customWidth="1"/>
+    <col min="11" max="11" width="38.6640625" customWidth="1"/>
+    <col min="12" max="12" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
-        <v>59</v>
-      </c>
-      <c r="I1" t="s">
-        <v>60</v>
+      <c r="K1" t="str">
+        <f>"&lt;span class=""bg-success"" markdown=""1""&gt;"&amp;C1&amp;"&lt;/span&gt;&lt;!-- new-content --&gt;"</f>
+        <v>&lt;span class="bg-success" markdown="1"&gt;X12 277RFAI-v6020&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+      <c r="L1" t="str">
+        <f t="shared" ref="L1:L16" si="0">"&lt;span class=""bg-success"" markdown=""1""&gt;"&amp;D1&amp;"&lt;/span&gt;&lt;!-- new-content --&gt;"</f>
+        <v>&lt;span class="bg-success" markdown="1"&gt;X12n 278 Response-v5010&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+      <c r="M1" t="str">
+        <f t="shared" ref="M1:M16" si="1">"&lt;span class=""bg-success"" markdown=""1""&gt;"&amp;E1&amp;"&lt;/span&gt;&lt;!-- new-content --&gt;"</f>
+        <v>&lt;span class="bg-success" markdown="1"&gt;X12n 275-v6020&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+      <c r="N1" t="str">
+        <f t="shared" ref="N1:N16" si="2">"&lt;span class=""bg-success"" markdown=""1""&gt;"&amp;F1&amp;"&lt;/span&gt;&lt;!-- new-content --&gt;"</f>
+        <v>&lt;span class="bg-success" markdown="1"&gt;X12n 275-v5010&lt;/span&gt;&lt;!-- new-content --&gt;</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="57" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="160" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>64</v>
+      <c r="J2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" t="str">
+        <f t="shared" ref="K2:K16" si="3">"&lt;span class=""bg-success"" markdown=""1""&gt;"&amp;C2&amp;"&lt;/span&gt;&lt;!-- new-content --&gt;"</f>
+        <v>&lt;span class="bg-success" markdown="1"&gt;2200D  TRN01 =1, TRN02 is payer assigned control number&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+      <c r="L2" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;2000E Event level TRN01= 1current or 2 references, TRN02 =Patient event Tracking Number.   2000F Service Level TRN01=1 current and 2 reference, TRN02 = Service level tracking number&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+      <c r="M2" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;2000A TRN02&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+      <c r="N2" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;2000A TRN02&lt;/span&gt;&lt;!-- new-content --&gt;</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
         <v>11</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>67</v>
       </c>
       <c r="G3" t="s">
         <v>12</v>
@@ -1175,309 +1392,633 @@
         <v>13</v>
       </c>
       <c r="I3" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="J3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;Claim&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;Prior Auth&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+      <c r="M3" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;Claim&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+      <c r="N3" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;Prior Auth&lt;/span&gt;&lt;!-- new-content --&gt;</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="119" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="F4" t="s">
+      <c r="C4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G4" t="s">
         <v>16</v>
       </c>
-      <c r="G4" t="s">
-        <v>58</v>
-      </c>
       <c r="H4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I4" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="J4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;2100A NM108 "PI" NM109  payer id&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;loop 2010A NM108 "PI" NM109  payer id&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+      <c r="M4" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;Loop 1000A NM1 segment NM109 is payer ID&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+      <c r="N4" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;Loop 1000A NM1 segment NM109 is payer ID&lt;/span&gt;&lt;!-- new-content --&gt;</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="68" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>20</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>21</v>
-      </c>
-      <c r="H5" t="s">
-        <v>22</v>
       </c>
       <c r="I5" t="s">
         <v>22</v>
       </c>
+      <c r="J5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;2100A PER03=UR, PER04 is the payer url&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;loop 2010A PER07 'UR', PER08 is the payer url&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+      <c r="M5" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;-&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+      <c r="N5" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;-&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="170" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>23</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>24</v>
       </c>
-      <c r="G6" t="s">
-        <v>27</v>
-      </c>
       <c r="H6" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="I6" t="s">
-        <v>69</v>
+        <v>26</v>
+      </c>
+      <c r="J6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;2100B NM108 Qualifier, NM109 is Org ID&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;loop 2010B 'NM101 NM102=2, NM109=ID#&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+      <c r="M6" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;Loop 1000B NM109 qualifer 46 Electronic Transmitter ID Number&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+      <c r="N6" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;-&lt;/span&gt;&lt;!-- new-content --&gt;</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="119" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" t="s">
         <v>25</v>
       </c>
-      <c r="F7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H7" t="s">
-        <v>28</v>
-      </c>
       <c r="I7" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="J7" t="s">
+        <v>29</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;2100C NM108 Qualifier, NM109 is Provider/org ID&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;2010EA NM101, NM102=1,NM109=ID#&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+      <c r="M7" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;1000C NM109 qualifer of XX is provider ID which is NPI&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+      <c r="N7" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;&lt;/span&gt;&lt;!-- new-content --&gt;</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="289" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" t="s">
         <v>19</v>
       </c>
-      <c r="G8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>65</v>
+      <c r="H8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" t="s">
+        <v>32</v>
+      </c>
+      <c r="J8" t="s">
+        <v>32</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;2200D REF01=X1, REF02= provider assigned identifier&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt; 2000F Service Level TRN01=1 current and 2 reference, TRN02 =  service trace number&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+      <c r="M8" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;Loop 1000D Ref Segment Qualifier Ref01=X1 Provider's Claim number and Ref02 is the number assigned by the provider&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+      <c r="N8" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;&lt;/span&gt;&lt;!-- new-content --&gt;</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="119" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" t="s">
-        <v>31</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F9" s="5"/>
       <c r="G9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H9" t="s">
-        <v>70</v>
+        <v>35</v>
       </c>
       <c r="I9" t="s">
-        <v>70</v>
+        <v>36</v>
+      </c>
+      <c r="J9" t="s">
+        <v>36</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;2220D SVC01 qualifier, SVC02 is the $, SVC04 is REV Code. Does not list what line this came in on in claim.&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;Line item level 2000F TRN01=1, TRN02 is Payer Tracking &lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+      <c r="M9" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;Loop 2000A STC10 Used to convey status of the entire claim or a specific service line. Situational.
+&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+      <c r="N9" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;&lt;/span&gt;&lt;!-- new-content --&gt;</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="102" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10" t="s">
-        <v>35</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F10" s="5"/>
       <c r="G10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H10" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="I10" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="J10" t="s">
+        <v>40</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;2220D  STC01-02, STC10-02, STC11-02&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;2000E HI or 2000F PWK?&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+      <c r="M10" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;2000A STC01-01 is the code. Ex.  STC*R4:19002-5::LOI~
+&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+      <c r="N10" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;&lt;/span&gt;&lt;!-- new-content --&gt;</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" ht="85" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" s="5"/>
+      <c r="G11" t="s">
         <v>19</v>
       </c>
-      <c r="G11" t="s">
-        <v>40</v>
-      </c>
       <c r="H11" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="I11" t="s">
-        <v>62</v>
+        <v>43</v>
+      </c>
+      <c r="J11" t="s">
+        <v>43</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;Loop 2200D DTP01 = 106, DTP02= D8 CCYYMMDD, DTP03 =Date&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;We cannot find a "due date" in the 278 response.
+&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+      <c r="M11" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;Not available&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+      <c r="N11" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;&lt;/span&gt;&lt;!-- new-content --&gt;</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="102" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" t="s">
-        <v>43</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F12" s="5"/>
       <c r="G12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H12" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="I12" t="s">
-        <v>68</v>
+        <v>47</v>
+      </c>
+      <c r="J12" t="s">
+        <v>47</v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;2220D DTP01=472, DTP02= single date or date range, DTP03 =claim date/s&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;2000E event level, 2000F line level   DTP 01=742, 02=format, 03=date&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+      <c r="M12" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;Loop 2100A DTP03&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+      <c r="N12" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;&lt;/span&gt;&lt;!-- new-content --&gt;</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" ht="119" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13" t="s">
-        <v>46</v>
-      </c>
-      <c r="F13" t="s">
-        <v>47</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F13" s="5"/>
       <c r="G13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I13" t="s">
-        <v>49</v>
+        <v>51</v>
+      </c>
+      <c r="J13" t="s">
+        <v>51</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;2100D NM108 qualifier, NM109 is ID&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;2010C NM1 Segment element 08 is the  Qualifier and NM109 is the actual ID.&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+      <c r="M13" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;1000D  NM108==Qualifier MI, NM109 is the number&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+      <c r="N13" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;&lt;/span&gt;&lt;!-- new-content --&gt;</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" ht="204" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
-      </c>
-      <c r="C14" t="s">
-        <v>51</v>
-      </c>
-      <c r="F14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" t="s">
         <v>19</v>
       </c>
-      <c r="G14" t="s">
-        <v>52</v>
-      </c>
       <c r="H14" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="I14" t="s">
-        <v>67</v>
+        <v>54</v>
+      </c>
+      <c r="J14" t="s">
+        <v>54</v>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;2100D NM102 Qualifer, NM103 last NM104 first, NM105 MI, NM107 suffix&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+      <c r="L14" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;2010C NM1 Segment element 03 is the last name, 04 is first, qualifier is NM101.&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+      <c r="M14" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;1000D  NM102 = 1 person, NM103=last name, NM104=first name, NM105=Middle Initial&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+      <c r="N14" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;&lt;/span&gt;&lt;!-- new-content --&gt;</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" ht="85" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" t="s">
-        <v>54</v>
-      </c>
-      <c r="F15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F15" s="5"/>
+      <c r="G15" t="s">
         <v>19</v>
       </c>
-      <c r="G15" t="s">
-        <v>48</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>66</v>
+      <c r="H15" t="s">
+        <v>50</v>
+      </c>
+      <c r="I15" t="s">
+        <v>56</v>
+      </c>
+      <c r="J15" t="s">
+        <v>56</v>
+      </c>
+      <c r="K15" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;2200D REF01= Qualifier, REF02=number assigned by provider&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+      <c r="L15" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;loop 2010C REF "EJ" REF02 "#"&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+      <c r="M15" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;Not available..must be pulled from the claim or the payer system&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+      <c r="N15" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;&lt;/span&gt;&lt;!-- new-content --&gt;</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" ht="68" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
-      </c>
-      <c r="C16" t="s">
-        <v>56</v>
-      </c>
-      <c r="F16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F16" s="5"/>
+      <c r="G16" t="s">
         <v>19</v>
       </c>
-      <c r="G16" t="s">
-        <v>57</v>
-      </c>
       <c r="H16" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="I16" t="s">
-        <v>67</v>
+        <v>54</v>
+      </c>
+      <c r="J16" t="s">
+        <v>54</v>
+      </c>
+      <c r="K16" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;not in 227 RFAI&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+      <c r="L16" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;2010C Loop DMG01 is the qualifier and DMG02 is actual date of birth&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+      <c r="M16" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;Not available..must be pulled from the claim or the payer system&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+      <c r="N16" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;span class="bg-success" markdown="1"&gt;&lt;/span&gt;&lt;!-- new-content --&gt;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated X12 element mappings and X12 required citations (FHIR-38287)
</commit_message>
<xml_diff>
--- a/input/images/data-element-mapping.xlsx
+++ b/input/images/data-element-mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/davinci-ecdx/input/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{479C103E-F463-9840-8AE7-F626EBE76960}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{CAAF3078-FA17-8C4C-8DB9-7345B8200D16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="54900" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51200" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data-element-mapping" sheetId="1" r:id="rId1"/>
@@ -35,6 +35,45 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={33F063C9-D438-2F4A-B60F-ED6425718629}</author>
+  </authors>
+  <commentList>
+    <comment ref="E10" authorId="0" shapeId="1025" xr:uid="{33F063C9-D438-2F4A-B60F-ED6425718629}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    What was the ~ at the end. it was messing up my formatting.</t>
+      </text>
+      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+        <mc:Choice Requires="v"/>
+        <mc:Fallback>
+          <commentPr defaultSize="0" autoFill="0" autoLine="0">
+            <anchor>
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>190500</xdr:colOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>1384300</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>1511300</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>749300</xdr:rowOff>
+              </to>
+            </anchor>
+          </commentPr>
+        </mc:Fallback>
+      </mc:AlternateContent>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="135" uniqueCount="105">
   <si>
@@ -342,10 +381,6 @@
     <t>2010C Loop DMG01 is the qualifier and DMG02 is actual date of birth</t>
   </si>
   <si>
-    <t xml:space="preserve">2000A STC01-01 is the code. Ex.  STC*R4:19002-5::LOI~
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Loop 2000A STC10 Used to convey status of the entire claim or a specific service line. Situational.
 </t>
   </si>
@@ -354,6 +389,9 @@
   </si>
   <si>
     <t>loop 2010A PER07 'UR', PER08 is the payer url</t>
+  </si>
+  <si>
+    <t>2000A STC01-01 is the code. Ex.  STC*R4:19002-5::LOI~</t>
   </si>
 </sst>
 </file>
@@ -949,6 +987,86 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing" xmlns:a="http://purl.oclc.org/ooxml/drawingml/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:v="urn:schemas-microsoft-com:vml" Requires="v"/>
+    <mc:Fallback>
+      <xdr:twoCellAnchor editAs="absolute">
+        <xdr:from>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>190500</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>1384300</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>1511300</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>749300</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1025" name="Comment 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4855D201-2420-0E79-C7F1-67B5AAA854FA}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1">
+              <a:spLocks noChangeArrowheads="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="7569200" y="13779500"/>
+              <a:ext cx="1320800" cy="876300"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="FFFFE1" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="80"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="510000"/>
+              </a:solidFill>
+              <a:miter lim="800%"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+            <a:effectLst/>
+            <a:extLst>
+              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+                <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                  <a:effectLst>
+                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
+                      <a:srgbClr val="510000"/>
+                    </a:outerShdw>
+                  </a:effectLst>
+                </a14:hiddenEffects>
+              </a:ext>
+              <a:ext uri="{53640926-AAD7-44D8-BBD7-CCE9431645EC}">
+                <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="1"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Fallback>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://purl.oclc.org/ooxml/spreadsheetml/main">
+  <person displayName="Eric Haas" id="{7A8DD75B-886D-EF4A-8EDA-90FC129037B5}" userId="deea5e002be8d274" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1246,12 +1364,20 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://purl.oclc.org/ooxml/spreadsheetml/main">
+  <threadedComment ref="E10" dT="2022-12-11T00:00:33.87" personId="{7A8DD75B-886D-EF4A-8EDA-90FC129037B5}" id="{33F063C9-D438-2F4A-B60F-ED6425718629}">
+    <text>What was the ~ at the end. it was messing up my formatting.</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1470,10 +1596,10 @@
         <v>18</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>103</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>104</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>19</v>
@@ -1664,7 +1790,7 @@
         <v>82</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" t="s">
@@ -1697,7 +1823,7 @@
         <v>&lt;span class="bg-success" markdown="1"&gt;&lt;/span&gt;&lt;!-- new-content --&gt;</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="102" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="68" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1711,7 +1837,7 @@
         <v>84</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" t="s">
@@ -1736,8 +1862,7 @@
       </c>
       <c r="M10" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;span class="bg-success" markdown="1"&gt;2000A STC01-01 is the code. Ex.  STC*R4:19002-5::LOI~
-&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+        <v>&lt;span class="bg-success" markdown="1"&gt;2000A STC01-01 is the code. Ex.  STC*R4:19002-5::LOI~&lt;/span&gt;&lt;!-- new-content --&gt;</v>
       </c>
       <c r="N10" t="str">
         <f t="shared" si="2"/>
@@ -2023,5 +2148,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="v">
+      <legacyDrawing r:id="rId2"/>
+    </mc:Choice>
+  </mc:AlternateContent>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Clarify in operation that either an OrganizationId or ProviderId is required. Allow for both Ids to be sent in request.FHIR-38189
</commit_message>
<xml_diff>
--- a/input/images/data-element-mapping.xlsx
+++ b/input/images/data-element-mapping.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/davinci-ecdx/input/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{8816B4C3-E1CE-C447-8307-8CD98B42D10D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{8DA11A81-40D5-2546-B20E-641C53B039B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51200" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data-element-mapping" sheetId="1" r:id="rId1"/>
-    <sheet name="TrimAll Macro" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -57,14 +56,14 @@
               <from>
                 <xdr:col>5</xdr:col>
                 <xdr:colOff>190500</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>1384300</xdr:rowOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>736600</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>5</xdr:col>
                 <xdr:colOff>1511300</xdr:colOff>
-                <xdr:row>9</xdr:row>
-                <xdr:rowOff>749300</xdr:rowOff>
+                <xdr:row>13</xdr:row>
+                <xdr:rowOff>101600</xdr:rowOff>
               </to>
             </anchor>
           </commentPr>
@@ -76,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="136" uniqueCount="106">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="135" uniqueCount="106">
   <si>
     <t>No</t>
   </si>
@@ -151,9 +150,6 @@
   </si>
   <si>
     <t>OrganizationId</t>
-  </si>
-  <si>
-    <t>Task.owner.identifier</t>
   </si>
   <si>
     <t>Organization of provider who submitted claim/prior authorization</t>
@@ -395,31 +391,237 @@
     <t>2000A STC01-01 is the code. Ex.  STC*R4:19002-5::LOI~</t>
   </si>
   <si>
-    <t>Sub a_TrimALL()
-'David McRitchie 2000-07-03 mod 2000-08-16
-    Application.ScreenUpdating = False
-    Application.Calculation = xlCalculationManual
-    Dim cell As Range
-    'Also Treat CHR 0160, as a space (CHR 032)
-    Selection.Replace what:=Chr(160), Replacement:=Chr(32), _
-                      LookAt:=xlPart, SearchOrder:=xlByRows, MatchCase:=False
-    'Trim in Excel removes extra internal spaces, VBA does not
-    On Error Resume Next   'in case no text cells in selection
-    For Each cell In Intersect(Selection, _
-                               Selection.SpecialCells(xlConstants, xlTextValues))
-        cell.Value = Application.Trim(cell.Value)
-    Next cell
-    On Error GoTo 0
-    Application.Calculation = xlCalculationAutomatic
-    Application.ScreenUpdating = True
-End Sub</t>
+    <r>
+      <t>&lt;span</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFE50000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>class</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>"bg-success"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFE50000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>markdown</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>"1"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF800000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>PractitionerRole.practitioner.identifier</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF800000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&lt;/span&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&lt;!-- new-content --&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;span</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFE50000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>class</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>"bg-success"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFE50000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>markdown</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>"1"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF800000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>PractitionerRole.organization.identifier</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF800000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&lt;/span&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&lt;!-- new-content --&gt;</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -560,6 +762,36 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF800000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFE50000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0000FF"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF008000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="35">
@@ -930,7 +1162,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -950,9 +1182,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1022,21 +1251,21 @@
         <xdr:from>
           <xdr:col>5</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
-          <xdr:row>8</xdr:row>
-          <xdr:rowOff>1384300</xdr:rowOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>736600</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>5</xdr:col>
           <xdr:colOff>1511300</xdr:colOff>
-          <xdr:row>9</xdr:row>
-          <xdr:rowOff>749300</xdr:rowOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>101600</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1025" name="Comment 1" hidden="1">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB6496BC-255D-35EE-9DC5-F8BBC9E03AC7}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{217D5894-3DF0-95E3-68D9-F54F10FB725E}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1400,8 +1629,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1428,16 +1657,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
@@ -1476,16 +1705,16 @@
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>65</v>
-      </c>
       <c r="F2" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G2" t="s">
         <v>7</v>
@@ -1524,16 +1753,16 @@
         <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="E3" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>67</v>
       </c>
       <c r="G3" t="s">
         <v>12</v>
@@ -1572,16 +1801,16 @@
         <v>15</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E4" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>70</v>
-      </c>
       <c r="F4" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G4" t="s">
         <v>16</v>
@@ -1620,10 +1849,10 @@
         <v>18</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>102</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>103</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>19</v>
@@ -1660,7 +1889,7 @@
         <v>&lt;span class="bg-success" markdown="1"&gt;-&lt;/span&gt;&lt;!-- new-content --&gt;</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="170" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="68" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1668,13 +1897,13 @@
         <v>23</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="E6" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>74</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>19</v>
@@ -1683,13 +1912,13 @@
         <v>24</v>
       </c>
       <c r="H6" t="s">
+        <v>104</v>
+      </c>
+      <c r="I6" t="s">
         <v>25</v>
       </c>
-      <c r="I6" t="s">
-        <v>26</v>
-      </c>
       <c r="J6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" si="3"/>
@@ -1708,34 +1937,34 @@
         <v>&lt;span class="bg-success" markdown="1"&gt;-&lt;/span&gt;&lt;!-- new-content --&gt;</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="119" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="68" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="E7" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>77</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" t="s">
+        <v>105</v>
+      </c>
+      <c r="I7" t="s">
         <v>28</v>
       </c>
-      <c r="H7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I7" t="s">
-        <v>29</v>
-      </c>
       <c r="J7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K7" t="str">
         <f t="shared" si="3"/>
@@ -1754,34 +1983,34 @@
         <v>&lt;span class="bg-success" markdown="1"&gt;&lt;/span&gt;&lt;!-- new-content --&gt;</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="289" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="119" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>80</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" t="s">
         <v>19</v>
       </c>
       <c r="H8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8" t="s">
         <v>31</v>
       </c>
-      <c r="I8" t="s">
-        <v>32</v>
-      </c>
       <c r="J8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K8" t="str">
         <f t="shared" si="3"/>
@@ -1805,29 +2034,29 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>82</v>
-      </c>
       <c r="E9" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" t="s">
         <v>34</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>35</v>
       </c>
-      <c r="I9" t="s">
-        <v>36</v>
-      </c>
       <c r="J9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K9" t="str">
         <f t="shared" si="3"/>
@@ -1852,29 +2081,29 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>84</v>
-      </c>
       <c r="E10" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" t="s">
         <v>38</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>39</v>
       </c>
-      <c r="I10" t="s">
-        <v>40</v>
-      </c>
       <c r="J10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K10" t="str">
         <f t="shared" si="3"/>
@@ -1898,29 +2127,29 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>86</v>
-      </c>
       <c r="E11" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" t="s">
         <v>19</v>
       </c>
       <c r="H11" t="s">
+        <v>41</v>
+      </c>
+      <c r="I11" t="s">
         <v>42</v>
       </c>
-      <c r="I11" t="s">
-        <v>43</v>
-      </c>
       <c r="J11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K11" t="str">
         <f t="shared" si="3"/>
@@ -1945,29 +2174,29 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>89</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12" t="s">
         <v>45</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>46</v>
       </c>
-      <c r="I12" t="s">
-        <v>47</v>
-      </c>
       <c r="J12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K12" t="str">
         <f t="shared" si="3"/>
@@ -1991,29 +2220,29 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="E13" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>92</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" t="s">
+        <v>48</v>
+      </c>
+      <c r="H13" t="s">
         <v>49</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>50</v>
       </c>
-      <c r="I13" t="s">
-        <v>51</v>
-      </c>
       <c r="J13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K13" t="str">
         <f t="shared" si="3"/>
@@ -2037,29 +2266,29 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="E14" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>95</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" t="s">
         <v>19</v>
       </c>
       <c r="H14" t="s">
+        <v>52</v>
+      </c>
+      <c r="I14" t="s">
         <v>53</v>
       </c>
-      <c r="I14" t="s">
-        <v>54</v>
-      </c>
       <c r="J14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K14" t="str">
         <f t="shared" si="3"/>
@@ -2083,29 +2312,29 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C15" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="F15" s="5"/>
       <c r="G15" t="s">
         <v>19</v>
       </c>
       <c r="H15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K15" t="str">
         <f t="shared" si="3"/>
@@ -2129,29 +2358,29 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C16" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>100</v>
-      </c>
       <c r="E16" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F16" s="5"/>
       <c r="G16" t="s">
         <v>19</v>
       </c>
       <c r="H16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" si="3"/>
@@ -2179,27 +2408,4 @@
     </mc:Choice>
   </mc:AlternateContent>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34811B7E-80CD-1B49-B950-9C741D1F8644}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="197" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
-        <v>105</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Expand Attachments and Task based approach to support Questionnaires and DTR (FHIR-38241) : Documentation
</commit_message>
<xml_diff>
--- a/input/images/data-element-mapping.xlsx
+++ b/input/images/data-element-mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/davinci-ecdx/input/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{8DA11A81-40D5-2546-B20E-641C53B039B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{76DA61EA-9D8F-8942-AADD-53B57840915B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-68800" yWindow="-18720" windowWidth="68800" windowHeight="28800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data-element-mapping" sheetId="1" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="135" uniqueCount="106">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="139" uniqueCount="110">
   <si>
     <t>No</t>
   </si>
@@ -615,6 +615,18 @@
       </rPr>
       <t>&lt;!-- new-content --&gt;</t>
     </r>
+  </si>
+  <si>
+    <t>&lt;span class="bg-success" markdown="1"&gt;“questionnaire” Task.input &lt;/span&gt;&lt;!-- new-content --&gt;</t>
+  </si>
+  <si>
+    <t>&lt;span class="bg-success" markdown="1"&gt;Questionnaire&lt;/span&gt;&lt;!-- new-content --&gt;</t>
+  </si>
+  <si>
+    <t>&lt;span class="bg-success" markdown="1"&gt;QuestionnaireResponse&lt;/span&gt;&lt;!-- new-content --&gt;</t>
+  </si>
+  <si>
+    <t>&lt;span class="bg-success" markdown="1"&gt;Attachment.Content&lt;/span&gt;&lt;!-- new-content --&gt;</t>
   </si>
 </sst>
 </file>
@@ -1265,7 +1277,7 @@
             <xdr:cNvPr id="1025" name="Comment 1" hidden="1">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{217D5894-3DF0-95E3-68D9-F54F10FB725E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5707AC75-2C86-7EB6-06AE-BC66365F2DE6}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1276,7 +1288,7 @@
           <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="7569200" y="13779500"/>
-              <a:ext cx="1320800" cy="876300"/>
+              <a:ext cx="1320800" cy="228600"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1323,7 +1335,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office Theme">
+<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1611,7 +1623,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1627,10 +1639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1729,7 +1741,7 @@
         <v>10</v>
       </c>
       <c r="K2" t="str">
-        <f t="shared" ref="K2:K16" si="3">"&lt;span class=""bg-success"" markdown=""1""&gt;"&amp;C2&amp;"&lt;/span&gt;&lt;!-- new-content --&gt;"</f>
+        <f t="shared" ref="K2:K17" si="3">"&lt;span class=""bg-success"" markdown=""1""&gt;"&amp;C2&amp;"&lt;/span&gt;&lt;!-- new-content --&gt;"</f>
         <v>&lt;span class="bg-success" markdown="1"&gt;2200D  TRN01 =1, TRN02 is payer assigned control number&lt;/span&gt;&lt;!-- new-content --&gt;</v>
       </c>
       <c r="L2" t="str">
@@ -2215,7 +2227,7 @@
         <v>&lt;span class="bg-success" markdown="1"&gt;&lt;/span&gt;&lt;!-- new-content --&gt;</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="119" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" ht="68" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2261,7 +2273,7 @@
         <v>&lt;span class="bg-success" markdown="1"&gt;&lt;/span&gt;&lt;!-- new-content --&gt;</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="204" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" ht="85" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2397,6 +2409,28 @@
       <c r="N16" t="str">
         <f t="shared" si="2"/>
         <v>&lt;span class="bg-success" markdown="1"&gt;&lt;/span&gt;&lt;!-- new-content --&gt;</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>107</v>
+      </c>
+      <c r="H17" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>108</v>
+      </c>
+      <c r="G18" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Normalize term “prior authorization” FHIR-38186
</commit_message>
<xml_diff>
--- a/input/images/data-element-mapping.xlsx
+++ b/input/images/data-element-mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/davinci-ecdx/input/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{76DA61EA-9D8F-8942-AADD-53B57840915B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{FB31007F-A755-864B-80A4-FF6D9FA4BD0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-68800" yWindow="-18720" windowWidth="68800" windowHeight="28800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-68800" yWindow="-18220" windowWidth="68800" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data-element-mapping" sheetId="1" r:id="rId1"/>
@@ -182,9 +182,6 @@
     <t>“code” Task.input.extension</t>
   </si>
   <si>
-    <t>Claim/prior-authorization line item numbers</t>
-  </si>
-  <si>
     <t>LOINC Attachment Code</t>
   </si>
   <si>
@@ -627,6 +624,9 @@
   </si>
   <si>
     <t>&lt;span class="bg-success" markdown="1"&gt;Attachment.Content&lt;/span&gt;&lt;!-- new-content --&gt;</t>
+  </si>
+  <si>
+    <t>Claim/prior authorization line item numbers</t>
   </si>
 </sst>
 </file>
@@ -1277,7 +1277,7 @@
             <xdr:cNvPr id="1025" name="Comment 1" hidden="1">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5707AC75-2C86-7EB6-06AE-BC66365F2DE6}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE859A5C-DCBA-D1D5-879C-EA5514077B18}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1641,8 +1641,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1669,16 +1669,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
@@ -1717,16 +1717,16 @@
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>64</v>
-      </c>
       <c r="F2" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G2" t="s">
         <v>7</v>
@@ -1741,7 +1741,7 @@
         <v>10</v>
       </c>
       <c r="K2" t="str">
-        <f t="shared" ref="K2:K17" si="3">"&lt;span class=""bg-success"" markdown=""1""&gt;"&amp;C2&amp;"&lt;/span&gt;&lt;!-- new-content --&gt;"</f>
+        <f t="shared" ref="K2:K16" si="3">"&lt;span class=""bg-success"" markdown=""1""&gt;"&amp;C2&amp;"&lt;/span&gt;&lt;!-- new-content --&gt;"</f>
         <v>&lt;span class="bg-success" markdown="1"&gt;2200D  TRN01 =1, TRN02 is payer assigned control number&lt;/span&gt;&lt;!-- new-content --&gt;</v>
       </c>
       <c r="L2" t="str">
@@ -1765,16 +1765,16 @@
         <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>66</v>
-      </c>
       <c r="E3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>65</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>66</v>
       </c>
       <c r="G3" t="s">
         <v>12</v>
@@ -1813,16 +1813,16 @@
         <v>15</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E4" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>69</v>
-      </c>
       <c r="F4" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G4" t="s">
         <v>16</v>
@@ -1861,10 +1861,10 @@
         <v>18</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>101</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>102</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>19</v>
@@ -1909,13 +1909,13 @@
         <v>23</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="E6" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>73</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>19</v>
@@ -1924,7 +1924,7 @@
         <v>24</v>
       </c>
       <c r="H6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I6" t="s">
         <v>25</v>
@@ -1957,20 +1957,20 @@
         <v>26</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="E7" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" t="s">
         <v>27</v>
       </c>
       <c r="H7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I7" t="s">
         <v>28</v>
@@ -2003,13 +2003,13 @@
         <v>29</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>79</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" t="s">
@@ -2049,13 +2049,13 @@
         <v>32</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>81</v>
-      </c>
       <c r="E9" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" t="s">
@@ -2065,10 +2065,10 @@
         <v>34</v>
       </c>
       <c r="I9" t="s">
-        <v>35</v>
+        <v>109</v>
       </c>
       <c r="J9" t="s">
-        <v>35</v>
+        <v>109</v>
       </c>
       <c r="K9" t="str">
         <f t="shared" si="3"/>
@@ -2093,29 +2093,29 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>83</v>
-      </c>
       <c r="E10" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" t="s">
         <v>37</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>38</v>
       </c>
-      <c r="I10" t="s">
-        <v>39</v>
-      </c>
       <c r="J10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K10" t="str">
         <f t="shared" si="3"/>
@@ -2139,29 +2139,29 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>85</v>
-      </c>
       <c r="E11" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" t="s">
         <v>19</v>
       </c>
       <c r="H11" t="s">
+        <v>40</v>
+      </c>
+      <c r="I11" t="s">
         <v>41</v>
       </c>
-      <c r="I11" t="s">
-        <v>42</v>
-      </c>
       <c r="J11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K11" t="str">
         <f t="shared" si="3"/>
@@ -2186,29 +2186,29 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>87</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>88</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" t="s">
+        <v>43</v>
+      </c>
+      <c r="H12" t="s">
         <v>44</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>45</v>
       </c>
-      <c r="I12" t="s">
-        <v>46</v>
-      </c>
       <c r="J12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K12" t="str">
         <f t="shared" si="3"/>
@@ -2232,29 +2232,29 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="E13" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>91</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" t="s">
+        <v>47</v>
+      </c>
+      <c r="H13" t="s">
         <v>48</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>49</v>
       </c>
-      <c r="I13" t="s">
-        <v>50</v>
-      </c>
       <c r="J13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K13" t="str">
         <f t="shared" si="3"/>
@@ -2278,29 +2278,29 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="E14" s="3" t="s">
         <v>93</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>94</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" t="s">
         <v>19</v>
       </c>
       <c r="H14" t="s">
+        <v>51</v>
+      </c>
+      <c r="I14" t="s">
         <v>52</v>
       </c>
-      <c r="I14" t="s">
-        <v>53</v>
-      </c>
       <c r="J14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K14" t="str">
         <f t="shared" si="3"/>
@@ -2324,29 +2324,29 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C15" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>97</v>
       </c>
       <c r="F15" s="5"/>
       <c r="G15" t="s">
         <v>19</v>
       </c>
       <c r="H15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K15" t="str">
         <f t="shared" si="3"/>
@@ -2370,29 +2370,29 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C16" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>99</v>
-      </c>
       <c r="E16" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F16" s="5"/>
       <c r="G16" t="s">
         <v>19</v>
       </c>
       <c r="H16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" si="3"/>
@@ -2416,10 +2416,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -2427,10 +2427,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>107</v>
+      </c>
+      <c r="G18" t="s">
         <v>108</v>
-      </c>
-      <c r="G18" t="s">
-        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correct operation name FHIR-38253
</commit_message>
<xml_diff>
--- a/input/images/data-element-mapping.xlsx
+++ b/input/images/data-element-mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/davinci-ecdx/input/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{FB31007F-A755-864B-80A4-FF6D9FA4BD0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{11DCAAAF-1000-EC47-8F51-C1B91CB17EB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-68800" yWindow="-18220" windowWidth="68800" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-68800" yWindow="-18220" windowWidth="34400" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data-element-mapping" sheetId="1" r:id="rId1"/>
@@ -143,9 +143,6 @@
     <t>"payer-url" Task.input</t>
   </si>
   <si>
-    <t>Payer endpoint where the attachments are submitted using the $submit-operation</t>
-  </si>
-  <si>
     <t>Organization ID</t>
   </si>
   <si>
@@ -627,6 +624,9 @@
   </si>
   <si>
     <t>Claim/prior authorization line item numbers</t>
+  </si>
+  <si>
+    <t>Payer endpoint where the attachments are submitted using the $submit-attachment operation</t>
   </si>
 </sst>
 </file>
@@ -1277,7 +1277,7 @@
             <xdr:cNvPr id="1025" name="Comment 1" hidden="1">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE859A5C-DCBA-D1D5-879C-EA5514077B18}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FEDADC37-B29C-0A45-6525-7E65111F001F}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1641,8 +1641,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1669,16 +1669,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
@@ -1717,16 +1717,16 @@
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>63</v>
-      </c>
       <c r="F2" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G2" t="s">
         <v>7</v>
@@ -1765,16 +1765,16 @@
         <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>65</v>
-      </c>
       <c r="E3" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>65</v>
       </c>
       <c r="G3" t="s">
         <v>12</v>
@@ -1813,16 +1813,16 @@
         <v>15</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E4" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>68</v>
-      </c>
       <c r="F4" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G4" t="s">
         <v>16</v>
@@ -1861,10 +1861,10 @@
         <v>18</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>100</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>101</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>19</v>
@@ -1879,10 +1879,10 @@
         <v>21</v>
       </c>
       <c r="I5" t="s">
-        <v>22</v>
+        <v>109</v>
       </c>
       <c r="J5" t="s">
-        <v>22</v>
+        <v>109</v>
       </c>
       <c r="K5" t="str">
         <f t="shared" si="3"/>
@@ -1906,31 +1906,31 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="E6" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>72</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>19</v>
       </c>
       <c r="G6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" t="s">
+        <v>102</v>
+      </c>
+      <c r="I6" t="s">
         <v>24</v>
       </c>
-      <c r="H6" t="s">
-        <v>103</v>
-      </c>
-      <c r="I6" t="s">
-        <v>25</v>
-      </c>
       <c r="J6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" si="3"/>
@@ -1954,29 +1954,29 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="E7" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>75</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" t="s">
+        <v>103</v>
+      </c>
+      <c r="I7" t="s">
         <v>27</v>
       </c>
-      <c r="H7" t="s">
-        <v>104</v>
-      </c>
-      <c r="I7" t="s">
-        <v>28</v>
-      </c>
       <c r="J7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K7" t="str">
         <f t="shared" si="3"/>
@@ -2000,29 +2000,29 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>77</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>78</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" t="s">
         <v>19</v>
       </c>
       <c r="H8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" t="s">
         <v>30</v>
       </c>
-      <c r="I8" t="s">
-        <v>31</v>
-      </c>
       <c r="J8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K8" t="str">
         <f t="shared" si="3"/>
@@ -2046,29 +2046,29 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>80</v>
-      </c>
       <c r="E9" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" t="s">
         <v>33</v>
       </c>
-      <c r="H9" t="s">
-        <v>34</v>
-      </c>
       <c r="I9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K9" t="str">
         <f t="shared" si="3"/>
@@ -2093,29 +2093,29 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>82</v>
-      </c>
       <c r="E10" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" t="s">
         <v>36</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>37</v>
       </c>
-      <c r="I10" t="s">
-        <v>38</v>
-      </c>
       <c r="J10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K10" t="str">
         <f t="shared" si="3"/>
@@ -2139,29 +2139,29 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>84</v>
-      </c>
       <c r="E11" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" t="s">
         <v>19</v>
       </c>
       <c r="H11" t="s">
+        <v>39</v>
+      </c>
+      <c r="I11" t="s">
         <v>40</v>
       </c>
-      <c r="I11" t="s">
-        <v>41</v>
-      </c>
       <c r="J11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K11" t="str">
         <f t="shared" si="3"/>
@@ -2186,29 +2186,29 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>87</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" t="s">
+        <v>42</v>
+      </c>
+      <c r="H12" t="s">
         <v>43</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>44</v>
       </c>
-      <c r="I12" t="s">
-        <v>45</v>
-      </c>
       <c r="J12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K12" t="str">
         <f t="shared" si="3"/>
@@ -2232,29 +2232,29 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="E13" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>90</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13" t="s">
         <v>47</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>48</v>
       </c>
-      <c r="I13" t="s">
-        <v>49</v>
-      </c>
       <c r="J13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K13" t="str">
         <f t="shared" si="3"/>
@@ -2278,29 +2278,29 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="E14" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>93</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" t="s">
         <v>19</v>
       </c>
       <c r="H14" t="s">
+        <v>50</v>
+      </c>
+      <c r="I14" t="s">
         <v>51</v>
       </c>
-      <c r="I14" t="s">
-        <v>52</v>
-      </c>
       <c r="J14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K14" t="str">
         <f t="shared" si="3"/>
@@ -2324,29 +2324,29 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C15" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>96</v>
       </c>
       <c r="F15" s="5"/>
       <c r="G15" t="s">
         <v>19</v>
       </c>
       <c r="H15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K15" t="str">
         <f t="shared" si="3"/>
@@ -2370,29 +2370,29 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C16" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>98</v>
-      </c>
       <c r="E16" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F16" s="5"/>
       <c r="G16" t="s">
         <v>19</v>
       </c>
       <c r="H16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" si="3"/>
@@ -2416,10 +2416,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -2427,10 +2427,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>106</v>
+      </c>
+      <c r="G18" t="s">
         <v>107</v>
-      </c>
-      <c r="G18" t="s">
-        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update files for IG build
</commit_message>
<xml_diff>
--- a/input/images/data-element-mapping.xlsx
+++ b/input/images/data-element-mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/davinci-ecdx/input/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{55E3F906-2D6B-1847-8F7E-3038E906D307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{88719C09-83BD-3046-AE70-EF981373A8B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4880" yWindow="500" windowWidth="37340" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51200" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data-element-mapping" sheetId="1" r:id="rId1"/>
@@ -35,47 +35,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={33F063C9-D438-2F4A-B60F-ED6425718629}</author>
-  </authors>
-  <commentList>
-    <comment ref="E10" authorId="0" shapeId="1025" xr:uid="{33F063C9-D438-2F4A-B60F-ED6425718629}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    What was the ~ at the end. it was messing up my formatting.</t>
-      </text>
-      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-        <mc:Choice Requires="v"/>
-        <mc:Fallback>
-          <commentPr defaultSize="0" autoFill="0" autoLine="0">
-            <anchor>
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>622300</xdr:colOff>
-                <xdr:row>13</xdr:row>
-                <xdr:rowOff>1041400</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>2425700</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
-              </to>
-            </anchor>
-          </commentPr>
-        </mc:Fallback>
-      </mc:AlternateContent>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="133" uniqueCount="104">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="271" uniqueCount="177">
   <si>
     <t>No</t>
   </si>
@@ -83,6 +44,15 @@
     <t>Data Element</t>
   </si>
   <si>
+    <t>X12 277RFAI-v6020</t>
+  </si>
+  <si>
+    <t>X12n 278 Response-v5010</t>
+  </si>
+  <si>
+    <t>X12n 275-v6020</t>
+  </si>
+  <si>
     <t>CDex $submit-attachment Parameter</t>
   </si>
   <si>
@@ -95,21 +65,39 @@
     <t>Request Attachments Comments</t>
   </si>
   <si>
+    <t>ClaimResponse (from PAS Response Bundle)</t>
+  </si>
+  <si>
+    <t>PAS Response Bundle</t>
+  </si>
+  <si>
+    <t>Tracking ID</t>
+  </si>
+  <si>
+    <t>Loop: 2200D Segment: TRN02 Notes: TRN01 = "1"</t>
+  </si>
+  <si>
+    <t>Loop: 2000A Segment: TRN02</t>
+  </si>
+  <si>
     <t>TrackingId</t>
   </si>
   <si>
     <t>Task.identifier</t>
   </si>
   <si>
-    <t>&lt;span class="bg-success" markdown="1"&gt;For *unsolicited* attachments, this is the provider-assigned tracking/control number. For *solicited* attachments, this is the payer-assigned tracking/control number.&lt;/span&gt;&lt;!-- new-content --&gt;</t>
-  </si>
-  <si>
-    <t>&lt;span class="bg-success" markdown="1"&gt;Payer-assigned tracking/control number&lt;/span&gt;&lt;!-- new-content --&gt;</t>
+    <t>ClaimResponse = Bundle.entry[0].resource, CommunicationRequest = Bundle.entry[n].resource referenced by ClaimResponse.communincationRequest</t>
   </si>
   <si>
     <t>Use</t>
   </si>
   <si>
+    <t>Claim</t>
+  </si>
+  <si>
+    <t>Prior Auth</t>
+  </si>
+  <si>
     <t>AttachTo</t>
   </si>
   <si>
@@ -119,18 +107,42 @@
     <t>Choice of "claim" or "preauthorization"</t>
   </si>
   <si>
+    <t>preauthorization</t>
+  </si>
+  <si>
+    <t>Fixed to "preauthorization"</t>
+  </si>
+  <si>
     <t>Payer ID</t>
   </si>
   <si>
+    <t>Loop: 2100A Segment: NM109 Notes: NM108 = "PI"</t>
+  </si>
+  <si>
+    <t>Loop: 2010A Segment: NM109 Notes: NM108 = "PI"</t>
+  </si>
+  <si>
+    <t>Loop: 1000A Segment: NM109</t>
+  </si>
+  <si>
     <t>PayerId</t>
   </si>
   <si>
     <t>Task.requester.identifier</t>
   </si>
   <si>
+    <t>out of band</t>
+  </si>
+  <si>
     <t>Payer URL</t>
   </si>
   <si>
+    <t>Loop: 2100A Segment: PER04 Notes: PER03 = "UR"</t>
+  </si>
+  <si>
+    <t>Loop: 2010A Segment: PER08 Notes: PER07 = "UR"</t>
+  </si>
+  <si>
     <t>-</t>
   </si>
   <si>
@@ -140,45 +152,114 @@
     <t>"payer-url" Task.input</t>
   </si>
   <si>
+    <t>Payer endpoint where the attachments are submitted using the $submit-attachment operation</t>
+  </si>
+  <si>
+    <t>ClaimResponse.insurer: Organization.identifier</t>
+  </si>
+  <si>
+    <t>ClaimResponse = Bundle.entry[0].resource, Organization = Bundle.entry[n].resource referenced by ClaimResponse.insurer</t>
+  </si>
+  <si>
     <t>Organization ID</t>
   </si>
   <si>
+    <t>Loop: 2100B Segment: NM109 Notes: NM108 = id code qualifier</t>
+  </si>
+  <si>
+    <t>Loop: 2010B Segment: NM109 Notes: NM101 = id code qualifier, NM102 = "2"</t>
+  </si>
+  <si>
+    <t>Loop: 1000B Segment: NM109 Notes: NM108="46"</t>
+  </si>
+  <si>
     <t>OrganizationId</t>
   </si>
   <si>
+    <t>PractitionerRole.practitioner.identifier</t>
+  </si>
+  <si>
     <t>Organization of provider who submitted claim/prior authorization</t>
   </si>
   <si>
     <t>Provider ID</t>
   </si>
   <si>
+    <t>Loop: 2100C Segment: NM109 Notes: NM108 = id code qualifier</t>
+  </si>
+  <si>
+    <t>Loop: 2010EA Segment: NM109 Notes: NM101 = id code qualifier , NM102 = "1"</t>
+  </si>
+  <si>
+    <t>Loop: 1000C Segment: NM109 Notes: NM108="XX"</t>
+  </si>
+  <si>
     <t>ProviderId</t>
   </si>
   <si>
+    <t>PractitionerRole.organization.identifier</t>
+  </si>
+  <si>
     <t>Provider who submitted claim/prior authorization</t>
   </si>
   <si>
     <t>Claim/PreAuth ID</t>
   </si>
   <si>
+    <t>Loop: 2200D Segment: REF02 Notes: REF01="X1"</t>
+  </si>
+  <si>
+    <t>Loop: 2000F Segment: TRN02 Notes: TRN01 ="1" or TRN01 ="2"</t>
+  </si>
+  <si>
+    <t>Loop: 1000D Segment: Ref02 Notes: Ref01="X1", provider assigned</t>
+  </si>
+  <si>
     <t>Task.reasonReference.identifier</t>
   </si>
   <si>
-    <t>&lt;span class="bg-success" markdown="1"&gt;Provider-assigned claim/prior authorization ID&lt;/span&gt;&lt;!-- new-content --&gt;</t>
+    <t>ClaimResponse.request: Claim.identifier</t>
+  </si>
+  <si>
+    <t>ClaimResponse = Bundle.entry[0].resource, Claim = Bundle.entry[n].resource referenced by ClaimResponse.request</t>
   </si>
   <si>
     <t>Line Item(s)</t>
   </si>
   <si>
+    <t>Loop: 2220D Notes: SVC01 = id code qualifier, SVC02 is the claim amount, SVC04 is REV Code, Does not list line item</t>
+  </si>
+  <si>
+    <t>Loop: 2000F Segment: TRN02 Notes: TRN01 = "1"</t>
+  </si>
+  <si>
+    <t>Loop: 2000A Segment: STC10 Notes: Used to convey status of the entire claim or a specific service line</t>
+  </si>
+  <si>
     <t>Attachment.LineItem</t>
   </si>
   <si>
     <t>“code” Task.input.extension</t>
   </si>
   <si>
+    <t>Claim/prior authorization line item numbers</t>
+  </si>
+  <si>
+    <t>ClaimResponse = Bundle.entry[0].resource</t>
+  </si>
+  <si>
     <t>LOINC Attachment Code</t>
   </si>
   <si>
+    <t>Loop: 2220D Segments: STC01-02, STC10-02, STC11-02</t>
+  </si>
+  <si>
+    <t>Loop: 2000E Segment: HI?? or Loop: 2000F Segment: PWK?? Notes: Clarify!</t>
+  </si>
+  <si>
+    <t>Loop: 2000A Segment: STC01-01</t>
+  </si>
+  <si>
     <t>Attachment.Code</t>
   </si>
   <si>
@@ -191,15 +272,30 @@
     <t>Due Date</t>
   </si>
   <si>
+    <t>Loop: 2200D Segment: DTP03 Notes: DTP01 = "106", DTP02 = "D8"</t>
+  </si>
+  <si>
     <t>Task.restriction.period</t>
   </si>
   <si>
     <t>Deadline for submitting attachments to Payer</t>
   </si>
   <si>
+    <t>?</t>
+  </si>
+  <si>
     <t>Date of Service</t>
   </si>
   <si>
+    <t>Loop: 2200D Segment: DTP03 Notes: DTP01 = "172", DTP02 = "D8" or DTP02 = "RD8"</t>
+  </si>
+  <si>
+    <t>Loop: 2000E (event level) or 2000F (line level) Segment: DTP03 Notes: DTP01="742" DTP02 = date format code</t>
+  </si>
+  <si>
+    <t>Loop: 2100A Segment: DTP03</t>
+  </si>
+  <si>
     <t>ServiceDate</t>
   </si>
   <si>
@@ -209,9 +305,18 @@
     <t>Date of service for claim/prior authorization</t>
   </si>
   <si>
+    <t>ClaimResponse.item.extension:requestedServiceDate</t>
+  </si>
+  <si>
     <t>Member ID</t>
   </si>
   <si>
+    <t>Loop: 2010C Segment: NM109 Notes: NM108 = id code qualifier</t>
+  </si>
+  <si>
+    <t>Loop: 1000D Segment: NM109 Notes: NM108="MI"</t>
+  </si>
+  <si>
     <t>MemberId</t>
   </si>
   <si>
@@ -221,179 +326,254 @@
     <t>Payer assigned patient identifier</t>
   </si>
   <si>
+    <t>ClaimResponse.patient: Patient.identifer</t>
+  </si>
+  <si>
+    <t>ClaimResponse = Bundle.entry[0].resource, Patient = Bundle.entry[n].resource referenced by ClaimResponse.patient</t>
+  </si>
+  <si>
     <t>Patient Name</t>
   </si>
   <si>
+    <t>Loop: 2100D Segments :NM103, NM104, NM105, NM107 Notes: NM102 = "1"</t>
+  </si>
+  <si>
+    <t>Loop: 2010C Segments: NM103, NM104 Notes: NM101 = id code qualifier</t>
+  </si>
+  <si>
+    <t>Loop: 1000D Segments: NM103, NM104, NM105 Notes: NM102 = "1"</t>
+  </si>
+  <si>
     <t>Patient.name</t>
   </si>
   <si>
     <t>Patient demographic information for patient matching</t>
   </si>
   <si>
+    <t>ClaimResponse.patient: Patient.name</t>
+  </si>
+  <si>
     <t>Patient Account No.</t>
   </si>
   <si>
-    <t>&lt;span class="bg-success" markdown="1"&gt;Patient Account Number is a provider-assigned identifier&lt;/span&gt;&lt;!-- new-content --&gt;</t>
+    <t>Loop: 2220D Segments: REF02 Notes: REF01= id code qualifier</t>
+  </si>
+  <si>
+    <t>Loop: 2010C Segment: REF02 Notes: REF01 = "EJ"</t>
   </si>
   <si>
     <t>Date of Birth</t>
   </si>
   <si>
+    <t>Loop: 2010C Segment: DMG02 Notes: DMG01 = date format code</t>
+  </si>
+  <si>
     <t>Patient.birthDate</t>
   </si>
   <si>
-    <t>X12 277RFAI-v6020</t>
-  </si>
-  <si>
-    <t>X12n 278 Response-v5010</t>
-  </si>
-  <si>
-    <t>X12n 275-v6020</t>
-  </si>
-  <si>
-    <t>Claim</t>
-  </si>
-  <si>
-    <t>Prior Auth</t>
-  </si>
-  <si>
-    <t>Claim/prior authorization line item numbers</t>
-  </si>
-  <si>
-    <t>Payer endpoint where the attachments are submitted using the $submit-attachment operation</t>
-  </si>
-  <si>
-    <t>Tracking ID</t>
-  </si>
-  <si>
-    <t>Loop: 2100A Segment: NM109 Notes: NM108 = "PI"</t>
-  </si>
-  <si>
-    <t>Loop: 2100A Segment: PER04 Notes: PER03 = "UR"</t>
-  </si>
-  <si>
-    <t>Loop: 2100C Segment: NM109 Notes: NM108 = id code qualifier</t>
-  </si>
-  <si>
-    <t>Loop: 2100B Segment: NM109 Notes: NM108 = id code qualifier</t>
-  </si>
-  <si>
-    <t>Loop: 2220D Notes: SVC01 = id code qualifier, SVC02 is the claim amount, SVC04 is REV Code, Does not list line item</t>
-  </si>
-  <si>
-    <t>Loop: 2220D Segments: STC01-02, STC10-02, STC11-02</t>
-  </si>
-  <si>
-    <t>Loop: 2100D Segments :NM103, NM104, NM105, NM107 Notes: NM102 = "1"</t>
+    <t>ClaimResponse.patient: Patient.birthDate</t>
+  </si>
+  <si>
+    <t>Questionnaire</t>
+  </si>
+  <si>
+    <t>“questionnaire” Task.input</t>
+  </si>
+  <si>
+    <t>QuestionnaireResponse</t>
+  </si>
+  <si>
+    <t>Attachment.Content</t>
+  </si>
+  <si>
+    <t>ClaimResponse.item.extension:itemTraceNumber  Note: CommunicationRequest.payload.extension:serviceLineNumber references this item</t>
+  </si>
+  <si>
+    <t>ClaimResponse = Bundle.entry[0].resource, PractitionerRole = Bundle.entry[n].resource referenced by ClaimResponse.requester</t>
+  </si>
+  <si>
+    <t>ClaimResponse = Bundle.entry[0].resource, Organization,PractitionerRole = Bundle.entry[n].resource referenced by ClaimResponse.requester</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ClaimResponse.identifier, ClaimResponse.item.commmunicationRequest: CommunicationRequest.identifier</t>
+  </si>
+  <si>
+    <t>ClaimResponse.requester: Organization.identifier, ClaimResponse.requester: PractitionerRole.organization: Organziation.identifier</t>
+  </si>
+  <si>
+    <t>ClaimResponse.requester: PractitionerRole.practitioner: Practitioner.identifier</t>
   </si>
   <si>
     <t>Loop: 2000E Segment: TRN02 Notes: TRN01 = "1", patient event tracking number. or Loop: 2000F Segment: TRN02 Notes: TRN01 = "1" or TRN01 = "2", service level tracking number</t>
   </si>
   <si>
-    <t>Loop: 2010A Segment: NM109 Notes: NM108 = "PI"</t>
-  </si>
-  <si>
-    <t>Loop: 2010A Segment: PER08 Notes: PER07 = "UR"</t>
-  </si>
-  <si>
-    <t>Loop: 2010EA Segment: NM109 Notes: NM101 = id code qualifier , NM102 = "1"</t>
-  </si>
-  <si>
-    <t>Loop: 2010B Segment: NM109 Notes: NM101 = id code qualifier, NM102 = "2"</t>
-  </si>
-  <si>
-    <t>Loop: 2000E (event level) or 2000F (line level) Segment: DTP03 Notes: DTP01="742" DTP02 = date format code</t>
-  </si>
-  <si>
-    <t>Loop: 2010C Segment: NM109 Notes: NM108 = id code qualifier</t>
-  </si>
-  <si>
-    <t>Loop: 2010C Segments: NM103, NM104 Notes: NM101 = id code qualifier</t>
-  </si>
-  <si>
-    <t>Loop: 2010C Segment: REF02 Notes: REF01 = "EJ"</t>
-  </si>
-  <si>
-    <t>Loop: 2010C Segment: DMG02 Notes: DMG01 = date format code</t>
-  </si>
-  <si>
-    <t>Loop: 2000A Segment: TRN02</t>
-  </si>
-  <si>
-    <t>Loop: 1000A Segment: NM109</t>
-  </si>
-  <si>
-    <t>Loop: 1000D Segment: Ref02 Notes: Ref01="X1", provider assigned</t>
-  </si>
-  <si>
-    <t>Loop: 2000A Segment: STC10 Notes: Used to convey status of the entire claim or a specific service line</t>
-  </si>
-  <si>
-    <t>Loop: 2000A Segment: STC01-01</t>
-  </si>
-  <si>
-    <t>Loop: 2100A Segment: DTP03</t>
-  </si>
-  <si>
-    <t>Loop: 1000D Segment: NM109 Notes: NM108="MI"</t>
-  </si>
-  <si>
-    <t>Loop: 1000C Segment: NM109 Notes: NM108="XX"</t>
-  </si>
-  <si>
-    <t>Loop: 1000B Segment: NM109 Notes: NM108="46"</t>
-  </si>
-  <si>
-    <t>Loop: 1000D Segments: NM103, NM104, NM105 Notes: NM102 = "1"</t>
-  </si>
-  <si>
-    <t>Loop: 2200D Segment: REF02 Notes: REF01="X1"</t>
-  </si>
-  <si>
-    <t>Loop: 2220D Segments: REF02 Notes: REF01= id code qualifier</t>
-  </si>
-  <si>
-    <t>Loop: 2000F Segment: TRN02 Notes: TRN01 ="1" or TRN01 ="2"</t>
-  </si>
-  <si>
-    <t>Loop: 2000F Segment: TRN02 Notes: TRN01 = "1"</t>
-  </si>
-  <si>
-    <t>Loop: 2000E Segment: HI?? or Loop: 2000F Segment: PWK?? Notes: Clarify!</t>
-  </si>
-  <si>
-    <t>Loop: 2200D Segment: TRN02 Notes: TRN01 = "1"</t>
-  </si>
-  <si>
-    <t>Loop: 2200D Segment: DTP03 Notes: DTP01 = "106", DTP02 = "D8"</t>
-  </si>
-  <si>
-    <t>Loop: 2200D Segment: DTP03 Notes: DTP01 = "172", DTP02 = "D8" or DTP02 = "RD8"</t>
-  </si>
-  <si>
-    <t>PractitionerRole.practitioner.identifier</t>
-  </si>
-  <si>
-    <t>PractitionerRole.organization.identifier</t>
-  </si>
-  <si>
-    <t>Questionnaire</t>
-  </si>
-  <si>
-    <t>QuestionnaireResponse</t>
-  </si>
-  <si>
-    <t>Attachment.Content</t>
-  </si>
-  <si>
-    <t>“questionnaire” Task.input</t>
+    <t>CR_element</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>element</t>
+  </si>
+  <si>
+    <t>ClaimResponse.identifier</t>
+  </si>
+  <si>
+    <t>ClaimResponse.insurer</t>
+  </si>
+  <si>
+    <t>Organization</t>
+  </si>
+  <si>
+    <t>ref</t>
+  </si>
+  <si>
+    <t>ClaimResponse.requester</t>
+  </si>
+  <si>
+    <t>identifier</t>
+  </si>
+  <si>
+    <t>PractitionerRole</t>
+  </si>
+  <si>
+    <t>practitioner.identifier</t>
+  </si>
+  <si>
+    <t>ClaimResponse.request</t>
+  </si>
+  <si>
+    <t>ClaimResponse.item.extension:itemTraceNumber</t>
+  </si>
+  <si>
+    <t>ClaimResponse.commmunicationRequest: CommunicationRequest.payload.extension:contentModifier</t>
+  </si>
+  <si>
+    <t>ClaimResponse.commmunicationRequest</t>
+  </si>
+  <si>
+    <t>CommunicationRequest</t>
+  </si>
+  <si>
+    <t>.payload.extension:contentModifier</t>
+  </si>
+  <si>
+    <t>ClaimResponse.patient</t>
+  </si>
+  <si>
+    <t>Patient</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>birthDate</t>
+  </si>
+  <si>
+    <t>CR_extension_url</t>
+  </si>
+  <si>
+    <t>element_extension_url</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-pas/StructureDefinition/extension-itemTraceNumber</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-pas/StructureDefinition/extension-itemRequestedServiceDate</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-pas/StructureDefinition/extension-contentModifier</t>
+  </si>
+  <si>
+    <t>For *unsolicited* attachments, this is the provider-assigned tracking/control number. For *solicited* attachments, this is the payer-assigned tracking/control number.</t>
+  </si>
+  <si>
+    <t>Payer-assigned tracking/control number</t>
+  </si>
+  <si>
+    <t>Provider-assigned claim/prior authorization ID</t>
+  </si>
+  <si>
+    <t>Patient Account Number is a provider-assigned identifier</t>
+  </si>
+  <si>
+    <t>Cdex_Task_Cardinality</t>
+  </si>
+  <si>
+    <t>Cdex_Task_Must Support</t>
+  </si>
+  <si>
+    <t>Cdex_Task_System_Constraints</t>
+  </si>
+  <si>
+    <t>1..*</t>
+  </si>
+  <si>
+    <t>fixed type to CDex code for "tracking-id"</t>
+  </si>
+  <si>
+    <t>1..1</t>
+  </si>
+  <si>
+    <t>limited to "claim" or "preuathorization" from http://hl7.org/fhir/claim-use</t>
+  </si>
+  <si>
+    <t>none!  - Should require  a unique payer identifier to be NAIC, TIN or something else?</t>
+  </si>
+  <si>
+    <t>payer url is pre-coordinated off-line</t>
+  </si>
+  <si>
+    <t>0..1</t>
+  </si>
+  <si>
+    <t>0..1  At least a practitioner.identifier or organization.identifier SHALL be present.</t>
+  </si>
+  <si>
+    <t>Only " (e.g., Type 1 NPI)" !</t>
+  </si>
+  <si>
+    <t>Only " (e.g., Type 2 NPI)" !</t>
+  </si>
+  <si>
+    <t>none!  - Should we require a type or assigner?</t>
+  </si>
+  <si>
+    <t>"http://hl7.org/fhir/us/davinci-pas/StructureDefinition/extension-serviceLineNumber"  ( data-type - positvie intger) !  should be "http://hl7.org/fhir/us/davinci-pas/StructureDefinition/extension-itemTraceNumber" (identifier?) or a just a string to represent the service-level tracking ID which could be an integer or an identifier?</t>
+  </si>
+  <si>
+    <t>0..1 If code = "attachment-request-code", must have one or more "code" inputs., Must only have "code" inputs or one "questionnaire" input not both.</t>
+  </si>
+  <si>
+    <t>LOINC</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>fixed type to "UMB" from http://hl7.org/fhir/us/davinci-hrex/CodeSystem/hrex-temp</t>
+  </si>
+  <si>
+    <t>fixed type to "pat" http://hl7.org/fhir/us/carin-bb/CodeSystem/C4BBIdentifierType</t>
+  </si>
+  <si>
+    <t>0..1 If code = "attachment-request-questionnaire", must have one "questionnaire" input., Must only have "code" inputs or one "questionnaire" input not both.</t>
+  </si>
+  <si>
+    <t>PAS_Bundle_Response_Cardinality</t>
+  </si>
+  <si>
+    <t>PAS_Bundle_Response_Constraints</t>
+  </si>
+  <si>
+    <t>PAS_Bundle_Response_MustSupport</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -530,12 +710,18 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF000000"/>
+      <color rgb="FF333333"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0000FF"/>
       <name val="Menlo"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -715,14 +901,8 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <start/>
       <end/>
@@ -837,21 +1017,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <start style="thin">
-        <color auto="1"/>
-      </start>
-      <end style="thin">
-        <color auto="1"/>
-      </end>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -897,22 +1062,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -971,88 +1125,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing" xmlns:a="http://purl.oclc.org/ooxml/drawingml/main">
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:v="urn:schemas-microsoft-com:vml" Requires="v"/>
-    <mc:Fallback>
-      <xdr:twoCellAnchor editAs="absolute">
-        <xdr:from>
-          <xdr:col>4</xdr:col>
-          <xdr:colOff>622300</xdr:colOff>
-          <xdr:row>13</xdr:row>
-          <xdr:rowOff>1041400</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>2425700</xdr:colOff>
-          <xdr:row>14</xdr:row>
-          <xdr:rowOff>190500</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1025" name="Comment 1" hidden="1">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1795BC95-5F80-BBD9-BB5B-F08A27DA9524}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1">
-              <a:spLocks noChangeArrowheads="1"/>
-            </xdr:cNvSpPr>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="7569200" y="13779500"/>
-              <a:ext cx="3263900" cy="228600"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:srgbClr xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="FFFFE1" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="80"/>
-            </a:solidFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:srgbClr val="510000"/>
-              </a:solidFill>
-              <a:miter lim="800%"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
-            <a:effectLst/>
-            <a:extLst>
-              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-                <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-                  <a:effectLst>
-                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                      <a:srgbClr val="510000"/>
-                    </a:outerShdw>
-                  </a:effectLst>
-                </a14:hiddenEffects>
-              </a:ext>
-              <a:ext uri="{53640926-AAD7-44D8-BBD7-CCE9431645EC}">
-                <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="1"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Fallback>
-  </mc:AlternateContent>
-</xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://purl.oclc.org/ooxml/spreadsheetml/main">
-  <person displayName="Eric Haas" id="{7A8DD75B-886D-EF4A-8EDA-90FC129037B5}" userId="deea5e002be8d274" providerId="Windows Live"/>
-</personList>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1340,536 +1414,1073 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://purl.oclc.org/ooxml/spreadsheetml/main">
-  <threadedComment ref="E10" dT="2022-12-11T00:00:33.87" personId="{7A8DD75B-886D-EF4A-8EDA-90FC129037B5}" id="{33F063C9-D438-2F4A-B60F-ED6425718629}">
-    <text>What was the ~ at the end. it was messing up my formatting.</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I18"/>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:W24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29" customWidth="1"/>
-    <col min="4" max="4" width="24.33203125" customWidth="1"/>
-    <col min="5" max="5" width="19.1640625" customWidth="1"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="94.1640625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="87.1640625" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="32.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="40.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="39.5" customWidth="1"/>
-    <col min="9" max="9" width="42.5" customWidth="1"/>
-    <col min="10" max="10" width="38.6640625" customWidth="1"/>
-    <col min="11" max="11" width="39" customWidth="1"/>
+    <col min="8" max="8" width="141" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="64.33203125" customWidth="1"/>
+    <col min="10" max="17" width="64.33203125" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="22" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="34.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>57</v>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>123</v>
+      </c>
+      <c r="K1" t="s">
+        <v>144</v>
+      </c>
+      <c r="L1" t="s">
+        <v>129</v>
+      </c>
+      <c r="M1" t="s">
+        <v>124</v>
+      </c>
+      <c r="N1" t="s">
+        <v>125</v>
+      </c>
+      <c r="O1" t="s">
+        <v>145</v>
+      </c>
+      <c r="P1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>10</v>
+      </c>
+      <c r="R1" t="s">
+        <v>153</v>
+      </c>
+      <c r="S1" t="s">
+        <v>154</v>
+      </c>
+      <c r="T1" t="s">
+        <v>155</v>
+      </c>
+      <c r="U1" t="s">
+        <v>174</v>
+      </c>
+      <c r="V1" t="s">
+        <v>176</v>
+      </c>
+      <c r="W1" t="s">
+        <v>175</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="187" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>80</v>
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="H2" t="s">
-        <v>8</v>
+        <v>149</v>
       </c>
       <c r="I2" t="s">
-        <v>9</v>
+        <v>150</v>
+      </c>
+      <c r="J2" t="s">
+        <v>126</v>
+      </c>
+      <c r="L2" t="b">
+        <v>0</v>
+      </c>
+      <c r="P2" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R2" t="s">
+        <v>156</v>
+      </c>
+      <c r="S2" t="b">
+        <v>1</v>
+      </c>
+      <c r="T2" t="s">
+        <v>157</v>
+      </c>
+      <c r="U2" t="s">
+        <v>156</v>
+      </c>
+      <c r="V2" t="b">
+        <v>1</v>
+      </c>
+      <c r="W2" t="s">
+        <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>58</v>
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="H3" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="I3" t="s">
-        <v>13</v>
+        <v>22</v>
+      </c>
+      <c r="P3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>24</v>
+      </c>
+      <c r="R3" t="s">
+        <v>158</v>
+      </c>
+      <c r="S3" t="b">
+        <v>1</v>
+      </c>
+      <c r="T3" t="s">
+        <v>159</v>
+      </c>
+      <c r="U3" t="s">
+        <v>158</v>
+      </c>
+      <c r="V3" t="b">
+        <v>1</v>
+      </c>
+      <c r="W3" t="s">
+        <v>159</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>81</v>
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
+        <v>28</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="G4" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="H4" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I4" t="s">
-        <v>14</v>
+        <v>25</v>
+      </c>
+      <c r="J4" t="s">
+        <v>127</v>
+      </c>
+      <c r="L4" t="b">
+        <v>1</v>
+      </c>
+      <c r="M4" t="s">
+        <v>128</v>
+      </c>
+      <c r="N4" t="s">
+        <v>131</v>
+      </c>
+      <c r="P4" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>40</v>
+      </c>
+      <c r="R4" t="s">
+        <v>158</v>
+      </c>
+      <c r="S4" t="b">
+        <v>1</v>
+      </c>
+      <c r="T4" t="s">
+        <v>160</v>
+      </c>
+      <c r="U4" t="s">
+        <v>158</v>
+      </c>
+      <c r="V4" t="b">
+        <v>1</v>
+      </c>
+      <c r="W4" t="s">
+        <v>160</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>18</v>
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" t="s">
+        <v>35</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="H5" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="I5" t="s">
-        <v>61</v>
+        <v>38</v>
+      </c>
+      <c r="P5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>31</v>
+      </c>
+      <c r="R5" t="s">
+        <v>158</v>
+      </c>
+      <c r="S5" t="b">
+        <v>1</v>
+      </c>
+      <c r="T5" t="s">
+        <v>161</v>
+      </c>
+      <c r="U5" t="s">
+        <v>158</v>
+      </c>
+      <c r="V5" t="b">
+        <v>1</v>
+      </c>
+      <c r="W5" t="s">
+        <v>161</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>88</v>
+        <v>41</v>
+      </c>
+      <c r="C6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" t="s">
+        <v>44</v>
       </c>
       <c r="F6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>98</v>
+        <v>45</v>
+      </c>
+      <c r="G6" t="s">
+        <v>46</v>
       </c>
       <c r="H6" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="I6" t="s">
-        <v>23</v>
+        <v>47</v>
+      </c>
+      <c r="J6" t="s">
+        <v>130</v>
+      </c>
+      <c r="L6" t="b">
+        <v>1</v>
+      </c>
+      <c r="M6" t="s">
+        <v>128</v>
+      </c>
+      <c r="N6" t="s">
+        <v>131</v>
+      </c>
+      <c r="P6" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>118</v>
+      </c>
+      <c r="R6" t="s">
+        <v>163</v>
+      </c>
+      <c r="S6" t="b">
+        <v>1</v>
+      </c>
+      <c r="T6" t="s">
+        <v>165</v>
+      </c>
+      <c r="U6" t="s">
+        <v>163</v>
+      </c>
+      <c r="V6" t="b">
+        <v>1</v>
+      </c>
+      <c r="W6" t="s">
+        <v>165</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>87</v>
+        <v>48</v>
+      </c>
+      <c r="C7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" t="s">
+        <v>51</v>
       </c>
       <c r="F7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>99</v>
+        <v>52</v>
+      </c>
+      <c r="G7" t="s">
+        <v>53</v>
       </c>
       <c r="H7" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="I7" t="s">
-        <v>26</v>
+        <v>54</v>
+      </c>
+      <c r="J7" t="s">
+        <v>130</v>
+      </c>
+      <c r="L7" t="b">
+        <v>1</v>
+      </c>
+      <c r="M7" t="s">
+        <v>132</v>
+      </c>
+      <c r="N7" t="s">
+        <v>133</v>
+      </c>
+      <c r="P7" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>117</v>
+      </c>
+      <c r="R7" t="s">
+        <v>163</v>
+      </c>
+      <c r="S7" t="b">
+        <v>1</v>
+      </c>
+      <c r="T7" t="s">
+        <v>164</v>
+      </c>
+      <c r="U7" t="s">
+        <v>163</v>
+      </c>
+      <c r="V7" t="b">
+        <v>1</v>
+      </c>
+      <c r="W7" t="s">
+        <v>164</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="102" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>82</v>
+        <v>55</v>
+      </c>
+      <c r="C8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" t="s">
+        <v>58</v>
       </c>
       <c r="F8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" t="s">
+        <v>59</v>
+      </c>
+      <c r="H8" t="s">
+        <v>151</v>
+      </c>
+      <c r="I8" t="s">
+        <v>151</v>
+      </c>
+      <c r="J8" t="s">
+        <v>134</v>
+      </c>
+      <c r="L8" t="b">
+        <v>1</v>
+      </c>
+      <c r="M8" t="s">
         <v>18</v>
       </c>
-      <c r="G8" t="s">
-        <v>28</v>
-      </c>
-      <c r="H8" t="s">
-        <v>29</v>
-      </c>
-      <c r="I8" t="s">
-        <v>29</v>
+      <c r="N8" t="s">
+        <v>131</v>
+      </c>
+      <c r="P8" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>61</v>
+      </c>
+      <c r="R8" t="s">
+        <v>158</v>
+      </c>
+      <c r="S8" t="b">
+        <v>1</v>
+      </c>
+      <c r="T8" t="s">
+        <v>166</v>
+      </c>
+      <c r="U8" t="s">
+        <v>158</v>
+      </c>
+      <c r="V8" t="b">
+        <v>1</v>
+      </c>
+      <c r="W8" t="s">
+        <v>166</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="136" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" t="s">
+        <v>66</v>
+      </c>
+      <c r="G9" t="s">
         <v>67</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="F9" t="s">
-        <v>31</v>
-      </c>
-      <c r="G9" t="s">
-        <v>32</v>
-      </c>
       <c r="H9" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="I9" t="s">
-        <v>60</v>
+        <v>68</v>
+      </c>
+      <c r="J9" t="s">
+        <v>135</v>
+      </c>
+      <c r="K9" t="s">
+        <v>146</v>
+      </c>
+      <c r="L9" t="b">
+        <v>0</v>
+      </c>
+      <c r="M9" t="s">
+        <v>138</v>
+      </c>
+      <c r="N9" t="s">
+        <v>139</v>
+      </c>
+      <c r="P9" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>69</v>
+      </c>
+      <c r="R9" t="s">
+        <v>162</v>
+      </c>
+      <c r="S9" t="b">
+        <v>1</v>
+      </c>
+      <c r="T9" t="s">
+        <v>167</v>
+      </c>
+      <c r="U9" t="s">
+        <v>162</v>
+      </c>
+      <c r="V9" t="b">
+        <v>1</v>
+      </c>
+      <c r="W9" t="s">
+        <v>167</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>84</v>
+        <v>70</v>
+      </c>
+      <c r="C10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" t="s">
+        <v>73</v>
       </c>
       <c r="F10" t="s">
-        <v>34</v>
+        <v>74</v>
       </c>
       <c r="G10" t="s">
-        <v>35</v>
+        <v>75</v>
       </c>
       <c r="H10" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
       <c r="I10" t="s">
-        <v>36</v>
+        <v>76</v>
+      </c>
+      <c r="J10" t="s">
+        <v>137</v>
+      </c>
+      <c r="K10" s="3"/>
+      <c r="L10" t="b">
+        <v>1</v>
+      </c>
+      <c r="M10" t="s">
+        <v>138</v>
+      </c>
+      <c r="N10" t="s">
+        <v>139</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="P10" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>69</v>
+      </c>
+      <c r="R10" t="s">
+        <v>168</v>
+      </c>
+      <c r="S10" t="b">
+        <v>1</v>
+      </c>
+      <c r="T10" t="s">
+        <v>169</v>
+      </c>
+      <c r="U10" t="s">
+        <v>168</v>
+      </c>
+      <c r="V10" t="b">
+        <v>1</v>
+      </c>
+      <c r="W10" t="s">
+        <v>169</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>18</v>
+        <v>77</v>
+      </c>
+      <c r="C11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" t="s">
+        <v>35</v>
       </c>
       <c r="F11" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="G11" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
       <c r="H11" t="s">
-        <v>39</v>
+        <v>80</v>
       </c>
       <c r="I11" t="s">
-        <v>39</v>
+        <v>80</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>81</v>
+      </c>
+      <c r="R11" t="s">
+        <v>162</v>
+      </c>
+      <c r="S11" t="b">
+        <v>1</v>
+      </c>
+      <c r="T11" t="s">
+        <v>170</v>
+      </c>
+      <c r="U11" t="s">
+        <v>162</v>
+      </c>
+      <c r="V11" t="b">
+        <v>1</v>
+      </c>
+      <c r="W11" t="s">
+        <v>170</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E12" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E12" t="s">
         <v>85</v>
       </c>
       <c r="F12" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
       <c r="G12" t="s">
-        <v>42</v>
+        <v>87</v>
       </c>
       <c r="H12" t="s">
-        <v>43</v>
+        <v>88</v>
       </c>
       <c r="I12" t="s">
-        <v>43</v>
+        <v>88</v>
+      </c>
+      <c r="J12" t="s">
+        <v>89</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="L12" t="b">
+        <v>0</v>
+      </c>
+      <c r="P12" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>69</v>
+      </c>
+      <c r="R12" t="s">
+        <v>162</v>
+      </c>
+      <c r="S12" t="b">
+        <v>1</v>
+      </c>
+      <c r="T12" t="s">
+        <v>170</v>
+      </c>
+      <c r="U12" t="s">
+        <v>162</v>
+      </c>
+      <c r="V12" t="b">
+        <v>1</v>
+      </c>
+      <c r="W12" t="s">
+        <v>170</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>86</v>
+        <v>90</v>
+      </c>
+      <c r="C13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E13" t="s">
+        <v>92</v>
       </c>
       <c r="F13" t="s">
-        <v>45</v>
+        <v>93</v>
       </c>
       <c r="G13" t="s">
-        <v>46</v>
+        <v>94</v>
       </c>
       <c r="H13" t="s">
-        <v>47</v>
+        <v>95</v>
       </c>
       <c r="I13" t="s">
-        <v>47</v>
+        <v>95</v>
+      </c>
+      <c r="J13" t="s">
+        <v>140</v>
+      </c>
+      <c r="L13" t="b">
+        <v>1</v>
+      </c>
+      <c r="M13" t="s">
+        <v>141</v>
+      </c>
+      <c r="N13" t="s">
+        <v>131</v>
+      </c>
+      <c r="P13" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>97</v>
+      </c>
+      <c r="R13" t="s">
+        <v>156</v>
+      </c>
+      <c r="S13" t="b">
+        <v>1</v>
+      </c>
+      <c r="T13" t="s">
+        <v>171</v>
+      </c>
+      <c r="U13" t="s">
+        <v>156</v>
+      </c>
+      <c r="V13" t="b">
+        <v>1</v>
+      </c>
+      <c r="W13" t="s">
+        <v>171</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>89</v>
+        <v>98</v>
+      </c>
+      <c r="C14" t="s">
+        <v>99</v>
+      </c>
+      <c r="D14" t="s">
+        <v>100</v>
+      </c>
+      <c r="E14" t="s">
+        <v>101</v>
       </c>
       <c r="F14" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="G14" t="s">
-        <v>49</v>
+        <v>102</v>
       </c>
       <c r="H14" t="s">
-        <v>50</v>
+        <v>103</v>
       </c>
       <c r="I14" t="s">
-        <v>50</v>
+        <v>103</v>
+      </c>
+      <c r="J14" t="s">
+        <v>140</v>
+      </c>
+      <c r="L14" t="b">
+        <v>1</v>
+      </c>
+      <c r="M14" t="s">
+        <v>141</v>
+      </c>
+      <c r="N14" t="s">
+        <v>142</v>
+      </c>
+      <c r="P14" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>97</v>
+      </c>
+      <c r="R14" t="s">
+        <v>158</v>
+      </c>
+      <c r="S14" t="b">
+        <v>1</v>
+      </c>
+      <c r="T14" t="s">
+        <v>170</v>
+      </c>
+      <c r="U14" t="s">
+        <v>158</v>
+      </c>
+      <c r="V14" t="b">
+        <v>1</v>
+      </c>
+      <c r="W14" t="s">
+        <v>170</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>78</v>
+        <v>105</v>
+      </c>
+      <c r="C15" t="s">
+        <v>106</v>
+      </c>
+      <c r="D15" t="s">
+        <v>107</v>
       </c>
       <c r="E15" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="F15" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="G15" t="s">
-        <v>46</v>
+        <v>94</v>
       </c>
       <c r="H15" t="s">
-        <v>52</v>
+        <v>152</v>
       </c>
       <c r="I15" t="s">
-        <v>52</v>
+        <v>152</v>
+      </c>
+      <c r="P15" t="s">
+        <v>81</v>
+      </c>
+      <c r="R15" t="s">
+        <v>156</v>
+      </c>
+      <c r="S15" t="b">
+        <v>1</v>
+      </c>
+      <c r="T15" t="s">
+        <v>172</v>
+      </c>
+      <c r="U15" t="s">
+        <v>156</v>
+      </c>
+      <c r="V15" t="b">
+        <v>1</v>
+      </c>
+      <c r="W15" t="s">
+        <v>172</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>18</v>
+        <v>108</v>
+      </c>
+      <c r="C16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" t="s">
+        <v>109</v>
+      </c>
+      <c r="E16" t="s">
+        <v>35</v>
       </c>
       <c r="F16" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="G16" t="s">
-        <v>54</v>
+        <v>110</v>
       </c>
       <c r="H16" t="s">
-        <v>50</v>
+        <v>103</v>
       </c>
       <c r="I16" t="s">
-        <v>50</v>
+        <v>103</v>
+      </c>
+      <c r="J16" t="s">
+        <v>140</v>
+      </c>
+      <c r="L16" t="b">
+        <v>1</v>
+      </c>
+      <c r="M16" t="s">
+        <v>141</v>
+      </c>
+      <c r="N16" t="s">
+        <v>143</v>
+      </c>
+      <c r="P16" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>97</v>
+      </c>
+      <c r="R16" t="s">
+        <v>158</v>
+      </c>
+      <c r="S16" t="b">
+        <v>1</v>
+      </c>
+      <c r="T16" t="s">
+        <v>170</v>
+      </c>
+      <c r="U16" t="s">
+        <v>158</v>
+      </c>
+      <c r="V16" t="b">
+        <v>1</v>
+      </c>
+      <c r="W16" t="s">
+        <v>170</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="G17" t="s">
-        <v>103</v>
+        <v>113</v>
+      </c>
+      <c r="R17" t="s">
+        <v>173</v>
+      </c>
+      <c r="S17" t="b">
+        <v>1</v>
+      </c>
+      <c r="T17" t="s">
+        <v>170</v>
+      </c>
+      <c r="U17" t="s">
+        <v>173</v>
+      </c>
+      <c r="V17" t="b">
+        <v>1</v>
+      </c>
+      <c r="W17" t="s">
+        <v>170</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="F18" t="s">
-        <v>102</v>
-      </c>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="D24" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing r:id="rId1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="v">
-      <legacyDrawing r:id="rId2"/>
-    </mc:Choice>
-  </mc:AlternateContent>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Pre-Applied (Enhancement) Change the LineNumber Extension [FHIR-44875] Pre-Applied (Clarification) Fix X12 277RFAI-v6020 mapping for Line Items [FHIR-45298]
</commit_message>
<xml_diff>
--- a/input/images/data-element-mapping.xlsx
+++ b/input/images/data-element-mapping.xlsx
@@ -1,42 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
-  <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/davinci-ecdx/input/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{88719C09-83BD-3046-AE70-EF981373A8B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{182B0C55-2482-2441-B491-48D57195849E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34140" yWindow="500" windowWidth="34120" windowHeight="28300"/>
   </bookViews>
   <sheets>
     <sheet name="data-element-mapping" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="271" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="128">
   <si>
     <t>No</t>
   </si>
@@ -86,6 +70,9 @@
     <t>Task.identifier</t>
   </si>
   <si>
+    <t xml:space="preserve"> ClaimResponse.identifier, ClaimResponse.item.commmunicationRequest: CommunicationRequest.identifier</t>
+  </si>
+  <si>
     <t>ClaimResponse = Bundle.entry[0].resource, CommunicationRequest = Bundle.entry[n].resource referenced by ClaimResponse.communincationRequest</t>
   </si>
   <si>
@@ -131,36 +118,33 @@
     <t>Task.requester.identifier</t>
   </si>
   <si>
+    <t>ClaimResponse.insurer: Organization.identifier</t>
+  </si>
+  <si>
+    <t>ClaimResponse = Bundle.entry[0].resource, Organization = Bundle.entry[n].resource referenced by ClaimResponse.insurer</t>
+  </si>
+  <si>
+    <t>Payer URL</t>
+  </si>
+  <si>
+    <t>Loop: 2100A Segment: PER04 Notes: PER03 = "UR"</t>
+  </si>
+  <si>
+    <t>Loop: 2010A Segment: PER08 Notes: PER07 = "UR"</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>(operation endpoint)</t>
+  </si>
+  <si>
+    <t>Payer endpoint where the attachments are submitted using the $submit-attachment operation</t>
+  </si>
+  <si>
     <t>out of band</t>
   </si>
   <si>
-    <t>Payer URL</t>
-  </si>
-  <si>
-    <t>Loop: 2100A Segment: PER04 Notes: PER03 = "UR"</t>
-  </si>
-  <si>
-    <t>Loop: 2010A Segment: PER08 Notes: PER07 = "UR"</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>(operation endpoint)</t>
-  </si>
-  <si>
-    <t>"payer-url" Task.input</t>
-  </si>
-  <si>
-    <t>Payer endpoint where the attachments are submitted using the $submit-attachment operation</t>
-  </si>
-  <si>
-    <t>ClaimResponse.insurer: Organization.identifier</t>
-  </si>
-  <si>
-    <t>ClaimResponse = Bundle.entry[0].resource, Organization = Bundle.entry[n].resource referenced by ClaimResponse.insurer</t>
-  </si>
-  <si>
     <t>Organization ID</t>
   </si>
   <si>
@@ -182,6 +166,12 @@
     <t>Organization of provider who submitted claim/prior authorization</t>
   </si>
   <si>
+    <t>ClaimResponse.requester: Organization.identifier, ClaimResponse.requester: PractitionerRole.organization: Organziation.identifier</t>
+  </si>
+  <si>
+    <t>ClaimResponse = Bundle.entry[0].resource, Organization,PractitionerRole = Bundle.entry[n].resource referenced by ClaimResponse.requester</t>
+  </si>
+  <si>
     <t>Provider ID</t>
   </si>
   <si>
@@ -203,6 +193,12 @@
     <t>Provider who submitted claim/prior authorization</t>
   </si>
   <si>
+    <t>ClaimResponse.requester: PractitionerRole.practitioner: Practitioner.identifier</t>
+  </si>
+  <si>
+    <t>ClaimResponse = Bundle.entry[0].resource, PractitionerRole = Bundle.entry[n].resource referenced by ClaimResponse.requester</t>
+  </si>
+  <si>
     <t>Claim/PreAuth ID</t>
   </si>
   <si>
@@ -227,24 +223,18 @@
     <t>Line Item(s)</t>
   </si>
   <si>
-    <t>Loop: 2220D Notes: SVC01 = id code qualifier, SVC02 is the claim amount, SVC04 is REV Code, Does not list line item</t>
-  </si>
-  <si>
-    <t>Loop: 2000F Segment: TRN02 Notes: TRN01 = "1"</t>
-  </si>
-  <si>
     <t>Loop: 2000A Segment: STC10 Notes: Used to convey status of the entire claim or a specific service line</t>
   </si>
   <si>
     <t>Attachment.LineItem</t>
   </si>
   <si>
-    <t>“code” Task.input.extension</t>
-  </si>
-  <si>
     <t>Claim/prior authorization line item numbers</t>
   </si>
   <si>
+    <t>ClaimResponse.item.extension:itemTraceNumber  Note: CommunicationRequest.payload.extension:serviceLineNumber references this item</t>
+  </si>
+  <si>
     <t>ClaimResponse = Bundle.entry[0].resource</t>
   </si>
   <si>
@@ -254,21 +244,18 @@
     <t>Loop: 2220D Segments: STC01-02, STC10-02, STC11-02</t>
   </si>
   <si>
-    <t>Loop: 2000E Segment: HI?? or Loop: 2000F Segment: PWK?? Notes: Clarify!</t>
-  </si>
-  <si>
     <t>Loop: 2000A Segment: STC01-01</t>
   </si>
   <si>
     <t>Attachment.Code</t>
   </si>
   <si>
-    <t>“code” Task.input </t>
-  </si>
-  <si>
     <t>LOINC attachment codes</t>
   </si>
   <si>
+    <t>ClaimResponse.item.commmunicationRequest: CommunicationRequest.payload.extension:contentModifier</t>
+  </si>
+  <si>
     <t>Due Date</t>
   </si>
   <si>
@@ -377,114 +364,12 @@
     <t>Questionnaire</t>
   </si>
   <si>
-    <t>“questionnaire” Task.input</t>
-  </si>
-  <si>
     <t>QuestionnaireResponse</t>
   </si>
   <si>
     <t>Attachment.Content</t>
   </si>
   <si>
-    <t>ClaimResponse.item.extension:itemTraceNumber  Note: CommunicationRequest.payload.extension:serviceLineNumber references this item</t>
-  </si>
-  <si>
-    <t>ClaimResponse = Bundle.entry[0].resource, PractitionerRole = Bundle.entry[n].resource referenced by ClaimResponse.requester</t>
-  </si>
-  <si>
-    <t>ClaimResponse = Bundle.entry[0].resource, Organization,PractitionerRole = Bundle.entry[n].resource referenced by ClaimResponse.requester</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ClaimResponse.identifier, ClaimResponse.item.commmunicationRequest: CommunicationRequest.identifier</t>
-  </si>
-  <si>
-    <t>ClaimResponse.requester: Organization.identifier, ClaimResponse.requester: PractitionerRole.organization: Organziation.identifier</t>
-  </si>
-  <si>
-    <t>ClaimResponse.requester: PractitionerRole.practitioner: Practitioner.identifier</t>
-  </si>
-  <si>
-    <t>Loop: 2000E Segment: TRN02 Notes: TRN01 = "1", patient event tracking number. or Loop: 2000F Segment: TRN02 Notes: TRN01 = "1" or TRN01 = "2", service level tracking number</t>
-  </si>
-  <si>
-    <t>CR_element</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>element</t>
-  </si>
-  <si>
-    <t>ClaimResponse.identifier</t>
-  </si>
-  <si>
-    <t>ClaimResponse.insurer</t>
-  </si>
-  <si>
-    <t>Organization</t>
-  </si>
-  <si>
-    <t>ref</t>
-  </si>
-  <si>
-    <t>ClaimResponse.requester</t>
-  </si>
-  <si>
-    <t>identifier</t>
-  </si>
-  <si>
-    <t>PractitionerRole</t>
-  </si>
-  <si>
-    <t>practitioner.identifier</t>
-  </si>
-  <si>
-    <t>ClaimResponse.request</t>
-  </si>
-  <si>
-    <t>ClaimResponse.item.extension:itemTraceNumber</t>
-  </si>
-  <si>
-    <t>ClaimResponse.commmunicationRequest: CommunicationRequest.payload.extension:contentModifier</t>
-  </si>
-  <si>
-    <t>ClaimResponse.commmunicationRequest</t>
-  </si>
-  <si>
-    <t>CommunicationRequest</t>
-  </si>
-  <si>
-    <t>.payload.extension:contentModifier</t>
-  </si>
-  <si>
-    <t>ClaimResponse.patient</t>
-  </si>
-  <si>
-    <t>Patient</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>birthDate</t>
-  </si>
-  <si>
-    <t>CR_extension_url</t>
-  </si>
-  <si>
-    <t>element_extension_url</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-pas/StructureDefinition/extension-itemTraceNumber</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-pas/StructureDefinition/extension-itemRequestedServiceDate</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-pas/StructureDefinition/extension-contentModifier</t>
-  </si>
-  <si>
     <t>For *unsolicited* attachments, this is the provider-assigned tracking/control number. For *solicited* attachments, this is the payer-assigned tracking/control number.</t>
   </si>
   <si>
@@ -497,101 +382,53 @@
     <t>Patient Account Number is a provider-assigned identifier</t>
   </si>
   <si>
-    <t>Cdex_Task_Cardinality</t>
-  </si>
-  <si>
-    <t>Cdex_Task_Must Support</t>
-  </si>
-  <si>
-    <t>Cdex_Task_System_Constraints</t>
-  </si>
-  <si>
-    <t>1..*</t>
-  </si>
-  <si>
-    <t>fixed type to CDex code for "tracking-id"</t>
-  </si>
-  <si>
-    <t>1..1</t>
-  </si>
-  <si>
-    <t>limited to "claim" or "preuathorization" from http://hl7.org/fhir/claim-use</t>
-  </si>
-  <si>
-    <t>none!  - Should require  a unique payer identifier to be NAIC, TIN or something else?</t>
-  </si>
-  <si>
-    <t>payer url is pre-coordinated off-line</t>
-  </si>
-  <si>
-    <t>0..1</t>
-  </si>
-  <si>
-    <t>0..1  At least a practitioner.identifier or organization.identifier SHALL be present.</t>
-  </si>
-  <si>
-    <t>Only " (e.g., Type 1 NPI)" !</t>
-  </si>
-  <si>
-    <t>Only " (e.g., Type 2 NPI)" !</t>
-  </si>
-  <si>
-    <t>none!  - Should we require a type or assigner?</t>
-  </si>
-  <si>
-    <t>"http://hl7.org/fhir/us/davinci-pas/StructureDefinition/extension-serviceLineNumber"  ( data-type - positvie intger) !  should be "http://hl7.org/fhir/us/davinci-pas/StructureDefinition/extension-itemTraceNumber" (identifier?) or a just a string to represent the service-level tracking ID which could be an integer or an identifier?</t>
-  </si>
-  <si>
-    <t>0..1 If code = "attachment-request-code", must have one or more "code" inputs., Must only have "code" inputs or one "questionnaire" input not both.</t>
-  </si>
-  <si>
-    <t>LOINC</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>fixed type to "UMB" from http://hl7.org/fhir/us/davinci-hrex/CodeSystem/hrex-temp</t>
-  </si>
-  <si>
-    <t>fixed type to "pat" http://hl7.org/fhir/us/carin-bb/CodeSystem/C4BBIdentifierType</t>
-  </si>
-  <si>
-    <t>0..1 If code = "attachment-request-questionnaire", must have one "questionnaire" input., Must only have "code" inputs or one "questionnaire" input not both.</t>
-  </si>
-  <si>
-    <t>PAS_Bundle_Response_Cardinality</t>
-  </si>
-  <si>
-    <t>PAS_Bundle_Response_Constraints</t>
-  </si>
-  <si>
-    <t>PAS_Bundle_Response_MustSupport</t>
+    <t>&lt;span class="bg-success" markdown="1"&gt;Note that this is an indirect mapping:  Loop 2220D (Service Line Information) Segment SVC01 or SVC04 codes reference the claim service item, which contains the line item.&lt;/span&gt;&lt;!-- new-content --&gt;</t>
+  </si>
+  <si>
+    <t>&lt;span class="bg-success" markdown="1"&gt;Loop: 2000E - Patient Event Level or Loop: 2000F Service Level Segment: TRN02 Notes: TRN01 = “1”: Payer Supplied TRN01 = “2” : Provider Supplied (echoed back)&lt;/span&gt;&lt;!-- new-content --&gt;</t>
+  </si>
+  <si>
+    <t>&lt;span class="bg-success" markdown="1"&gt;Loop: 2000F Segment: HL01&lt;!-- new-content --&gt;</t>
+  </si>
+  <si>
+    <t>&lt;span class="bg-success" markdown="1"&gt;Loop: 2000E - Patient Event Level or Loop: 2000F Service Level Segment: HI (LOINC) or Segment: PWK01 Report Type Codes &lt;!-- new-content --&gt;</t>
+  </si>
+  <si>
+    <t>"PayerUrl" Task.input</t>
+  </si>
+  <si>
+    <t>“attachmentsNeeded” Task.input.extension</t>
+  </si>
+  <si>
+    <t>“attachmentsNeeded” Task.input </t>
+  </si>
+  <si>
+    <t>“questionnaireNeeded” Task.input</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Calibri Light"/>
+      <name val="Aptos Display"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -599,7 +436,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -607,7 +444,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -615,35 +452,35 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -651,7 +488,7 @@
       <b/>
       <sz val="12"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -659,14 +496,14 @@
       <b/>
       <sz val="12"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -674,14 +511,14 @@
       <b/>
       <sz val="12"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -689,7 +526,7 @@
       <i/>
       <sz val="12"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -697,29 +534,17 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF333333"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF0000FF"/>
-      <name val="Menlo"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -904,15 +729,15 @@
   </fills>
   <borders count="10">
     <border>
-      <start/>
-      <end/>
+      <left/>
+      <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <start/>
-      <end/>
+      <left/>
+      <right/>
       <top/>
       <bottom style="thick">
         <color theme="4"/>
@@ -920,8 +745,8 @@
       <diagonal/>
     </border>
     <border>
-      <start/>
-      <end/>
+      <left/>
+      <right/>
       <top/>
       <bottom style="thick">
         <color theme="4" tint="0.499984740745262"/>
@@ -929,8 +754,8 @@
       <diagonal/>
     </border>
     <border>
-      <start/>
-      <end/>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.39997558519241921"/>
@@ -938,12 +763,12 @@
       <diagonal/>
     </border>
     <border>
-      <start style="thin">
+      <left style="thin">
         <color rgb="FF7F7F7F"/>
-      </start>
-      <end style="thin">
+      </left>
+      <right style="thin">
         <color rgb="FF7F7F7F"/>
-      </end>
+      </right>
       <top style="thin">
         <color rgb="FF7F7F7F"/>
       </top>
@@ -953,12 +778,12 @@
       <diagonal/>
     </border>
     <border>
-      <start style="thin">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
-      </start>
-      <end style="thin">
+      </left>
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
-      </end>
+      </right>
       <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
@@ -968,8 +793,8 @@
       <diagonal/>
     </border>
     <border>
-      <start/>
-      <end/>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -977,12 +802,12 @@
       <diagonal/>
     </border>
     <border>
-      <start style="double">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
-      </start>
-      <end style="double">
+      </left>
+      <right style="double">
         <color rgb="FF3F3F3F"/>
-      </end>
+      </right>
       <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
@@ -992,12 +817,12 @@
       <diagonal/>
     </border>
     <border>
-      <start style="thin">
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
-      </start>
-      <end style="thin">
+      </left>
+      <right style="thin">
         <color rgb="FFB2B2B2"/>
-      </end>
+      </right>
       <top style="thin">
         <color rgb="FFB2B2B2"/>
       </top>
@@ -1007,8 +832,8 @@
       <diagonal/>
     </border>
     <border>
-      <start/>
-      <end/>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -1062,11 +887,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1126,7 +948,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1136,39 +958,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="E97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="196B24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1220,7 +1042,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1279,25 +1101,25 @@
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0%">
+            <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110%"/>
-                <a:satMod val="105%"/>
-                <a:tint val="67%"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50%">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105%"/>
-                <a:satMod val="103%"/>
-                <a:tint val="73%"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100%">
+            <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105%"/>
-                <a:satMod val="109%"/>
-                <a:tint val="81%"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -1305,25 +1127,25 @@
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0%">
+            <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103%"/>
-                <a:lumMod val="102%"/>
-                <a:tint val="94%"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50%">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110%"/>
-                <a:lumMod val="100%"/>
-                <a:shade val="100%"/>
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100%">
+            <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99%"/>
-                <a:satMod val="120%"/>
-                <a:shade val="78%"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -1331,26 +1153,26 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800%"/>
-        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800%"/>
+          <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800%"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
@@ -1364,7 +1186,7 @@
           <a:effectLst>
             <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63%"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -1376,32 +1198,32 @@
         </a:solidFill>
         <a:solidFill>
           <a:schemeClr val="phClr">
-            <a:tint val="95%"/>
-            <a:satMod val="170%"/>
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0%">
+            <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93%"/>
-                <a:satMod val="150%"/>
-                <a:shade val="98%"/>
-                <a:lumMod val="102%"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50%">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="98%"/>
-                <a:satMod val="130%"/>
-                <a:shade val="90%"/>
-                <a:lumMod val="103%"/>
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100%">
+            <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63%"/>
-                <a:satMod val="120%"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -1410,44 +1232,53 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="94.1640625" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="87.1640625" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="40.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="141" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="64.33203125" customWidth="1"/>
-    <col min="10" max="17" width="64.33203125" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="34.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="22" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="96" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="5" max="5" width="31.83203125" customWidth="1"/>
+    <col min="7" max="7" width="39.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1476,49 +1307,13 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>123</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>144</v>
-      </c>
-      <c r="L1" t="s">
-        <v>129</v>
-      </c>
-      <c r="M1" t="s">
-        <v>124</v>
-      </c>
-      <c r="N1" t="s">
-        <v>125</v>
-      </c>
-      <c r="O1" t="s">
-        <v>145</v>
-      </c>
-      <c r="P1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q1" t="s">
         <v>10</v>
       </c>
-      <c r="R1" t="s">
-        <v>153</v>
-      </c>
-      <c r="S1" t="s">
-        <v>154</v>
-      </c>
-      <c r="T1" t="s">
-        <v>155</v>
-      </c>
-      <c r="U1" t="s">
-        <v>174</v>
-      </c>
-      <c r="V1" t="s">
-        <v>176</v>
-      </c>
-      <c r="W1" t="s">
-        <v>175</v>
-      </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1528,8 +1323,8 @@
       <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>122</v>
+      <c r="D2" t="s">
+        <v>121</v>
       </c>
       <c r="E2" t="s">
         <v>13</v>
@@ -1541,214 +1336,124 @@
         <v>15</v>
       </c>
       <c r="H2" t="s">
-        <v>149</v>
+        <v>116</v>
       </c>
       <c r="I2" t="s">
-        <v>150</v>
+        <v>117</v>
       </c>
       <c r="J2" t="s">
-        <v>126</v>
-      </c>
-      <c r="L2" t="b">
-        <v>0</v>
-      </c>
-      <c r="P2" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q2" t="s">
         <v>16</v>
       </c>
-      <c r="R2" t="s">
-        <v>156</v>
-      </c>
-      <c r="S2" t="b">
-        <v>1</v>
-      </c>
-      <c r="T2" t="s">
-        <v>157</v>
-      </c>
-      <c r="U2" t="s">
-        <v>156</v>
-      </c>
-      <c r="V2" t="b">
-        <v>1</v>
-      </c>
-      <c r="W2" t="s">
-        <v>157</v>
+      <c r="K2" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
         <v>19</v>
       </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P3" t="s">
         <v>23</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="J3" t="s">
         <v>24</v>
       </c>
-      <c r="R3" t="s">
-        <v>158</v>
-      </c>
-      <c r="S3" t="b">
-        <v>1</v>
-      </c>
-      <c r="T3" t="s">
-        <v>159</v>
-      </c>
-      <c r="U3" t="s">
-        <v>158</v>
-      </c>
-      <c r="V3" t="b">
-        <v>1</v>
-      </c>
-      <c r="W3" t="s">
-        <v>159</v>
+      <c r="K3" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" t="s">
         <v>26</v>
       </c>
-      <c r="D4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" t="s">
-        <v>25</v>
-      </c>
       <c r="I4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J4" t="s">
-        <v>127</v>
-      </c>
-      <c r="L4" t="b">
-        <v>1</v>
-      </c>
-      <c r="M4" t="s">
-        <v>128</v>
-      </c>
-      <c r="N4" t="s">
-        <v>131</v>
-      </c>
-      <c r="P4" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>40</v>
-      </c>
-      <c r="R4" t="s">
-        <v>158</v>
-      </c>
-      <c r="S4" t="b">
-        <v>1</v>
-      </c>
-      <c r="T4" t="s">
-        <v>160</v>
-      </c>
-      <c r="U4" t="s">
-        <v>158</v>
-      </c>
-      <c r="V4" t="b">
-        <v>1</v>
-      </c>
-      <c r="W4" t="s">
-        <v>160</v>
+        <v>32</v>
+      </c>
+      <c r="K4" t="s">
+        <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G5" t="s">
-        <v>37</v>
+        <v>124</v>
       </c>
       <c r="H5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I5" t="s">
-        <v>38</v>
-      </c>
-      <c r="P5" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>31</v>
-      </c>
-      <c r="R5" t="s">
-        <v>158</v>
-      </c>
-      <c r="S5" t="b">
-        <v>1</v>
-      </c>
-      <c r="T5" t="s">
-        <v>161</v>
-      </c>
-      <c r="U5" t="s">
-        <v>158</v>
-      </c>
-      <c r="V5" t="b">
-        <v>1</v>
-      </c>
-      <c r="W5" t="s">
-        <v>161</v>
+        <v>39</v>
+      </c>
+      <c r="J5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" t="s">
+        <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1777,261 +1482,138 @@
         <v>47</v>
       </c>
       <c r="J6" t="s">
-        <v>130</v>
-      </c>
-      <c r="L6" t="b">
-        <v>1</v>
-      </c>
-      <c r="M6" t="s">
-        <v>128</v>
-      </c>
-      <c r="N6" t="s">
-        <v>131</v>
-      </c>
-      <c r="P6" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>118</v>
-      </c>
-      <c r="R6" t="s">
-        <v>163</v>
-      </c>
-      <c r="S6" t="b">
-        <v>1</v>
-      </c>
-      <c r="T6" t="s">
-        <v>165</v>
-      </c>
-      <c r="U6" t="s">
-        <v>163</v>
-      </c>
-      <c r="V6" t="b">
-        <v>1</v>
-      </c>
-      <c r="W6" t="s">
-        <v>165</v>
+        <v>48</v>
+      </c>
+      <c r="K6" t="s">
+        <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E7" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H7" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="I7" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="J7" t="s">
-        <v>130</v>
-      </c>
-      <c r="L7" t="b">
-        <v>1</v>
-      </c>
-      <c r="M7" t="s">
-        <v>132</v>
-      </c>
-      <c r="N7" t="s">
-        <v>133</v>
-      </c>
-      <c r="P7" t="s">
-        <v>121</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>117</v>
-      </c>
-      <c r="R7" t="s">
-        <v>163</v>
-      </c>
-      <c r="S7" t="b">
-        <v>1</v>
-      </c>
-      <c r="T7" t="s">
-        <v>164</v>
-      </c>
-      <c r="U7" t="s">
-        <v>163</v>
-      </c>
-      <c r="V7" t="b">
-        <v>1</v>
-      </c>
-      <c r="W7" t="s">
-        <v>164</v>
+        <v>57</v>
+      </c>
+      <c r="K7" t="s">
+        <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C8" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D8" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E8" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="F8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G8" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="H8" t="s">
-        <v>151</v>
+        <v>118</v>
       </c>
       <c r="I8" t="s">
-        <v>151</v>
+        <v>118</v>
       </c>
       <c r="J8" t="s">
-        <v>134</v>
-      </c>
-      <c r="L8" t="b">
-        <v>1</v>
-      </c>
-      <c r="M8" t="s">
-        <v>18</v>
-      </c>
-      <c r="N8" t="s">
-        <v>131</v>
-      </c>
-      <c r="P8" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>61</v>
-      </c>
-      <c r="R8" t="s">
-        <v>158</v>
-      </c>
-      <c r="S8" t="b">
-        <v>1</v>
-      </c>
-      <c r="T8" t="s">
-        <v>166</v>
-      </c>
-      <c r="U8" t="s">
-        <v>158</v>
-      </c>
-      <c r="V8" t="b">
-        <v>1</v>
-      </c>
-      <c r="W8" t="s">
-        <v>166</v>
+        <v>64</v>
+      </c>
+      <c r="K8" t="s">
+        <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>63</v>
+        <v>120</v>
       </c>
       <c r="D9" t="s">
-        <v>64</v>
+        <v>122</v>
       </c>
       <c r="E9" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F9" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G9" t="s">
-        <v>67</v>
+        <v>125</v>
       </c>
       <c r="H9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J9" t="s">
-        <v>135</v>
+        <v>70</v>
       </c>
       <c r="K9" t="s">
-        <v>146</v>
-      </c>
-      <c r="L9" t="b">
-        <v>0</v>
-      </c>
-      <c r="M9" t="s">
-        <v>138</v>
-      </c>
-      <c r="N9" t="s">
-        <v>139</v>
-      </c>
-      <c r="P9" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>69</v>
-      </c>
-      <c r="R9" t="s">
-        <v>162</v>
-      </c>
-      <c r="S9" t="b">
-        <v>1</v>
-      </c>
-      <c r="T9" t="s">
-        <v>167</v>
-      </c>
-      <c r="U9" t="s">
-        <v>162</v>
-      </c>
-      <c r="V9" t="b">
-        <v>1</v>
-      </c>
-      <c r="W9" t="s">
-        <v>167</v>
+        <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C10" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D10" t="s">
-        <v>72</v>
+        <v>123</v>
       </c>
       <c r="E10" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F10" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G10" t="s">
-        <v>75</v>
+        <v>126</v>
       </c>
       <c r="H10" t="s">
         <v>76</v>
@@ -2040,433 +1622,228 @@
         <v>76</v>
       </c>
       <c r="J10" t="s">
-        <v>137</v>
-      </c>
-      <c r="K10" s="3"/>
-      <c r="L10" t="b">
-        <v>1</v>
-      </c>
-      <c r="M10" t="s">
-        <v>138</v>
-      </c>
-      <c r="N10" t="s">
-        <v>139</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="P10" t="s">
-        <v>136</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>69</v>
-      </c>
-      <c r="R10" t="s">
-        <v>168</v>
-      </c>
-      <c r="S10" t="b">
-        <v>1</v>
-      </c>
-      <c r="T10" t="s">
-        <v>169</v>
-      </c>
-      <c r="U10" t="s">
-        <v>168</v>
-      </c>
-      <c r="V10" t="b">
-        <v>1</v>
-      </c>
-      <c r="W10" t="s">
-        <v>169</v>
+        <v>77</v>
+      </c>
+      <c r="K10" t="s">
+        <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C11" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F11" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G11" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I11" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q11" t="s">
         <v>81</v>
       </c>
-      <c r="R11" t="s">
-        <v>162</v>
-      </c>
-      <c r="S11" t="b">
-        <v>1</v>
-      </c>
-      <c r="T11" t="s">
-        <v>170</v>
-      </c>
-      <c r="U11" t="s">
-        <v>162</v>
-      </c>
-      <c r="V11" t="b">
-        <v>1</v>
-      </c>
-      <c r="W11" t="s">
-        <v>170</v>
+      <c r="J11" t="s">
+        <v>82</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C12" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D12" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E12" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F12" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G12" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H12" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I12" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="J12" t="s">
-        <v>89</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="L12" t="b">
-        <v>0</v>
-      </c>
-      <c r="P12" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>69</v>
-      </c>
-      <c r="R12" t="s">
-        <v>162</v>
-      </c>
-      <c r="S12" t="b">
-        <v>1</v>
-      </c>
-      <c r="T12" t="s">
-        <v>170</v>
-      </c>
-      <c r="U12" t="s">
-        <v>162</v>
-      </c>
-      <c r="V12" t="b">
-        <v>1</v>
-      </c>
-      <c r="W12" t="s">
-        <v>170</v>
+        <v>90</v>
+      </c>
+      <c r="K12" t="s">
+        <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D13" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E13" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F13" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G13" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H13" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I13" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J13" t="s">
-        <v>140</v>
-      </c>
-      <c r="L13" t="b">
-        <v>1</v>
-      </c>
-      <c r="M13" t="s">
-        <v>141</v>
-      </c>
-      <c r="N13" t="s">
-        <v>131</v>
-      </c>
-      <c r="P13" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q13" t="s">
         <v>97</v>
       </c>
-      <c r="R13" t="s">
-        <v>156</v>
-      </c>
-      <c r="S13" t="b">
-        <v>1</v>
-      </c>
-      <c r="T13" t="s">
-        <v>171</v>
-      </c>
-      <c r="U13" t="s">
-        <v>156</v>
-      </c>
-      <c r="V13" t="b">
-        <v>1</v>
-      </c>
-      <c r="W13" t="s">
-        <v>171</v>
+      <c r="K13" t="s">
+        <v>98</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>99</v>
+      </c>
+      <c r="C14" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14" t="s">
+        <v>101</v>
+      </c>
+      <c r="E14" t="s">
+        <v>102</v>
+      </c>
+      <c r="F14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" t="s">
+        <v>103</v>
+      </c>
+      <c r="H14" t="s">
+        <v>104</v>
+      </c>
+      <c r="I14" t="s">
+        <v>104</v>
+      </c>
+      <c r="J14" t="s">
+        <v>105</v>
+      </c>
+      <c r="K14" t="s">
         <v>98</v>
       </c>
-      <c r="C14" t="s">
-        <v>99</v>
-      </c>
-      <c r="D14" t="s">
-        <v>100</v>
-      </c>
-      <c r="E14" t="s">
-        <v>101</v>
-      </c>
-      <c r="F14" t="s">
-        <v>35</v>
-      </c>
-      <c r="G14" t="s">
-        <v>102</v>
-      </c>
-      <c r="H14" t="s">
-        <v>103</v>
-      </c>
-      <c r="I14" t="s">
-        <v>103</v>
-      </c>
-      <c r="J14" t="s">
-        <v>140</v>
-      </c>
-      <c r="L14" t="b">
-        <v>1</v>
-      </c>
-      <c r="M14" t="s">
-        <v>141</v>
-      </c>
-      <c r="N14" t="s">
-        <v>142</v>
-      </c>
-      <c r="P14" t="s">
-        <v>104</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>97</v>
-      </c>
-      <c r="R14" t="s">
-        <v>158</v>
-      </c>
-      <c r="S14" t="b">
-        <v>1</v>
-      </c>
-      <c r="T14" t="s">
-        <v>170</v>
-      </c>
-      <c r="U14" t="s">
-        <v>158</v>
-      </c>
-      <c r="V14" t="b">
-        <v>1</v>
-      </c>
-      <c r="W14" t="s">
-        <v>170</v>
-      </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E15" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F15" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G15" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H15" t="s">
-        <v>152</v>
+        <v>119</v>
       </c>
       <c r="I15" t="s">
-        <v>152</v>
-      </c>
-      <c r="P15" t="s">
-        <v>81</v>
-      </c>
-      <c r="R15" t="s">
-        <v>156</v>
-      </c>
-      <c r="S15" t="b">
-        <v>1</v>
-      </c>
-      <c r="T15" t="s">
-        <v>172</v>
-      </c>
-      <c r="U15" t="s">
-        <v>156</v>
-      </c>
-      <c r="V15" t="b">
-        <v>1</v>
-      </c>
-      <c r="W15" t="s">
-        <v>172</v>
+        <v>119</v>
+      </c>
+      <c r="J15" t="s">
+        <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D16" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E16" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F16" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G16" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H16" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I16" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="J16" t="s">
-        <v>140</v>
-      </c>
-      <c r="L16" t="b">
-        <v>1</v>
-      </c>
-      <c r="M16" t="s">
-        <v>141</v>
-      </c>
-      <c r="N16" t="s">
-        <v>143</v>
-      </c>
-      <c r="P16" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>97</v>
-      </c>
-      <c r="R16" t="s">
-        <v>158</v>
-      </c>
-      <c r="S16" t="b">
-        <v>1</v>
-      </c>
-      <c r="T16" t="s">
-        <v>170</v>
-      </c>
-      <c r="U16" t="s">
-        <v>158</v>
-      </c>
-      <c r="V16" t="b">
-        <v>1</v>
-      </c>
-      <c r="W16" t="s">
-        <v>170</v>
+        <v>112</v>
+      </c>
+      <c r="K16" t="s">
+        <v>98</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G17" t="s">
-        <v>113</v>
-      </c>
-      <c r="R17" t="s">
-        <v>173</v>
-      </c>
-      <c r="S17" t="b">
-        <v>1</v>
-      </c>
-      <c r="T17" t="s">
-        <v>170</v>
-      </c>
-      <c r="U17" t="s">
-        <v>173</v>
-      </c>
-      <c r="V17" t="b">
-        <v>1</v>
-      </c>
-      <c r="W17" t="s">
-        <v>170</v>
+        <v>127</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2476,9 +1853,6 @@
       <c r="F18" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="D24" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
**Pre-Applied:** (Enhancement) Include PWK01 attachment codes [FHIR-44871]
</commit_message>
<xml_diff>
--- a/input/images/data-element-mapping.xlsx
+++ b/input/images/data-element-mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/davinci-ecdx/input/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{182B0C55-2482-2441-B491-48D57195849E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{781E147C-4A71-024C-8907-5EF46D18CA77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34140" yWindow="500" windowWidth="34120" windowHeight="28300"/>
+    <workbookView xWindow="52500" yWindow="500" windowWidth="51200" windowHeight="28300"/>
   </bookViews>
   <sheets>
     <sheet name="data-element-mapping" sheetId="1" r:id="rId1"/>
@@ -61,6 +61,9 @@
     <t>Loop: 2200D Segment: TRN02 Notes: TRN01 = "1"</t>
   </si>
   <si>
+    <t>&lt;span class="bg-success" markdown="1"&gt;Loop: 2000E - Patient Event Level or Loop: 2000F Service Level Segment: TRN02 Notes: TRN01 = “1”: Payer Supplied TRN01 = “2” : Provider Supplied (echoed back)&lt;/span&gt;&lt;!-- new-content --&gt;</t>
+  </si>
+  <si>
     <t>Loop: 2000A Segment: TRN02</t>
   </si>
   <si>
@@ -70,6 +73,12 @@
     <t>Task.identifier</t>
   </si>
   <si>
+    <t>For *unsolicited* attachments, this is the provider-assigned tracking/control number. For *solicited* attachments, this is the payer-assigned tracking/control number.</t>
+  </si>
+  <si>
+    <t>Payer-assigned tracking/control number</t>
+  </si>
+  <si>
     <t xml:space="preserve"> ClaimResponse.identifier, ClaimResponse.item.commmunicationRequest: CommunicationRequest.identifier</t>
   </si>
   <si>
@@ -139,6 +148,9 @@
     <t>(operation endpoint)</t>
   </si>
   <si>
+    <t>"PayerUrl" Task.input</t>
+  </si>
+  <si>
     <t>Payer endpoint where the attachments are submitted using the $submit-attachment operation</t>
   </si>
   <si>
@@ -214,6 +226,9 @@
     <t>Task.reasonReference.identifier</t>
   </si>
   <si>
+    <t>Provider-assigned claim/prior authorization ID</t>
+  </si>
+  <si>
     <t>ClaimResponse.request: Claim.identifier</t>
   </si>
   <si>
@@ -223,12 +238,21 @@
     <t>Line Item(s)</t>
   </si>
   <si>
+    <t>&lt;span class="bg-success" markdown="1"&gt;Note that this is an indirect mapping:  Loop 2220D (Service Line Information) Segment SVC01 or SVC04 codes reference the claim service item, which contains the line item.&lt;/span&gt;&lt;!-- new-content --&gt;</t>
+  </si>
+  <si>
+    <t>&lt;span class="bg-success" markdown="1"&gt;Loop: 2000F Segment: HL01&lt;!-- new-content --&gt;</t>
+  </si>
+  <si>
     <t>Loop: 2000A Segment: STC10 Notes: Used to convey status of the entire claim or a specific service line</t>
   </si>
   <si>
     <t>Attachment.LineItem</t>
   </si>
   <si>
+    <t>“attachmentsNeeded” Task.input.extension</t>
+  </si>
+  <si>
     <t>Claim/prior authorization line item numbers</t>
   </si>
   <si>
@@ -238,19 +262,19 @@
     <t>ClaimResponse = Bundle.entry[0].resource</t>
   </si>
   <si>
-    <t>LOINC Attachment Code</t>
-  </si>
-  <si>
     <t>Loop: 2220D Segments: STC01-02, STC10-02, STC11-02</t>
   </si>
   <si>
+    <t>&lt;span class="bg-success" markdown="1"&gt;Loop: 2000E - Patient Event Level or Loop: 2000F Service Level Segment: HI (LOINC) or Segment: PWK01 Report Type Codes &lt;!-- new-content --&gt;</t>
+  </si>
+  <si>
     <t>Loop: 2000A Segment: STC01-01</t>
   </si>
   <si>
     <t>Attachment.Code</t>
   </si>
   <si>
-    <t>LOINC attachment codes</t>
+    <t>“attachmentsNeeded” Task.input </t>
   </si>
   <si>
     <t>ClaimResponse.item.commmunicationRequest: CommunicationRequest.payload.extension:contentModifier</t>
@@ -349,6 +373,9 @@
     <t>Loop: 2010C Segment: REF02 Notes: REF01 = "EJ"</t>
   </si>
   <si>
+    <t>Patient Account Number is a provider-assigned identifier</t>
+  </si>
+  <si>
     <t>Date of Birth</t>
   </si>
   <si>
@@ -364,46 +391,19 @@
     <t>Questionnaire</t>
   </si>
   <si>
+    <t>“questionnaireNeeded” Task.input</t>
+  </si>
+  <si>
     <t>QuestionnaireResponse</t>
   </si>
   <si>
     <t>Attachment.Content</t>
   </si>
   <si>
-    <t>For *unsolicited* attachments, this is the provider-assigned tracking/control number. For *solicited* attachments, this is the payer-assigned tracking/control number.</t>
-  </si>
-  <si>
-    <t>Payer-assigned tracking/control number</t>
-  </si>
-  <si>
-    <t>Provider-assigned claim/prior authorization ID</t>
-  </si>
-  <si>
-    <t>Patient Account Number is a provider-assigned identifier</t>
-  </si>
-  <si>
-    <t>&lt;span class="bg-success" markdown="1"&gt;Note that this is an indirect mapping:  Loop 2220D (Service Line Information) Segment SVC01 or SVC04 codes reference the claim service item, which contains the line item.&lt;/span&gt;&lt;!-- new-content --&gt;</t>
-  </si>
-  <si>
-    <t>&lt;span class="bg-success" markdown="1"&gt;Loop: 2000E - Patient Event Level or Loop: 2000F Service Level Segment: TRN02 Notes: TRN01 = “1”: Payer Supplied TRN01 = “2” : Provider Supplied (echoed back)&lt;/span&gt;&lt;!-- new-content --&gt;</t>
-  </si>
-  <si>
-    <t>&lt;span class="bg-success" markdown="1"&gt;Loop: 2000F Segment: HL01&lt;!-- new-content --&gt;</t>
-  </si>
-  <si>
-    <t>&lt;span class="bg-success" markdown="1"&gt;Loop: 2000E - Patient Event Level or Loop: 2000F Service Level Segment: HI (LOINC) or Segment: PWK01 Report Type Codes &lt;!-- new-content --&gt;</t>
-  </si>
-  <si>
-    <t>"PayerUrl" Task.input</t>
-  </si>
-  <si>
-    <t>“attachmentsNeeded” Task.input.extension</t>
-  </si>
-  <si>
-    <t>“attachmentsNeeded” Task.input </t>
-  </si>
-  <si>
-    <t>“questionnaireNeeded” Task.input</t>
+    <t xml:space="preserve"> &lt;span class="bg-success" markdown="1"&gt;LOINC Attachment Code.  For prior authorization, [X12] PWK01 Report Type Codes may also be used&lt;/span&gt;&lt;!-- new-content --&gt;.</t>
+  </si>
+  <si>
+    <t>&lt;span class="bg-success" markdown="1"&gt;Attachment Code&lt;!-- new-content --&gt;</t>
   </si>
 </sst>
 </file>
@@ -1266,16 +1266,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="96" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1"/>
-    <col min="5" max="5" width="31.83203125" customWidth="1"/>
-    <col min="7" max="7" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="192.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="138.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="78.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
@@ -1324,28 +1326,28 @@
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>121</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H2" t="s">
-        <v>116</v>
+        <v>17</v>
       </c>
       <c r="I2" t="s">
-        <v>117</v>
+        <v>18</v>
       </c>
       <c r="J2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="K2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -1353,34 +1355,34 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="H3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="I3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="J3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="K3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -1388,34 +1390,34 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" t="s">
         <v>29</v>
       </c>
-      <c r="F4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" t="s">
-        <v>26</v>
-      </c>
       <c r="I4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="J4" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="K4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -1423,34 +1425,34 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G5" t="s">
-        <v>124</v>
+        <v>42</v>
       </c>
       <c r="H5" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="I5" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="J5" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="K5" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -1458,34 +1460,34 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E6" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F6" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G6" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="H6" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="I6" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="J6" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="K6" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -1493,34 +1495,34 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D7" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="E7" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="F7" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="G7" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="H7" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="I7" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="J7" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="K7" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -1528,34 +1530,34 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C8" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D8" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E8" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F8" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G8" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="H8" t="s">
-        <v>118</v>
+        <v>68</v>
       </c>
       <c r="I8" t="s">
-        <v>118</v>
+        <v>68</v>
       </c>
       <c r="J8" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="K8" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -1563,34 +1565,34 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C9" t="s">
-        <v>120</v>
+        <v>72</v>
       </c>
       <c r="D9" t="s">
-        <v>122</v>
+        <v>73</v>
       </c>
       <c r="E9" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="F9" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="G9" t="s">
-        <v>125</v>
+        <v>76</v>
       </c>
       <c r="H9" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="I9" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="J9" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="K9" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -1598,34 +1600,34 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
+        <v>127</v>
       </c>
       <c r="C10" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="D10" t="s">
-        <v>123</v>
+        <v>81</v>
       </c>
       <c r="E10" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F10" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="G10" t="s">
+        <v>84</v>
+      </c>
+      <c r="H10" t="s">
         <v>126</v>
       </c>
-      <c r="H10" t="s">
-        <v>76</v>
-      </c>
       <c r="I10" t="s">
-        <v>76</v>
+        <v>126</v>
       </c>
       <c r="J10" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="K10" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -1633,31 +1635,31 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="C11" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="D11" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E11" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F11" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G11" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="H11" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="I11" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="J11" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -1665,34 +1667,34 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="C12" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="D12" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="E12" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="F12" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="G12" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="H12" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="I12" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="J12" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="K12" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -1700,34 +1702,34 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D13" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="E13" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="F13" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="G13" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="H13" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="I13" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="J13" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="K13" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -1735,34 +1737,34 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="C14" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="D14" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="E14" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="F14" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G14" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="H14" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="I14" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="J14" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="K14" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -1770,31 +1772,31 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="C15" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="D15" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="E15" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F15" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G15" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="H15" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I15" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="J15" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -1802,34 +1804,34 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="C16" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D16" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="E16" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F16" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G16" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="H16" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="I16" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="J16" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="K16" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -1837,10 +1839,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="G17" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -1848,10 +1850,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="F18" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Conforming to CDex Attachments and Requesting Attachments Using Attachments Codes pages; Copy editing changes prior to comment period to ensure accuracy, clarity, and readability. [FHIR-46508]
</commit_message>
<xml_diff>
--- a/input/images/data-element-mapping.xlsx
+++ b/input/images/data-element-mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/davinci-ecdx/input/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{781E147C-4A71-024C-8907-5EF46D18CA77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8F831299-FB97-7641-8860-0FCDAF07DC4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="52500" yWindow="500" windowWidth="51200" windowHeight="28300"/>
+    <workbookView xWindow="68260" yWindow="500" windowWidth="34140" windowHeight="28300" xr2:uid="{74E55104-5A40-144F-87B8-0E41B2524620}"/>
   </bookViews>
   <sheets>
     <sheet name="data-element-mapping" sheetId="1" r:id="rId1"/>
@@ -250,9 +250,6 @@
     <t>Attachment.LineItem</t>
   </si>
   <si>
-    <t>“attachmentsNeeded” Task.input.extension</t>
-  </si>
-  <si>
     <t>Claim/prior authorization line item numbers</t>
   </si>
   <si>
@@ -262,6 +259,9 @@
     <t>ClaimResponse = Bundle.entry[0].resource</t>
   </si>
   <si>
+    <t>&lt;span class="bg-success" markdown="1"&gt;Attachment Code&lt;!-- new-content --&gt;</t>
+  </si>
+  <si>
     <t>Loop: 2220D Segments: STC01-02, STC10-02, STC11-02</t>
   </si>
   <si>
@@ -274,7 +274,7 @@
     <t>Attachment.Code</t>
   </si>
   <si>
-    <t>“attachmentsNeeded” Task.input </t>
+    <t xml:space="preserve"> &lt;span class="bg-success" markdown="1"&gt;LOINC Attachment Code.  For prior authorization, [X12] PWK01 Report Type Codes may also be used&lt;/span&gt;&lt;!-- new-content --&gt;.</t>
   </si>
   <si>
     <t>ClaimResponse.item.commmunicationRequest: CommunicationRequest.payload.extension:contentModifier</t>
@@ -391,26 +391,356 @@
     <t>Questionnaire</t>
   </si>
   <si>
-    <t>“questionnaireNeeded” Task.input</t>
-  </si>
-  <si>
     <t>QuestionnaireResponse</t>
   </si>
   <si>
     <t>Attachment.Content</t>
   </si>
   <si>
-    <t xml:space="preserve"> &lt;span class="bg-success" markdown="1"&gt;LOINC Attachment Code.  For prior authorization, [X12] PWK01 Report Type Codes may also be used&lt;/span&gt;&lt;!-- new-content --&gt;.</t>
-  </si>
-  <si>
-    <t>&lt;span class="bg-success" markdown="1"&gt;Attachment Code&lt;!-- new-content --&gt;</t>
+    <r>
+      <t>&lt;span</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFE50000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>class</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>"bg-success"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFE50000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>markdown</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>"1"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF800000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>“AttachmentsNeeded” Task.input.extension</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF800000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&lt;/span&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&lt;!-- new-content --&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;span</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFE50000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>class</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>"bg-success"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFE50000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>markdown</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>"1"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF800000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>“AttachmentsNeeded” Task.input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF800000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&lt;/span&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&lt;!-- new-content --&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;span</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFE50000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>class</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>"bg-success"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFE50000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>markdown</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>"1"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF800000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>“QuestionnairesNeeded” Task.input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF800000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&lt;/span&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&lt;!-- new-content --&gt;</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -544,6 +874,36 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF800000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFE50000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0000FF"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF008000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -887,8 +1247,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1263,21 +1624,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3907BD1-DC2D-9048-8A82-02F0B554F1F0}">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="192.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="40" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="138.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="78.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="67" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="127.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="68.1640625" customWidth="1"/>
+    <col min="9" max="9" width="47.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
@@ -1580,19 +1939,19 @@
         <v>75</v>
       </c>
       <c r="G9" t="s">
+        <v>125</v>
+      </c>
+      <c r="H9" t="s">
         <v>76</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
+        <v>76</v>
+      </c>
+      <c r="J9" t="s">
         <v>77</v>
       </c>
-      <c r="I9" t="s">
-        <v>77</v>
-      </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>78</v>
-      </c>
-      <c r="K9" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -1600,7 +1959,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>127</v>
+        <v>79</v>
       </c>
       <c r="C10" t="s">
         <v>80</v>
@@ -1615,19 +1974,19 @@
         <v>83</v>
       </c>
       <c r="G10" t="s">
+        <v>126</v>
+      </c>
+      <c r="H10" t="s">
         <v>84</v>
       </c>
-      <c r="H10" t="s">
-        <v>126</v>
-      </c>
       <c r="I10" t="s">
-        <v>126</v>
+        <v>84</v>
       </c>
       <c r="J10" t="s">
         <v>85</v>
       </c>
       <c r="K10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -1694,7 +2053,7 @@
         <v>98</v>
       </c>
       <c r="K12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -1841,8 +2200,8 @@
       <c r="B17" t="s">
         <v>122</v>
       </c>
-      <c r="G17" t="s">
-        <v>123</v>
+      <c r="G17" s="1" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -1850,13 +2209,14 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>123</v>
+      </c>
+      <c r="F18" t="s">
         <v>124</v>
-      </c>
-      <c r="F18" t="s">
-        <v>125</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed malformed csv, and excel files
</commit_message>
<xml_diff>
--- a/input/images/data-element-mapping.xlsx
+++ b/input/images/data-element-mapping.xlsx
@@ -1,26 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <workbookPr dateCompatibility="0" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/davinci-ecdx/input/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8F831299-FB97-7641-8860-0FCDAF07DC4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EBA63223-C770-8F43-9F9E-C23CC2A041C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="68260" yWindow="500" windowWidth="34140" windowHeight="28300" xr2:uid="{74E55104-5A40-144F-87B8-0E41B2524620}"/>
+    <workbookView xWindow="51200" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{32788C65-FB79-0C4A-973F-D0B6FDEBC2B8}"/>
   </bookViews>
   <sheets>
     <sheet name="data-element-mapping" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="128">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="163" uniqueCount="128">
   <si>
     <t>No</t>
   </si>
@@ -61,7 +66,7 @@
     <t>Loop: 2200D Segment: TRN02 Notes: TRN01 = "1"</t>
   </si>
   <si>
-    <t>&lt;span class="bg-success" markdown="1"&gt;Loop: 2000E - Patient Event Level or Loop: 2000F Service Level Segment: TRN02 Notes: TRN01 = “1”: Payer Supplied TRN01 = “2” : Provider Supplied (echoed back)&lt;/span&gt;&lt;!-- new-content --&gt;</t>
+    <t>Loop: 2000E - Patient Event Level or Loop: 2000F Service Level Segment: TRN02 Notes: TRN01 = “1”: Payer Supplied TRN01 = “2” : Provider Supplied (echoed back)</t>
   </si>
   <si>
     <t>Loop: 2000A Segment: TRN02</t>
@@ -238,10 +243,10 @@
     <t>Line Item(s)</t>
   </si>
   <si>
-    <t>&lt;span class="bg-success" markdown="1"&gt;Note that this is an indirect mapping:  Loop 2220D (Service Line Information) Segment SVC01 or SVC04 codes reference the claim service item, which contains the line item.&lt;/span&gt;&lt;!-- new-content --&gt;</t>
-  </si>
-  <si>
-    <t>&lt;span class="bg-success" markdown="1"&gt;Loop: 2000F Segment: HL01&lt;!-- new-content --&gt;</t>
+    <t>Note that this is an indirect mapping:  Loop 2220D (Service Line Information) Segment SVC01 or SVC04 codes reference the claim service item, which contains the line item.</t>
+  </si>
+  <si>
+    <t>Loop: 2000F Segment: HL01</t>
   </si>
   <si>
     <t>Loop: 2000A Segment: STC10 Notes: Used to convey status of the entire claim or a specific service line</t>
@@ -250,6 +255,9 @@
     <t>Attachment.LineItem</t>
   </si>
   <si>
+    <t>“AttachmentsNeeded” Task.input.extension</t>
+  </si>
+  <si>
     <t>Claim/prior authorization line item numbers</t>
   </si>
   <si>
@@ -259,13 +267,13 @@
     <t>ClaimResponse = Bundle.entry[0].resource</t>
   </si>
   <si>
-    <t>&lt;span class="bg-success" markdown="1"&gt;Attachment Code&lt;!-- new-content --&gt;</t>
+    <t>Attachment Code</t>
   </si>
   <si>
     <t>Loop: 2220D Segments: STC01-02, STC10-02, STC11-02</t>
   </si>
   <si>
-    <t>&lt;span class="bg-success" markdown="1"&gt;Loop: 2000E - Patient Event Level or Loop: 2000F Service Level Segment: HI (LOINC) or Segment: PWK01 Report Type Codes &lt;!-- new-content --&gt;</t>
+    <t xml:space="preserve">Loop: 2000E - Patient Event Level or Loop: 2000F Service Level Segment: HI (LOINC) or Segment: PWK01 Report Type Codes </t>
   </si>
   <si>
     <t>Loop: 2000A Segment: STC01-01</t>
@@ -274,7 +282,10 @@
     <t>Attachment.Code</t>
   </si>
   <si>
-    <t xml:space="preserve"> &lt;span class="bg-success" markdown="1"&gt;LOINC Attachment Code.  For prior authorization, [X12] PWK01 Report Type Codes may also be used&lt;/span&gt;&lt;!-- new-content --&gt;.</t>
+    <t>“AttachmentsNeeded” Task.input</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LOINC Attachment Code.  For prior authorization, [X12] PWK01 Report Type Codes may also be used.</t>
   </si>
   <si>
     <t>ClaimResponse.item.commmunicationRequest: CommunicationRequest.payload.extension:contentModifier</t>
@@ -391,356 +402,20 @@
     <t>Questionnaire</t>
   </si>
   <si>
+    <t>“QuestionnairesNeeded” Task.input</t>
+  </si>
+  <si>
     <t>QuestionnaireResponse</t>
   </si>
   <si>
     <t>Attachment.Content</t>
-  </si>
-  <si>
-    <r>
-      <t>&lt;span</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFE50000"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>class</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>"bg-success"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFE50000"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>markdown</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>"1"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF800000"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>“AttachmentsNeeded” Task.input.extension</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF800000"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>&lt;/span&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF008000"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>&lt;!-- new-content --&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>&lt;span</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFE50000"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>class</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>"bg-success"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFE50000"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>markdown</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>"1"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF800000"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>“AttachmentsNeeded” Task.input</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF800000"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>&lt;/span&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF008000"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>&lt;!-- new-content --&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>&lt;span</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFE50000"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>class</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>"bg-success"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFE50000"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>markdown</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>"1"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF800000"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>“QuestionnairesNeeded” Task.input</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF800000"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>&lt;/span&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF008000"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>&lt;!-- new-content --&gt;</t>
-    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -875,36 +550,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Menlo"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF800000"/>
-      <name val="Menlo"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFE50000"/>
-      <name val="Menlo"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF0000FF"/>
-      <name val="Menlo"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF008000"/>
-      <name val="Menlo"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -1089,15 +734,15 @@
   </fills>
   <borders count="10">
     <border>
-      <left/>
-      <right/>
+      <start/>
+      <end/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <start/>
+      <end/>
       <top/>
       <bottom style="thick">
         <color theme="4"/>
@@ -1105,8 +750,8 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <start/>
+      <end/>
       <top/>
       <bottom style="thick">
         <color theme="4" tint="0.499984740745262"/>
@@ -1114,8 +759,8 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <start/>
+      <end/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.39997558519241921"/>
@@ -1123,12 +768,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <start style="thin">
         <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
+      </start>
+      <end style="thin">
         <color rgb="FF7F7F7F"/>
-      </right>
+      </end>
       <top style="thin">
         <color rgb="FF7F7F7F"/>
       </top>
@@ -1138,12 +783,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <start style="thin">
         <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
+      </start>
+      <end style="thin">
         <color rgb="FF3F3F3F"/>
-      </right>
+      </end>
       <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
@@ -1153,8 +798,8 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <start/>
+      <end/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -1162,12 +807,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <start style="double">
         <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
+      </start>
+      <end style="double">
         <color rgb="FF3F3F3F"/>
-      </right>
+      </end>
       <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
@@ -1177,12 +822,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <start style="thin">
         <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
+      </start>
+      <end style="thin">
         <color rgb="FFB2B2B2"/>
-      </right>
+      </end>
       <top style="thin">
         <color rgb="FFB2B2B2"/>
       </top>
@@ -1192,8 +837,8 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <start/>
+      <end/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -1247,9 +892,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1309,7 +953,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1462,25 +1106,25 @@
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
+            <a:gs pos="0%">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:lumMod val="110%"/>
+                <a:satMod val="105%"/>
+                <a:tint val="67%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="50%">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:lumMod val="105%"/>
+                <a:satMod val="103%"/>
+                <a:tint val="73%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100000">
+            <a:gs pos="100%">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:lumMod val="105%"/>
+                <a:satMod val="109%"/>
+                <a:tint val="81%"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -1488,25 +1132,25 @@
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
+            <a:gs pos="0%">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:satMod val="103%"/>
+                <a:lumMod val="102%"/>
+                <a:tint val="94%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="50%">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:satMod val="110%"/>
+                <a:lumMod val="100%"/>
+                <a:shade val="100%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100000">
+            <a:gs pos="100%">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:lumMod val="99%"/>
+                <a:satMod val="120%"/>
+                <a:shade val="78%"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -1519,21 +1163,21 @@
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter lim="800%"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter lim="800%"/>
         </a:ln>
         <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter lim="800%"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
@@ -1547,7 +1191,7 @@
           <a:effectLst>
             <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="63%"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -1559,32 +1203,32 @@
         </a:solidFill>
         <a:solidFill>
           <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
+            <a:tint val="95%"/>
+            <a:satMod val="170%"/>
           </a:schemeClr>
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
+            <a:gs pos="0%">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="93%"/>
+                <a:satMod val="150%"/>
+                <a:shade val="98%"/>
+                <a:lumMod val="102%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="50%">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="98%"/>
+                <a:satMod val="130%"/>
+                <a:shade val="90%"/>
+                <a:lumMod val="103%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100000">
+            <a:gs pos="100%">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="63%"/>
+                <a:satMod val="120%"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -1624,19 +1268,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3907BD1-DC2D-9048-8A82-02F0B554F1F0}">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67F1E6EC-B097-3D43-BD18-7F9C05C4BA68}">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="67" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="127.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="68.1640625" customWidth="1"/>
-    <col min="9" max="9" width="47.5" customWidth="1"/>
+    <col min="1" max="12" width="45.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
@@ -1939,19 +1580,19 @@
         <v>75</v>
       </c>
       <c r="G9" t="s">
-        <v>125</v>
+        <v>76</v>
       </c>
       <c r="H9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -1959,34 +1600,34 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" t="s">
+        <v>83</v>
+      </c>
+      <c r="F10" t="s">
+        <v>84</v>
+      </c>
+      <c r="G10" t="s">
+        <v>85</v>
+      </c>
+      <c r="H10" t="s">
+        <v>86</v>
+      </c>
+      <c r="I10" t="s">
+        <v>86</v>
+      </c>
+      <c r="J10" t="s">
+        <v>87</v>
+      </c>
+      <c r="K10" t="s">
         <v>79</v>
-      </c>
-      <c r="C10" t="s">
-        <v>80</v>
-      </c>
-      <c r="D10" t="s">
-        <v>81</v>
-      </c>
-      <c r="E10" t="s">
-        <v>82</v>
-      </c>
-      <c r="F10" t="s">
-        <v>83</v>
-      </c>
-      <c r="G10" t="s">
-        <v>126</v>
-      </c>
-      <c r="H10" t="s">
-        <v>84</v>
-      </c>
-      <c r="I10" t="s">
-        <v>84</v>
-      </c>
-      <c r="J10" t="s">
-        <v>85</v>
-      </c>
-      <c r="K10" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -1994,10 +1635,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C11" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D11" t="s">
         <v>40</v>
@@ -2009,16 +1650,16 @@
         <v>40</v>
       </c>
       <c r="G11" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H11" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="I11" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="J11" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -2026,34 +1667,34 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C12" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D12" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E12" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F12" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="G12" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="H12" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="I12" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="J12" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="K12" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -2061,34 +1702,34 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C13" t="s">
         <v>55</v>
       </c>
       <c r="D13" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E13" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F13" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G13" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H13" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I13" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="J13" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="K13" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -2096,34 +1737,34 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C14" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D14" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E14" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="F14" t="s">
         <v>40</v>
       </c>
       <c r="G14" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="H14" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="I14" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="J14" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="K14" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -2131,13 +1772,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C15" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D15" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E15" t="s">
         <v>40</v>
@@ -2146,16 +1787,16 @@
         <v>40</v>
       </c>
       <c r="G15" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H15" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="I15" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="J15" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -2163,13 +1804,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C16" t="s">
         <v>40</v>
       </c>
       <c r="D16" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E16" t="s">
         <v>40</v>
@@ -2178,19 +1819,19 @@
         <v>40</v>
       </c>
       <c r="G16" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="H16" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="I16" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="J16" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="K16" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -2198,10 +1839,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>122</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
+      </c>
+      <c r="G17" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -2209,14 +1850,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="F18" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add FHIR-49828 Add Administration Reference Number as identifier to Task and $submit-attachments
</commit_message>
<xml_diff>
--- a/input/images/data-element-mapping.xlsx
+++ b/input/images/data-element-mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/davinci-ecdx/input/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EBA63223-C770-8F43-9F9E-C23CC2A041C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DCC26676-81D7-7949-A804-9C227FF72F58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{32788C65-FB79-0C4A-973F-D0B6FDEBC2B8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="102400" windowHeight="28800" xr2:uid="{8E0805B7-C227-7B40-8113-5FF95FC0AF88}"/>
   </bookViews>
   <sheets>
     <sheet name="data-element-mapping" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="163" uniqueCount="128">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="244" uniqueCount="169">
   <si>
     <t>No</t>
   </si>
@@ -54,10 +54,22 @@
     <t>Request Attachments Comments</t>
   </si>
   <si>
-    <t>ClaimResponse (from PAS Response Bundle)</t>
-  </si>
-  <si>
-    <t>PAS Response Bundle</t>
+    <t>PAS Response Bundle Mapping to $submit-attachment Description</t>
+  </si>
+  <si>
+    <t>FHIRPath mapping to $submit-attachment</t>
+  </si>
+  <si>
+    <t>PAS Response Bundle Mapping to $submit-attachment Comments</t>
+  </si>
+  <si>
+    <t>PAS Task Profile Element</t>
+  </si>
+  <si>
+    <t>FHIRPath for mapping from PAS Claim Response Bundle to PAS Task</t>
+  </si>
+  <si>
+    <t>PAS Response Bundle Mapping  to PAS Task Comments</t>
   </si>
   <si>
     <t>Tracking ID</t>
@@ -84,10 +96,13 @@
     <t>Payer-assigned tracking/control number</t>
   </si>
   <si>
-    <t xml:space="preserve"> ClaimResponse.identifier, ClaimResponse.item.commmunicationRequest: CommunicationRequest.identifier</t>
-  </si>
-  <si>
-    <t>ClaimResponse = Bundle.entry[0].resource, CommunicationRequest = Bundle.entry[n].resource referenced by ClaimResponse.communincationRequest</t>
+    <t>The ClaimResponse's first identifier element</t>
+  </si>
+  <si>
+    <t>Bundle.entry[0].resource.identifier[0]</t>
+  </si>
+  <si>
+    <t>Maps to the "Patient Event Trace Number" in X12 278R</t>
   </si>
   <si>
     <t>Use</t>
@@ -108,12 +123,15 @@
     <t>Choice of "claim" or "preauthorization"</t>
   </si>
   <si>
-    <t>preauthorization</t>
-  </si>
-  <si>
     <t>Fixed to "preauthorization"</t>
   </si>
   <si>
+    <t>Task.reasonCode ( Fixed to "priorAuthorization")</t>
+  </si>
+  <si>
+    <t>Fixed to "priorAuthorization"</t>
+  </si>
+  <si>
     <t>Payer ID</t>
   </si>
   <si>
@@ -132,10 +150,13 @@
     <t>Task.requester.identifier</t>
   </si>
   <si>
-    <t>ClaimResponse.insurer: Organization.identifier</t>
-  </si>
-  <si>
-    <t>ClaimResponse = Bundle.entry[0].resource, Organization = Bundle.entry[n].resource referenced by ClaimResponse.insurer</t>
+    <t>The first identifier element of the Organization referenced by the ClaimResponse's insurer element.</t>
+  </si>
+  <si>
+    <t>Bundle.entry.where(fullUrl = %context.entry[0].resource.insurer.reference or (resource.resourceType = 'Organization' and resource.id =%context.entry[0].resource.insurer.reference.split('/').last())).resource.identifier[0]</t>
+  </si>
+  <si>
+    <t>FHIRPath for absolute and relative references. Using the FHIRPath function. "resolve()" which is not universally supported and untested: "Bundle.entry[0].resource.insurer.resolve().resource.identifier[0]</t>
   </si>
   <si>
     <t>Payer URL</t>
@@ -156,10 +177,16 @@
     <t>"PayerUrl" Task.input</t>
   </si>
   <si>
+    <t>See the [Endpoint Discovery Strategy](https://hl7.org/fhir/us/davinci-hrex/endpoint-discovery.html) documented in the  Da Vinci Health Record Exchange (HRex) Impelementation guide</t>
+  </si>
+  <si>
     <t>Payer endpoint where the attachments are submitted using the $submit-attachment operation</t>
   </si>
   <si>
-    <t>out of band</t>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>"PayerUrl" Task.input (Task.input.where(''payer-url' in  type,codining.code)).valueUrl</t>
   </si>
   <si>
     <t>Organization ID</t>
@@ -183,10 +210,16 @@
     <t>Organization of provider who submitted claim/prior authorization</t>
   </si>
   <si>
-    <t>ClaimResponse.requester: Organization.identifier, ClaimResponse.requester: PractitionerRole.organization: Organziation.identifier</t>
-  </si>
-  <si>
-    <t>ClaimResponse = Bundle.entry[0].resource, Organization,PractitionerRole = Bundle.entry[n].resource referenced by ClaimResponse.requester</t>
+    <t>If present, the first identifier element of the Organization referenced by the ClaimResponse's requester element or the first identifier element of the Organization referenced by the organization element of the PractitiionerRole referenced by the ClaimResponse's requester element.</t>
+  </si>
+  <si>
+    <t>Bundle.entry.where(resource.resourceType = 'Organization' and (fullUrl = %context.entry[0].resource.requester.reference or resource.id =%context.entry[0].resource.requester.reference.split('/').last() or (fullUrl = (%context.entry.where(resource.resourceType = 'PractitionerRole' and (fullUrl = %context.entry[0].resource.requester.reference or resource.id = %context.entry[0].resource.requester.reference.split('/').last())).resource.organization.reference) or resource.id = (%context.entry.where(resource.resourceType = 'PractitionerRole' and (fullUrl = %context.entry[0].resource.requester.reference or resource.id = %context.entry[0].resource.requester.reference.split('/').last())).resource.organization.reference).split('/').last()))).resource.identifier[0]</t>
+  </si>
+  <si>
+    <t>"The ClaimResponse's requester element has a choice of Organization and PractitionerRole target types. FHIRPath for absolute and relative references.  Using the FHIRPath function. "resolve()" which in not universally supported and untested: "Bundle.entry.where(resource.resourceType = 'Organization' and (fulllUrl = %context.entry[0].resource.requester.reference or fulllUrl = %context.entry[0].resource.requester.resolve().organization.reference or resource.id = %context.entry[0].resource.requester.reference.split('/').last() or resource.id = %context.entry[0].resource.requester.resolve().organization.reference.split('/').last())).resource.identifier[0]"</t>
+  </si>
+  <si>
+    <t>Task.owner.PractitionerRole.resolves().organization.identifier|Task.owner.organization.identifier</t>
   </si>
   <si>
     <t>Provider ID</t>
@@ -210,10 +243,16 @@
     <t>Provider who submitted claim/prior authorization</t>
   </si>
   <si>
-    <t>ClaimResponse.requester: PractitionerRole.practitioner: Practitioner.identifier</t>
-  </si>
-  <si>
-    <t>ClaimResponse = Bundle.entry[0].resource, PractitionerRole = Bundle.entry[n].resource referenced by ClaimResponse.requester</t>
+    <t>The first identifier element of the Practitioner referenced by the practitioner element of the PractitionerRole referenced by the ClaimResponse's requester element.</t>
+  </si>
+  <si>
+    <t>Bundle.entry.where(resource.resourceType = 'Practitioner' and (fullUrl = (%context.entry.where(resource.resourceType = 'PractitionerRole' and (fullUrl = %context.entry[0].resource.requester.reference or resource.id = %context.entry[0].resource.requester.reference.split('/').last())).resource.practitioner.reference) or resource.id = (%context.entry.where(resource.resourceType = 'PractitionerRole' and (fullUrl = %context.entry[0].resource.requester.reference or resource.id = %context.entry[0].resource.requester.reference.split('/').last())).resource.practitioner.reference).split('/').last())).resource.identifier[0]</t>
+  </si>
+  <si>
+    <t>The ClaimResponse's requester element has a choice of Organization and PractitionerRole target types. FHIRPath for absolute and relative references.  Using the FHIRPath function. "resolve()" which in not universally supported and untested: "Bundle.entry.where(fullUrl = %context.entry[0].resource.requester.resolve().practitioner.reference or (resource.resourceType = 'Practitioner' and resource.id = %context.entry[0].resource.requester.resolve().practitioner.reference.split('/').last()).resource.identifier[0]"</t>
+  </si>
+  <si>
+    <t>Task.owner.PractitionerRole.resolves().practitioner.identifier|Task.owner.practitioner.identifier</t>
   </si>
   <si>
     <t>Claim/PreAuth ID</t>
@@ -234,10 +273,22 @@
     <t>Provider-assigned claim/prior authorization ID</t>
   </si>
   <si>
-    <t>ClaimResponse.request: Claim.identifier</t>
-  </si>
-  <si>
-    <t>ClaimResponse = Bundle.entry[0].resource, Claim = Bundle.entry[n].resource referenced by ClaimResponse.request</t>
+    <t>The first  identifier element of the Claim referenced by the ClaimResponse's "request" element.</t>
+  </si>
+  <si>
+    <t>Bundle.entry.where(fullUrl = %context.entry[0].resource.request.reference or (resource.resourceType = 'Claim' and resource.id =%context.entry[0].resource.request.reference.split('/').last())).resource.identifier[0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FHIRPath for absolute and relative references. Using the FHIRPath function. "resolve()" which is not universally supported and untested: "Bundle.entry[0].resource.request.resolve().resource.identifier[0]"</t>
+  </si>
+  <si>
+    <t>Task.reasonReference. ( Task.reasonReference.resolves() to Claim resource)</t>
+  </si>
+  <si>
+    <t>Bundle.entry.where(fullUrl = %context.entry[0].resource.request.reference or (resource.resourceType = 'Claim' and resource.id =%context.entry[0].resource.request.reference.split('/').last())).resource</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> This element may reference the local FHIR CLAIM resource that was submitted</t>
   </si>
   <si>
     <t>Line Item(s)</t>
@@ -261,10 +312,16 @@
     <t>Claim/prior authorization line item numbers</t>
   </si>
   <si>
-    <t>ClaimResponse.item.extension:itemTraceNumber  Note: CommunicationRequest.payload.extension:serviceLineNumber references this item</t>
-  </si>
-  <si>
-    <t>ClaimResponse = Bundle.entry[0].resource</t>
+    <t>The CommunicationRequest payload element "serviceLineNumber" extension.</t>
+  </si>
+  <si>
+    <t>Bundle.entry.where(fullUrl = %context.entry[0].resource.communicationRequest.reference or (resource.resourceType = 'CommunicationRequest' and resource.id =%context.entry[0].resource.communicationRequest.reference.split('/').last())).resource.payload.extension.where(url='http://hl7.org/fhir/us/davinci-pas/StructureDefinition/extension-serviceLineNumber').valuePositiveInt</t>
+  </si>
+  <si>
+    <t>The ClaimResponse's communicationRequest element references the CommunicationRequest resource in the PAS response Bundle.  Will need to iterate through the payload items FHIRPath for absolute and relative references. Using the FHIRPath function. "resolve()" which is not universally supported and untested: "Bundle.entry[0].resource.communicationRequest.resolve().resource.payload.extension.where(url='http://hl7.org/fhir/us/davinci-pas/StructureDefinition/extension-serviceLineNumber').valuePositiveInt"</t>
+  </si>
+  <si>
+    <t>Task.input "paLineNumber" extension   (Task.input.extension.where(url = 'http://hl7.org/fhir/us/davinci-pas/StructureDefinition/extension-paLineNumber').valuePositiveInt)</t>
   </si>
   <si>
     <t>Attachment Code</t>
@@ -288,7 +345,16 @@
     <t xml:space="preserve"> LOINC Attachment Code.  For prior authorization, [X12] PWK01 Report Type Codes may also be used.</t>
   </si>
   <si>
-    <t>ClaimResponse.item.commmunicationRequest: CommunicationRequest.payload.extension:contentModifier</t>
+    <t>The CommunicationRequest payload element  "contentModifier" extension.</t>
+  </si>
+  <si>
+    <t>Bundle.entry.where(fullUrl = %context.entry[0].resource.communicationRequest.reference or (resource.resourceType = 'CommunicationRequest' and resource.id =%context.entry[0].resource.communicationRequest.reference.split('/').last())).resource.payload.extension.where(url='http://hl7.org/fhir/us/davinci-pas/StructureDefinition/extension-contentModifier').valueCodeableConcept</t>
+  </si>
+  <si>
+    <t>The ClaimResponse's communicationRequest element references the CommunicationRequest resource in the PAS response Bundle.  Will need to iterate through the payload items. FHIRPath for absolute and relative references. Using the FHIRPath function. "resolve()" which is not universally supported and untested: "Bundle.entry[0].resource.communicationRequest.resolve().resource.payload.extension.where(url='http://hl7.org/fhir/us/davinci-pas/StructureDefinition/extension-contentModifier').valueCodeableConcept"</t>
+  </si>
+  <si>
+    <t>“AttachmentsNeeded” Task.input  (Task.input.where('attachments-needed' in  type.coding.code.valueCodeableConcept)</t>
   </si>
   <si>
     <t>Due Date</t>
@@ -327,7 +393,13 @@
     <t>Date of service for claim/prior authorization</t>
   </si>
   <si>
-    <t>ClaimResponse.item.extension:requestedServiceDate</t>
+    <t>The ClaimResponse "preAuthPeriod" element's  start date.</t>
+  </si>
+  <si>
+    <t>Bundle.entry[0].resource.preAuthPeriod.start</t>
+  </si>
+  <si>
+    <t>Date of Service maps to the event level, not the service detail ( Item level) effective dates.</t>
   </si>
   <si>
     <t>Member ID</t>
@@ -348,10 +420,22 @@
     <t>Payer assigned patient identifier</t>
   </si>
   <si>
-    <t>ClaimResponse.patient: Patient.identifer</t>
-  </si>
-  <si>
-    <t>ClaimResponse = Bundle.entry[0].resource, Patient = Bundle.entry[n].resource referenced by ClaimResponse.patient</t>
+    <t>The member identifier element of the Patient referenced by the ClaimResponse's "patient" element.</t>
+  </si>
+  <si>
+    <t>Bundle.entry.where(fullUrl = %context.entry[0].resource.patient.reference or (resource.resourceType = 'Patient' and resource.id =%context.entry[0].resource.patient.reference.split('/').last())).resource.identifier.where('MB' in type.coding.code)</t>
+  </si>
+  <si>
+    <t>This identifier has a fixed type code of "MB". FHIRPath for absolute and relative references.  Using the FHIRPath function. "resolve()" which is not universally supported and untested: "Bundle.entry[0].resource.patient.resolve().resource.identifier.where('MB' in type.coding.code)"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Task.for (Task.for.resolves() to Patient resource) </t>
+  </si>
+  <si>
+    <t>Bundle.entry.where(fullUrl = %context.entry[0].resource.patient.reference or (resource.resourceType = 'Patient' and resource.id =%context.entry[0].resource.patient.reference.split('/').last())).resource</t>
+  </si>
+  <si>
+    <t>The element may contain a local reference to the Patient.</t>
   </si>
   <si>
     <t>Patient Name</t>
@@ -372,7 +456,13 @@
     <t>Patient demographic information for patient matching</t>
   </si>
   <si>
-    <t>ClaimResponse.patient: Patient.name</t>
+    <t>The name element of the Patient referenced by the ClaimResponse's "patient" element.</t>
+  </si>
+  <si>
+    <t>Bundle.entry.where(fullUrl = %context.entry[0].resource.patient.reference or (resource.resourceType = 'Patient' and resource.id =%context.entry[0].resource.patient.reference.split('/').last())).resource.name</t>
+  </si>
+  <si>
+    <t>FHIRPath for absolute and relative references.  Using the FHIRPath function. "resolve()" which is not universally supported and untested: "Bundle.entry[0].resource.patient.resolve().resource.name"</t>
   </si>
   <si>
     <t>Patient Account No.</t>
@@ -396,26 +486,59 @@
     <t>Patient.birthDate</t>
   </si>
   <si>
-    <t>ClaimResponse.patient: Patient.birthDate</t>
+    <t>The date of birth element of the Patient referenced by the ClaimResponse's "patient" element.</t>
+  </si>
+  <si>
+    <t>Bundle.entry.where(fullUrl = %context.entry[0].resource.patient.reference or (resource.resourceType = 'Patient' and resource.id =%context.entry[0].resource.patient.reference.split('/').last())).resource.birthDate</t>
+  </si>
+  <si>
+    <t>FHIRPath for absolute and relative references. Using the FHIRPath function. "resolve()" which is not universally supported and untested: "Bundle.entry[0].resource.patient.resolve().resource.birthDate"</t>
   </si>
   <si>
     <t>Questionnaire</t>
   </si>
   <si>
-    <t>“QuestionnairesNeeded” Task.input</t>
+    <t>“QuestionnairesContext” Task.input</t>
+  </si>
+  <si>
+    <t>“QuestionnaireContext” Task.input.value[x]  (Task.input.where('questiionnaire-context' in  type.coding.code).valueString)</t>
   </si>
   <si>
     <t>QuestionnaireResponse</t>
   </si>
   <si>
     <t>Attachment.Content</t>
+  </si>
+  <si>
+    <t>The attachment payload is created and returned by the Provider</t>
+  </si>
+  <si>
+    <t>Administrative Reference Number</t>
+  </si>
+  <si>
+    <t>AdminRefNumber</t>
+  </si>
+  <si>
+    <t>Payer-assigned administrative reference number</t>
+  </si>
+  <si>
+    <t>The ClaimResponse item element "AdministrationReferenceNumber" extension</t>
+  </si>
+  <si>
+    <t>TODO</t>
+  </si>
+  <si>
+    <t>Loop: 2000E - Patient Event Level or Loop: 2000F Service Level:REF02 where REF01 == "NT"</t>
+  </si>
+  <si>
+    <t>This payer assigned identifier is only for  prior authorization solicited attachments.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -549,6 +672,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -892,8 +1021,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1268,19 +1399,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67F1E6EC-B097-3D43-BD18-7F9C05C4BA68}">
-  <dimension ref="A1:K18"/>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC22C27-9062-5D42-B139-CE42F1F1FD99}">
+  <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="12" width="45.33203125" customWidth="1"/>
+    <col min="1" max="1" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="141.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="133.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="84.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="152.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="83.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="230" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="255.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="142.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="255.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1314,171 +1457,228 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="H2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="J2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="K2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" t="s">
         <v>20</v>
       </c>
+      <c r="N2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O2" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" t="s">
-        <v>22</v>
+        <v>162</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>163</v>
       </c>
       <c r="G3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H3" t="s">
-        <v>26</v>
+        <v>168</v>
       </c>
       <c r="I3" t="s">
-        <v>26</v>
+        <v>164</v>
       </c>
       <c r="J3" t="s">
-        <v>27</v>
+        <v>165</v>
       </c>
       <c r="K3" t="s">
-        <v>28</v>
+        <v>166</v>
+      </c>
+      <c r="M3" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" t="s">
+        <v>166</v>
+      </c>
+      <c r="O3" t="s">
+        <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s">
         <v>29</v>
       </c>
-      <c r="C4" t="s">
+      <c r="G4" t="s">
         <v>30</v>
       </c>
-      <c r="D4" t="s">
+      <c r="H4" t="s">
         <v>31</v>
       </c>
-      <c r="E4" t="s">
+      <c r="I4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" t="s">
         <v>32</v>
       </c>
-      <c r="F4" t="s">
+      <c r="K4" t="s">
+        <v>32</v>
+      </c>
+      <c r="L4" t="s">
+        <v>32</v>
+      </c>
+      <c r="M4" t="s">
         <v>33</v>
       </c>
-      <c r="G4" t="s">
+      <c r="N4" t="s">
         <v>34</v>
       </c>
-      <c r="H4" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4" t="s">
-        <v>29</v>
-      </c>
-      <c r="J4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K4" t="s">
-        <v>36</v>
+      <c r="O4" t="s">
+        <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" t="s">
         <v>37</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>38</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>39</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>40</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" t="s">
         <v>41</v>
       </c>
-      <c r="G5" t="s">
+      <c r="K5" t="s">
         <v>42</v>
       </c>
-      <c r="H5" t="s">
+      <c r="L5" t="s">
         <v>43</v>
       </c>
-      <c r="I5" t="s">
+      <c r="M5" t="s">
+        <v>40</v>
+      </c>
+      <c r="N5" t="s">
+        <v>42</v>
+      </c>
+      <c r="O5" t="s">
         <v>43</v>
       </c>
-      <c r="J5" t="s">
-        <v>44</v>
-      </c>
-      <c r="K5" t="s">
-        <v>44</v>
-      </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" t="s">
         <v>45</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>46</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>47</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>48</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>49</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>50</v>
-      </c>
-      <c r="H6" t="s">
-        <v>51</v>
       </c>
       <c r="I6" t="s">
         <v>51</v>
@@ -1487,10 +1687,22 @@
         <v>52</v>
       </c>
       <c r="K6" t="s">
+        <v>52</v>
+      </c>
+      <c r="L6" t="s">
+        <v>50</v>
+      </c>
+      <c r="M6" t="s">
         <v>53</v>
       </c>
+      <c r="N6" t="s">
+        <v>52</v>
+      </c>
+      <c r="O6" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1524,336 +1736,518 @@
       <c r="K7" t="s">
         <v>62</v>
       </c>
+      <c r="L7" t="s">
+        <v>63</v>
+      </c>
+      <c r="M7" t="s">
+        <v>64</v>
+      </c>
+      <c r="N7" t="s">
+        <v>62</v>
+      </c>
+      <c r="O7" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C8" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D8" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F8" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
       <c r="G8" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="H8" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="I8" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="J8" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="K8" t="s">
-        <v>70</v>
+        <v>73</v>
+      </c>
+      <c r="L8" t="s">
+        <v>74</v>
+      </c>
+      <c r="M8" t="s">
+        <v>75</v>
+      </c>
+      <c r="N8" t="s">
+        <v>73</v>
+      </c>
+      <c r="O8" t="s">
+        <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C9" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="D9" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="E9" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="F9" t="s">
-        <v>75</v>
+        <v>47</v>
       </c>
       <c r="G9" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="H9" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="I9" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="J9" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="K9" t="s">
-        <v>79</v>
+        <v>83</v>
+      </c>
+      <c r="L9" t="s">
+        <v>84</v>
+      </c>
+      <c r="M9" t="s">
+        <v>85</v>
+      </c>
+      <c r="N9" t="s">
+        <v>86</v>
+      </c>
+      <c r="O9" t="s">
+        <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="C10" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="D10" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="E10" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="F10" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="G10" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="H10" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="I10" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="J10" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="K10" t="s">
-        <v>79</v>
+        <v>96</v>
+      </c>
+      <c r="L10" t="s">
+        <v>97</v>
+      </c>
+      <c r="M10" t="s">
+        <v>98</v>
+      </c>
+      <c r="N10" t="s">
+        <v>96</v>
+      </c>
+      <c r="O10" t="s">
+        <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="C11" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>101</v>
       </c>
       <c r="E11" t="s">
-        <v>40</v>
+        <v>102</v>
       </c>
       <c r="F11" t="s">
-        <v>40</v>
+        <v>103</v>
       </c>
       <c r="G11" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="H11" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="I11" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="J11" t="s">
-        <v>92</v>
+        <v>106</v>
+      </c>
+      <c r="K11" t="s">
+        <v>107</v>
+      </c>
+      <c r="L11" t="s">
+        <v>108</v>
+      </c>
+      <c r="M11" t="s">
+        <v>109</v>
+      </c>
+      <c r="N11" t="s">
+        <v>107</v>
+      </c>
+      <c r="O11" t="s">
+        <v>108</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="C12" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="D12" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="E12" t="s">
-        <v>96</v>
+        <v>47</v>
       </c>
       <c r="F12" t="s">
-        <v>97</v>
+        <v>47</v>
       </c>
       <c r="G12" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="H12" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="I12" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="J12" t="s">
-        <v>100</v>
-      </c>
-      <c r="K12" t="s">
-        <v>79</v>
+        <v>114</v>
+      </c>
+      <c r="L12" t="s">
+        <v>114</v>
+      </c>
+      <c r="M12" t="s">
+        <v>112</v>
+      </c>
+      <c r="O12" t="s">
+        <v>114</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>116</v>
       </c>
       <c r="D13" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="E13" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="F13" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
       <c r="G13" t="s">
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="H13" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c r="I13" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c r="J13" t="s">
-        <v>107</v>
+        <v>122</v>
       </c>
       <c r="K13" t="s">
-        <v>108</v>
+        <v>123</v>
+      </c>
+      <c r="L13" t="s">
+        <v>124</v>
+      </c>
+      <c r="M13" t="s">
+        <v>52</v>
+      </c>
+      <c r="N13" t="s">
+        <v>123</v>
+      </c>
+      <c r="O13" t="s">
+        <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="C14" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
       <c r="D14" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
       <c r="E14" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="F14" t="s">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="G14" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
       <c r="H14" t="s">
-        <v>114</v>
+        <v>130</v>
       </c>
       <c r="I14" t="s">
-        <v>114</v>
+        <v>130</v>
       </c>
       <c r="J14" t="s">
-        <v>115</v>
+        <v>131</v>
       </c>
       <c r="K14" t="s">
-        <v>108</v>
+        <v>132</v>
+      </c>
+      <c r="L14" t="s">
+        <v>133</v>
+      </c>
+      <c r="M14" t="s">
+        <v>134</v>
+      </c>
+      <c r="N14" t="s">
+        <v>135</v>
+      </c>
+      <c r="O14" t="s">
+        <v>136</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>116</v>
+        <v>137</v>
       </c>
       <c r="C15" t="s">
-        <v>117</v>
+        <v>138</v>
       </c>
       <c r="D15" t="s">
-        <v>118</v>
+        <v>139</v>
       </c>
       <c r="E15" t="s">
-        <v>40</v>
-      </c>
-      <c r="F15" t="s">
-        <v>40</v>
+        <v>140</v>
+      </c>
+      <c r="F15" t="e">
+        <v>#VALUE!</v>
       </c>
       <c r="G15" t="s">
-        <v>105</v>
+        <v>141</v>
       </c>
       <c r="H15" t="s">
-        <v>119</v>
+        <v>142</v>
       </c>
       <c r="I15" t="s">
-        <v>119</v>
+        <v>142</v>
       </c>
       <c r="J15" t="s">
-        <v>92</v>
+        <v>143</v>
+      </c>
+      <c r="K15" t="s">
+        <v>144</v>
+      </c>
+      <c r="L15" t="s">
+        <v>145</v>
+      </c>
+      <c r="M15" t="s">
+        <v>134</v>
+      </c>
+      <c r="N15" t="s">
+        <v>135</v>
+      </c>
+      <c r="O15" t="s">
+        <v>136</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>120</v>
+        <v>146</v>
       </c>
       <c r="C16" t="s">
-        <v>40</v>
+        <v>147</v>
       </c>
       <c r="D16" t="s">
-        <v>121</v>
+        <v>148</v>
       </c>
       <c r="E16" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="F16" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="G16" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="H16" t="s">
+        <v>149</v>
+      </c>
+      <c r="I16" t="s">
+        <v>149</v>
+      </c>
+      <c r="J16" t="s">
         <v>114</v>
       </c>
-      <c r="I16" t="s">
+      <c r="L16" t="s">
         <v>114</v>
       </c>
-      <c r="J16" t="s">
-        <v>123</v>
-      </c>
-      <c r="K16" t="s">
-        <v>108</v>
+      <c r="M16" t="s">
+        <v>114</v>
+      </c>
+      <c r="O16" t="s">
+        <v>114</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>124</v>
+        <v>150</v>
+      </c>
+      <c r="C17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" t="s">
+        <v>151</v>
+      </c>
+      <c r="E17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" t="s">
+        <v>47</v>
       </c>
       <c r="G17" t="s">
-        <v>125</v>
+        <v>152</v>
+      </c>
+      <c r="H17" t="s">
+        <v>142</v>
+      </c>
+      <c r="I17" t="s">
+        <v>142</v>
+      </c>
+      <c r="J17" t="s">
+        <v>153</v>
+      </c>
+      <c r="K17" t="s">
+        <v>154</v>
+      </c>
+      <c r="L17" t="s">
+        <v>155</v>
+      </c>
+      <c r="M17" t="s">
+        <v>134</v>
+      </c>
+      <c r="N17" t="s">
+        <v>135</v>
+      </c>
+      <c r="O17" t="s">
+        <v>136</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>126</v>
-      </c>
-      <c r="F18" t="s">
-        <v>127</v>
+        <v>156</v>
+      </c>
+      <c r="G18" t="s">
+        <v>157</v>
+      </c>
+      <c r="J18" t="s">
+        <v>52</v>
+      </c>
+      <c r="M18" t="s">
+        <v>158</v>
+      </c>
+      <c r="N18" t="s">
+        <v>107</v>
+      </c>
+      <c r="O18" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>159</v>
+      </c>
+      <c r="F19" t="s">
+        <v>160</v>
+      </c>
+      <c r="J19" t="s">
+        <v>52</v>
+      </c>
+      <c r="L19" t="s">
+        <v>161</v>
+      </c>
+      <c r="O19" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FHIR-49828 Add a new $submit-attachment parameter for Administrative reference number
</commit_message>
<xml_diff>
--- a/input/images/data-element-mapping.xlsx
+++ b/input/images/data-element-mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/davinci-ecdx/input/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DCC26676-81D7-7949-A804-9C227FF72F58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{28FD3339-9328-A14D-8EE7-0110D85F240F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="102400" windowHeight="28800" xr2:uid="{8E0805B7-C227-7B40-8113-5FF95FC0AF88}"/>
   </bookViews>
@@ -1402,8 +1402,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC22C27-9062-5D42-B139-CE42F1F1FD99}">
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
qa FHIR-49828 and add change log for next version
</commit_message>
<xml_diff>
--- a/input/images/data-element-mapping.xlsx
+++ b/input/images/data-element-mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/davinci-ecdx/input/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{28FD3339-9328-A14D-8EE7-0110D85F240F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{076DDF84-5A4A-904E-98AC-B015FDDED62F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="102400" windowHeight="28800" xr2:uid="{8E0805B7-C227-7B40-8113-5FF95FC0AF88}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="102400" windowHeight="28800" xr2:uid="{5B896470-A209-0646-AF80-12B9912726E7}"/>
   </bookViews>
   <sheets>
     <sheet name="data-element-mapping" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="244" uniqueCount="169">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="245" uniqueCount="170">
   <si>
     <t>No</t>
   </si>
@@ -105,6 +105,33 @@
     <t>Maps to the "Patient Event Trace Number" in X12 278R</t>
   </si>
   <si>
+    <t>Administrative Reference Number</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Loop: 2000E - Patient Event Level or Loop: 2000F Service Level:REF02 where REF01 == "NT"</t>
+  </si>
+  <si>
+    <t>AdminRefNumber</t>
+  </si>
+  <si>
+    <t>This payer assigned identifier is only for  prior authorization solicited attachments.</t>
+  </si>
+  <si>
+    <t>Payer-assigned administrative reference number</t>
+  </si>
+  <si>
+    <t>The ClaimResponse item element "AdministrationReferenceNumber" extension</t>
+  </si>
+  <si>
+    <t>TODO</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
     <t>Use</t>
   </si>
   <si>
@@ -168,9 +195,6 @@
     <t>Loop: 2010A Segment: PER08 Notes: PER07 = "UR"</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>(operation endpoint)</t>
   </si>
   <si>
@@ -369,9 +393,6 @@
     <t>Deadline for submitting attachments to Payer</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Date of Service</t>
   </si>
   <si>
@@ -513,32 +534,14 @@
     <t>The attachment payload is created and returned by the Provider</t>
   </si>
   <si>
-    <t>Administrative Reference Number</t>
-  </si>
-  <si>
-    <t>AdminRefNumber</t>
-  </si>
-  <si>
-    <t>Payer-assigned administrative reference number</t>
-  </si>
-  <si>
-    <t>The ClaimResponse item element "AdministrationReferenceNumber" extension</t>
-  </si>
-  <si>
-    <t>TODO</t>
-  </si>
-  <si>
-    <t>Loop: 2000E - Patient Event Level or Loop: 2000F Service Level:REF02 where REF01 == "NT"</t>
-  </si>
-  <si>
-    <t>This payer assigned identifier is only for  prior authorization solicited attachments.</t>
+    <t>isNew</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -672,12 +675,6 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Menlo"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1021,10 +1018,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1399,11 +1394,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC22C27-9062-5D42-B139-CE42F1F1FD99}">
-  <dimension ref="A1:O19"/>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3175DFE1-6E88-A347-9F85-B7B1695D3A6D}">
+  <dimension ref="A1:P19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1420,10 +1415,11 @@
     <col min="10" max="10" width="230" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="255.83203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="142.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="255.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="255.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1469,8 +1465,11 @@
       <c r="O1" t="s">
         <v>14</v>
       </c>
+      <c r="P1" t="s">
+        <v>169</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1516,738 +1515,792 @@
       <c r="O2" t="s">
         <v>25</v>
       </c>
+      <c r="P2" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>162</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>47</v>
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>163</v>
+        <v>29</v>
       </c>
       <c r="G3" t="s">
         <v>20</v>
       </c>
       <c r="H3" t="s">
-        <v>168</v>
+        <v>30</v>
       </c>
       <c r="I3" t="s">
-        <v>164</v>
+        <v>31</v>
       </c>
       <c r="J3" t="s">
-        <v>165</v>
+        <v>32</v>
       </c>
       <c r="K3" t="s">
-        <v>166</v>
+        <v>33</v>
       </c>
       <c r="M3" t="s">
         <v>20</v>
       </c>
       <c r="N3" t="s">
-        <v>166</v>
+        <v>33</v>
       </c>
       <c r="O3" t="s">
-        <v>114</v>
+        <v>34</v>
+      </c>
+      <c r="P3" t="b">
+        <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="F4" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="G4" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="H4" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="I4" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J4" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="K4" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="L4" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="M4" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="N4" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="O4" t="s">
-        <v>34</v>
+        <v>43</v>
+      </c>
+      <c r="P4" t="b">
+        <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="E5" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="F5" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="G5" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="H5" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="I5" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="J5" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="K5" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="L5" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="M5" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="N5" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="O5" t="s">
-        <v>43</v>
+        <v>52</v>
+      </c>
+      <c r="P5" t="b">
+        <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="E6" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="F6" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="G6" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="H6" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="I6" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="J6" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="K6" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="L6" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="M6" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="N6" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="O6" t="s">
-        <v>50</v>
+        <v>58</v>
+      </c>
+      <c r="P6" t="b">
+        <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="C7" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="D7" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="E7" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="F7" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="G7" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="H7" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="I7" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="J7" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="K7" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="L7" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="M7" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="N7" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="O7" t="s">
-        <v>63</v>
+        <v>71</v>
+      </c>
+      <c r="P7" t="b">
+        <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D8" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="E8" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="F8" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="G8" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="H8" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="I8" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="J8" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="K8" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="L8" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="M8" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="N8" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="O8" t="s">
-        <v>74</v>
+        <v>82</v>
+      </c>
+      <c r="P8" t="b">
+        <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="C9" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D9" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="E9" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="F9" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="G9" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="H9" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="I9" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="J9" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="K9" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="L9" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="M9" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="N9" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="O9" t="s">
-        <v>87</v>
+        <v>95</v>
+      </c>
+      <c r="P9" t="b">
+        <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="C10" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="D10" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="E10" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="F10" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="G10" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="H10" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="I10" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="J10" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="K10" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="L10" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="M10" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="N10" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="O10" t="s">
-        <v>97</v>
+        <v>105</v>
+      </c>
+      <c r="P10" t="b">
+        <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="C11" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="D11" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="E11" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="F11" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="G11" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="H11" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="I11" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="J11" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="K11" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="L11" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="M11" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="N11" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="O11" t="s">
-        <v>108</v>
+        <v>116</v>
+      </c>
+      <c r="P11" t="b">
+        <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="C12" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="D12" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="E12" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="F12" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="G12" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="H12" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="I12" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="J12" t="s">
-        <v>114</v>
+        <v>34</v>
       </c>
       <c r="L12" t="s">
-        <v>114</v>
+        <v>34</v>
       </c>
       <c r="M12" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="O12" t="s">
-        <v>114</v>
+        <v>34</v>
+      </c>
+      <c r="P12" t="b">
+        <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="C13" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="D13" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="E13" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="F13" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="G13" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="H13" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="I13" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="J13" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="K13" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="L13" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="M13" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="N13" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="O13" t="s">
-        <v>124</v>
+        <v>131</v>
+      </c>
+      <c r="P13" t="b">
+        <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="C14" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D14" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="E14" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="F14" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="G14" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="H14" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="I14" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="J14" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="K14" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="L14" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="M14" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="N14" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="O14" t="s">
-        <v>136</v>
+        <v>143</v>
+      </c>
+      <c r="P14" t="b">
+        <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="C15" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="D15" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="E15" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="F15" t="e">
         <v>#VALUE!</v>
       </c>
       <c r="G15" t="s">
+        <v>148</v>
+      </c>
+      <c r="H15" t="s">
+        <v>149</v>
+      </c>
+      <c r="I15" t="s">
+        <v>149</v>
+      </c>
+      <c r="J15" t="s">
+        <v>150</v>
+      </c>
+      <c r="K15" t="s">
+        <v>151</v>
+      </c>
+      <c r="L15" t="s">
+        <v>152</v>
+      </c>
+      <c r="M15" t="s">
         <v>141</v>
       </c>
-      <c r="H15" t="s">
+      <c r="N15" t="s">
         <v>142</v>
       </c>
-      <c r="I15" t="s">
-        <v>142</v>
-      </c>
-      <c r="J15" t="s">
+      <c r="O15" t="s">
         <v>143</v>
       </c>
-      <c r="K15" t="s">
-        <v>144</v>
-      </c>
-      <c r="L15" t="s">
-        <v>145</v>
-      </c>
-      <c r="M15" t="s">
-        <v>134</v>
-      </c>
-      <c r="N15" t="s">
-        <v>135</v>
-      </c>
-      <c r="O15" t="s">
-        <v>136</v>
+      <c r="P15" t="b">
+        <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="C16" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="D16" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="E16" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="F16" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="G16" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="H16" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="I16" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="J16" t="s">
-        <v>114</v>
+        <v>34</v>
       </c>
       <c r="L16" t="s">
-        <v>114</v>
+        <v>34</v>
       </c>
       <c r="M16" t="s">
-        <v>114</v>
+        <v>34</v>
       </c>
       <c r="O16" t="s">
-        <v>114</v>
+        <v>34</v>
+      </c>
+      <c r="P16" t="b">
+        <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="C17" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="D17" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="E17" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="F17" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="G17" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="H17" t="s">
+        <v>149</v>
+      </c>
+      <c r="I17" t="s">
+        <v>149</v>
+      </c>
+      <c r="J17" t="s">
+        <v>160</v>
+      </c>
+      <c r="K17" t="s">
+        <v>161</v>
+      </c>
+      <c r="L17" t="s">
+        <v>162</v>
+      </c>
+      <c r="M17" t="s">
+        <v>141</v>
+      </c>
+      <c r="N17" t="s">
         <v>142</v>
       </c>
-      <c r="I17" t="s">
-        <v>142</v>
-      </c>
-      <c r="J17" t="s">
-        <v>153</v>
-      </c>
-      <c r="K17" t="s">
-        <v>154</v>
-      </c>
-      <c r="L17" t="s">
-        <v>155</v>
-      </c>
-      <c r="M17" t="s">
-        <v>134</v>
-      </c>
-      <c r="N17" t="s">
-        <v>135</v>
-      </c>
       <c r="O17" t="s">
-        <v>136</v>
+        <v>143</v>
+      </c>
+      <c r="P17" t="b">
+        <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="G18" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="J18" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="M18" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="N18" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="O18" t="s">
-        <v>108</v>
+        <v>116</v>
+      </c>
+      <c r="P18" t="b">
+        <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="F19" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="J19" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="L19" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="O19" t="s">
-        <v>161</v>
+        <v>168</v>
+      </c>
+      <c r="P19" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>